<commit_message>
updated documentation RD files and added stratcorr
</commit_message>
<xml_diff>
--- a/inst/extdata/cometsInputAge.xlsx
+++ b/inst/extdata/cometsInputAge.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1320" yWindow="645" windowWidth="20730" windowHeight="11760" activeTab="3"/>
+    <workbookView xWindow="1320" yWindow="645" windowWidth="20730" windowHeight="11760" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Metabolites" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="86">
   <si>
     <t>METABOLITE_NAME</t>
   </si>
@@ -275,6 +275,12 @@
   </si>
   <si>
     <t>metabid</t>
+  </si>
+  <si>
+    <t>STRATIFICATION</t>
+  </si>
+  <si>
+    <t>SITE</t>
   </si>
 </sst>
 </file>
@@ -1149,7 +1155,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -3129,7 +3135,7 @@
   <dimension ref="A1:S20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -4347,236 +4353,297 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C20"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="8.85546875" style="1"/>
+    <col min="2" max="2" width="14.28515625" style="1" customWidth="1"/>
+    <col min="3" max="4" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="14.1" customHeight="1">
+    <row r="1" spans="1:4" ht="14.1" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="D1" s="5" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15.95" customHeight="1">
+    <row r="2" spans="1:4" ht="15.95" customHeight="1">
       <c r="A2" s="2">
         <v>1000121</v>
       </c>
-      <c r="B2" s="6">
+      <c r="B2" s="2">
+        <v>1</v>
+      </c>
+      <c r="C2" s="6">
         <v>48</v>
       </c>
-      <c r="C2" s="6">
+      <c r="D2" s="6">
         <v>26.8</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15.95" customHeight="1">
+    <row r="3" spans="1:4" ht="15.95" customHeight="1">
       <c r="A3" s="2">
         <v>1000122</v>
       </c>
-      <c r="B3" s="6">
+      <c r="B3" s="2">
+        <v>1</v>
+      </c>
+      <c r="C3" s="6">
         <v>65</v>
       </c>
-      <c r="C3" s="6">
+      <c r="D3" s="6">
         <v>32.4</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15.95" customHeight="1">
+    <row r="4" spans="1:4" ht="15.95" customHeight="1">
       <c r="A4" s="2">
         <v>1000123</v>
       </c>
-      <c r="B4" s="6">
+      <c r="B4" s="2">
+        <v>1</v>
+      </c>
+      <c r="C4" s="6">
         <v>49</v>
       </c>
-      <c r="C4" s="6">
+      <c r="D4" s="6">
         <v>33.4</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="15.95" customHeight="1">
+    <row r="5" spans="1:4" ht="15.95" customHeight="1">
       <c r="A5" s="2">
         <v>1000124</v>
       </c>
-      <c r="B5" s="6">
+      <c r="B5" s="2">
+        <v>2</v>
+      </c>
+      <c r="C5" s="6">
         <v>57</v>
       </c>
-      <c r="C5" s="6">
+      <c r="D5" s="6">
         <v>29.7</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="15.95" customHeight="1">
+    <row r="6" spans="1:4" ht="15.95" customHeight="1">
       <c r="A6" s="2">
         <v>1000125</v>
       </c>
-      <c r="B6" s="6">
+      <c r="B6" s="2">
+        <v>3</v>
+      </c>
+      <c r="C6" s="6">
         <v>63</v>
       </c>
-      <c r="C6" s="6">
+      <c r="D6" s="6">
         <v>22.7</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="15.95" customHeight="1">
+    <row r="7" spans="1:4" ht="15.95" customHeight="1">
       <c r="A7" s="2">
         <v>1000126</v>
       </c>
-      <c r="B7" s="6">
+      <c r="B7" s="2">
+        <v>1</v>
+      </c>
+      <c r="C7" s="6">
         <v>59</v>
       </c>
-      <c r="C7" s="6">
+      <c r="D7" s="6">
         <v>26.4</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="15.95" customHeight="1">
+    <row r="8" spans="1:4" ht="15.95" customHeight="1">
       <c r="A8" s="2">
         <v>1000127</v>
       </c>
-      <c r="B8" s="6">
+      <c r="B8" s="2">
+        <v>1</v>
+      </c>
+      <c r="C8" s="6">
         <v>50</v>
       </c>
-      <c r="C8" s="6">
+      <c r="D8" s="6">
         <v>24.9</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="15.95" customHeight="1">
+    <row r="9" spans="1:4" ht="15.95" customHeight="1">
       <c r="A9" s="2">
         <v>1000128</v>
       </c>
-      <c r="B9" s="6">
+      <c r="B9" s="2">
+        <v>2</v>
+      </c>
+      <c r="C9" s="6">
         <v>74</v>
       </c>
-      <c r="C9" s="6">
+      <c r="D9" s="6">
         <v>22.4</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="15.95" customHeight="1">
+    <row r="10" spans="1:4" ht="15.95" customHeight="1">
       <c r="A10" s="2">
         <v>1000129</v>
       </c>
-      <c r="B10" s="6">
+      <c r="B10" s="2">
+        <v>2</v>
+      </c>
+      <c r="C10" s="6">
         <v>36</v>
       </c>
-      <c r="C10" s="6">
+      <c r="D10" s="6">
         <v>28.6</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="15.95" customHeight="1">
+    <row r="11" spans="1:4" ht="15.95" customHeight="1">
       <c r="A11" s="2">
         <v>1000130</v>
       </c>
-      <c r="B11" s="6">
+      <c r="B11" s="2">
+        <v>2</v>
+      </c>
+      <c r="C11" s="6">
         <v>44</v>
       </c>
-      <c r="C11" s="6">
+      <c r="D11" s="6">
         <v>21.4</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="15.95" customHeight="1">
+    <row r="12" spans="1:4" ht="15.95" customHeight="1">
       <c r="A12" s="2">
         <v>1000131</v>
       </c>
-      <c r="B12" s="6">
+      <c r="B12" s="2">
+        <v>3</v>
+      </c>
+      <c r="C12" s="6">
         <v>49</v>
       </c>
-      <c r="C12" s="6">
+      <c r="D12" s="6">
         <v>20.7</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="15.95" customHeight="1">
+    <row r="13" spans="1:4" ht="15.95" customHeight="1">
       <c r="A13" s="2">
         <v>1000132</v>
       </c>
-      <c r="B13" s="6">
+      <c r="B13" s="2">
+        <v>3</v>
+      </c>
+      <c r="C13" s="6">
         <v>61</v>
       </c>
-      <c r="C13" s="6">
+      <c r="D13" s="6">
         <v>29.4</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="15.95" customHeight="1">
+    <row r="14" spans="1:4" ht="15.95" customHeight="1">
       <c r="A14" s="2">
         <v>1000133</v>
       </c>
-      <c r="B14" s="6">
+      <c r="B14" s="2">
+        <v>3</v>
+      </c>
+      <c r="C14" s="6">
         <v>57</v>
       </c>
-      <c r="C14" s="6">
+      <c r="D14" s="6">
         <v>28.7</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="15.95" customHeight="1">
+    <row r="15" spans="1:4" ht="15.95" customHeight="1">
       <c r="A15" s="2">
         <v>1000134</v>
       </c>
-      <c r="B15" s="6">
+      <c r="B15" s="2">
+        <v>3</v>
+      </c>
+      <c r="C15" s="6">
         <v>48</v>
       </c>
-      <c r="C15" s="6">
+      <c r="D15" s="6">
         <v>26.8</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="15.95" customHeight="1">
+    <row r="16" spans="1:4" ht="15.95" customHeight="1">
       <c r="A16" s="2">
         <v>1000135</v>
       </c>
-      <c r="B16" s="6">
+      <c r="B16" s="2">
+        <v>2</v>
+      </c>
+      <c r="C16" s="6">
         <v>47</v>
       </c>
-      <c r="C16" s="6">
+      <c r="D16" s="6">
         <v>27.3</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="15.95" customHeight="1">
+    <row r="17" spans="1:4" ht="15.95" customHeight="1">
       <c r="A17" s="2">
         <v>1000136</v>
       </c>
-      <c r="B17" s="6">
+      <c r="B17" s="2">
+        <v>2</v>
+      </c>
+      <c r="C17" s="6">
         <v>56</v>
       </c>
-      <c r="C17" s="6">
+      <c r="D17" s="6">
         <v>22.4</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="15.95" customHeight="1">
+    <row r="18" spans="1:4" ht="15.95" customHeight="1">
       <c r="A18" s="2">
         <v>1000137</v>
       </c>
-      <c r="B18" s="6">
+      <c r="B18" s="2">
+        <v>3</v>
+      </c>
+      <c r="C18" s="6">
         <v>50</v>
       </c>
-      <c r="C18" s="6">
+      <c r="D18" s="6">
         <v>21.6</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="15.95" customHeight="1">
+    <row r="19" spans="1:4" ht="15.95" customHeight="1">
       <c r="A19" s="2">
         <v>1000138</v>
       </c>
-      <c r="B19" s="6">
+      <c r="B19" s="2">
+        <v>2</v>
+      </c>
+      <c r="C19" s="6">
         <v>49</v>
       </c>
-      <c r="C19" s="6">
+      <c r="D19" s="6">
         <v>23.4</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="15.95" customHeight="1">
+    <row r="20" spans="1:4" ht="15.95" customHeight="1">
       <c r="A20" s="2">
         <v>1000139</v>
       </c>
-      <c r="B20" s="6">
+      <c r="B20" s="2">
+        <v>1</v>
+      </c>
+      <c r="C20" s="6">
         <v>46</v>
       </c>
-      <c r="C20" s="6">
+      <c r="D20" s="6">
         <v>22.7</v>
       </c>
     </row>
@@ -4596,7 +4663,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
@@ -4693,17 +4760,20 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="4" width="42.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.85546875" style="1"/>
+    <col min="5" max="5" width="36.28515625" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="14.1" customHeight="1">
+    <row r="1" spans="1:5" ht="14.1" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>72</v>
       </c>
@@ -4716,8 +4786,11 @@
       <c r="D1" s="2" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="15.95" customHeight="1">
+      <c r="E1" s="8" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="15.95" customHeight="1">
       <c r="A2" s="2" t="s">
         <v>76</v>
       </c>
@@ -4731,7 +4804,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15.95" customHeight="1">
+    <row r="3" spans="1:5" ht="15.95" customHeight="1">
       <c r="A3" s="2" t="s">
         <v>78</v>
       </c>
@@ -4745,7 +4818,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="14.1" customHeight="1">
+    <row r="4" spans="1:5" ht="14.1" customHeight="1">
       <c r="A4" s="4"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added integrity check to error when stratification and adjustment/exposure are the same.
</commit_message>
<xml_diff>
--- a/inst/extdata/cometsInputAge.xlsx
+++ b/inst/extdata/cometsInputAge.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="27729"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1320" yWindow="645" windowWidth="20730" windowHeight="11760" activeTab="2"/>
+    <workbookView xWindow="1320" yWindow="640" windowWidth="25200" windowHeight="14760" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Metabolites" sheetId="1" r:id="rId1"/>
     <sheet name="SubjectMetabolites" sheetId="2" r:id="rId2"/>
     <sheet name="SubjectData" sheetId="3" r:id="rId3"/>
-    <sheet name="VarMap" sheetId="4" r:id="rId4"/>
+    <sheet name="VarMap" sheetId="6" r:id="rId4"/>
     <sheet name="Models" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="125725" concurrentCalc="0"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="86">
   <si>
     <t>METABOLITE_NAME</t>
   </si>
@@ -238,9 +238,6 @@
     <t>metabolite_id</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
     <t>MODEL</t>
   </si>
   <si>
@@ -281,13 +278,16 @@
   </si>
   <si>
     <t>SITE</t>
+  </si>
+  <si>
+    <t>site</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="22">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -648,7 +648,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -774,6 +774,15 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FFC1C1C1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -819,7 +828,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="19" fillId="34" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -842,6 +851,13 @@
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="34" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="35" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1162,24 +1178,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E352"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="36.42578125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="38.5703125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="8.85546875" style="1"/>
+    <col min="1" max="1" width="36.5" style="1" customWidth="1"/>
+    <col min="2" max="2" width="38.5" style="1" customWidth="1"/>
+    <col min="3" max="3" width="12.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="14.1" customHeight="1">
+    <row r="1" spans="1:5" ht="14" customHeight="1">
       <c r="A1" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -1188,13 +1204,13 @@
         <v>1</v>
       </c>
       <c r="D1" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="E1" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="E1" s="8" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="15.95" customHeight="1">
+    </row>
+    <row r="2" spans="1:5" ht="16" customHeight="1">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -1211,7 +1227,7 @@
         <v>146.11689999999999</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="15.95" customHeight="1">
+    <row r="3" spans="1:5" ht="16" customHeight="1">
       <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
@@ -1225,7 +1241,7 @@
         <v>117.04259999999999</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15.95" customHeight="1">
+    <row r="4" spans="1:5" ht="16" customHeight="1">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
@@ -1239,7 +1255,7 @@
         <v>188.03210000000001</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="15.95" customHeight="1">
+    <row r="5" spans="1:5" ht="16" customHeight="1">
       <c r="A5" s="2" t="s">
         <v>11</v>
       </c>
@@ -1253,7 +1269,7 @@
         <v>135.05449999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="15.95" customHeight="1">
+    <row r="6" spans="1:5" ht="16" customHeight="1">
       <c r="A6" s="2" t="s">
         <v>14</v>
       </c>
@@ -1267,7 +1283,7 @@
         <v>267.09675499999997</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="15.95" customHeight="1">
+    <row r="7" spans="1:5" ht="16" customHeight="1">
       <c r="A7" s="2" t="s">
         <v>17</v>
       </c>
@@ -1281,7 +1297,7 @@
         <v>145.1</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="15.95" customHeight="1">
+    <row r="8" spans="1:5" ht="16" customHeight="1">
       <c r="A8" s="2" t="s">
         <v>20</v>
       </c>
@@ -1298,7 +1314,7 @@
         <v>203.15</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="15.95" customHeight="1">
+    <row r="9" spans="1:5" ht="16" customHeight="1">
       <c r="A9" s="2" t="s">
         <v>22</v>
       </c>
@@ -1312,7 +1328,7 @@
         <v>462.2</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="15.95" customHeight="1">
+    <row r="10" spans="1:5" ht="16" customHeight="1">
       <c r="A10" s="2" t="s">
         <v>24</v>
       </c>
@@ -1329,7 +1345,7 @@
         <v>90.06</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="15.95" customHeight="1">
+    <row r="11" spans="1:5" ht="16" customHeight="1">
       <c r="A11" s="2" t="s">
         <v>27</v>
       </c>
@@ -1343,7 +1359,7 @@
         <v>157.1</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="15.95" customHeight="1">
+    <row r="12" spans="1:5" ht="16" customHeight="1">
       <c r="A12" s="2" t="s">
         <v>30</v>
       </c>
@@ -1354,7 +1370,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="15.95" customHeight="1">
+    <row r="13" spans="1:5" ht="16" customHeight="1">
       <c r="A13" s="2" t="s">
         <v>33</v>
       </c>
@@ -1371,7 +1387,7 @@
         <v>258.1105</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="15.95" customHeight="1">
+    <row r="14" spans="1:5" ht="16" customHeight="1">
       <c r="A14" s="2" t="s">
         <v>36</v>
       </c>
@@ -1382,7 +1398,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="15.95" customHeight="1">
+    <row r="15" spans="1:5" ht="16" customHeight="1">
       <c r="A15" s="2" t="s">
         <v>39</v>
       </c>
@@ -1393,7 +1409,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="15.95" customHeight="1">
+    <row r="16" spans="1:5" ht="16" customHeight="1">
       <c r="A16" s="2" t="s">
         <v>42</v>
       </c>
@@ -1410,7 +1426,7 @@
         <v>104.07</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="15.95" customHeight="1">
+    <row r="17" spans="1:5" ht="16" customHeight="1">
       <c r="A17" s="2" t="s">
         <v>45</v>
       </c>
@@ -1424,7 +1440,7 @@
         <v>346.2</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="15.95" customHeight="1">
+    <row r="18" spans="1:5" ht="16" customHeight="1">
       <c r="A18" s="2" t="s">
         <v>47</v>
       </c>
@@ -1441,7 +1457,7 @@
         <v>241.13</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="15.95" customHeight="1">
+    <row r="19" spans="1:5" ht="16" customHeight="1">
       <c r="A19" s="2" t="s">
         <v>50</v>
       </c>
@@ -1455,1673 +1471,1673 @@
         <v>136.1</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="15.95" customHeight="1">
+    <row r="20" spans="1:5" ht="16" customHeight="1">
       <c r="A20" s="2"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
     </row>
-    <row r="21" spans="1:5" ht="15.95" customHeight="1">
+    <row r="21" spans="1:5" ht="16" customHeight="1">
       <c r="A21" s="2"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
     </row>
-    <row r="22" spans="1:5" ht="15.95" customHeight="1">
+    <row r="22" spans="1:5" ht="16" customHeight="1">
       <c r="A22" s="2"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
     </row>
-    <row r="23" spans="1:5" ht="15.95" customHeight="1">
+    <row r="23" spans="1:5" ht="16" customHeight="1">
       <c r="A23" s="2"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
     </row>
-    <row r="24" spans="1:5" ht="15.95" customHeight="1">
+    <row r="24" spans="1:5" ht="16" customHeight="1">
       <c r="A24" s="2"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
     </row>
-    <row r="25" spans="1:5" ht="15.95" customHeight="1">
+    <row r="25" spans="1:5" ht="16" customHeight="1">
       <c r="A25" s="2"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
     </row>
-    <row r="26" spans="1:5" ht="15.95" customHeight="1">
+    <row r="26" spans="1:5" ht="16" customHeight="1">
       <c r="A26" s="2"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
     </row>
-    <row r="27" spans="1:5" ht="15.95" customHeight="1">
+    <row r="27" spans="1:5" ht="16" customHeight="1">
       <c r="A27" s="2"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
     </row>
-    <row r="28" spans="1:5" ht="15.95" customHeight="1">
+    <row r="28" spans="1:5" ht="16" customHeight="1">
       <c r="A28" s="2"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
     </row>
-    <row r="29" spans="1:5" ht="15.95" customHeight="1">
+    <row r="29" spans="1:5" ht="16" customHeight="1">
       <c r="A29" s="2"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
     </row>
-    <row r="30" spans="1:5" ht="15.95" customHeight="1">
+    <row r="30" spans="1:5" ht="16" customHeight="1">
       <c r="A30" s="2"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
     </row>
-    <row r="31" spans="1:5" ht="15.95" customHeight="1">
+    <row r="31" spans="1:5" ht="16" customHeight="1">
       <c r="A31" s="2"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
     </row>
-    <row r="32" spans="1:5" ht="15.95" customHeight="1">
+    <row r="32" spans="1:5" ht="16" customHeight="1">
       <c r="A32" s="2"/>
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
     </row>
-    <row r="33" spans="1:3" ht="15.95" customHeight="1">
+    <row r="33" spans="1:3" ht="16" customHeight="1">
       <c r="A33" s="2"/>
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
     </row>
-    <row r="34" spans="1:3" ht="15.95" customHeight="1">
+    <row r="34" spans="1:3" ht="16" customHeight="1">
       <c r="A34" s="2"/>
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
     </row>
-    <row r="35" spans="1:3" ht="15.95" customHeight="1">
+    <row r="35" spans="1:3" ht="16" customHeight="1">
       <c r="A35" s="2"/>
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
     </row>
-    <row r="36" spans="1:3" ht="15.95" customHeight="1">
+    <row r="36" spans="1:3" ht="16" customHeight="1">
       <c r="A36" s="2"/>
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
     </row>
-    <row r="37" spans="1:3" ht="15.95" customHeight="1">
+    <row r="37" spans="1:3" ht="16" customHeight="1">
       <c r="A37" s="2"/>
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
     </row>
-    <row r="38" spans="1:3" ht="15.95" customHeight="1">
+    <row r="38" spans="1:3" ht="16" customHeight="1">
       <c r="A38" s="2"/>
       <c r="B38" s="3"/>
       <c r="C38" s="3"/>
     </row>
-    <row r="39" spans="1:3" ht="15.95" customHeight="1">
+    <row r="39" spans="1:3" ht="16" customHeight="1">
       <c r="A39" s="2"/>
       <c r="B39" s="3"/>
       <c r="C39" s="3"/>
     </row>
-    <row r="40" spans="1:3" ht="15.95" customHeight="1">
+    <row r="40" spans="1:3" ht="16" customHeight="1">
       <c r="A40" s="2"/>
       <c r="B40" s="3"/>
       <c r="C40" s="3"/>
     </row>
-    <row r="41" spans="1:3" ht="15.95" customHeight="1">
+    <row r="41" spans="1:3" ht="16" customHeight="1">
       <c r="A41" s="2"/>
       <c r="B41" s="3"/>
       <c r="C41" s="3"/>
     </row>
-    <row r="42" spans="1:3" ht="15.95" customHeight="1">
+    <row r="42" spans="1:3" ht="16" customHeight="1">
       <c r="A42" s="2"/>
       <c r="B42" s="3"/>
       <c r="C42" s="3"/>
     </row>
-    <row r="43" spans="1:3" ht="15.95" customHeight="1">
+    <row r="43" spans="1:3" ht="16" customHeight="1">
       <c r="A43" s="2"/>
       <c r="B43" s="3"/>
       <c r="C43" s="3"/>
     </row>
-    <row r="44" spans="1:3" ht="15.95" customHeight="1">
+    <row r="44" spans="1:3" ht="16" customHeight="1">
       <c r="A44" s="2"/>
       <c r="B44" s="3"/>
       <c r="C44" s="3"/>
     </row>
-    <row r="45" spans="1:3" ht="15.95" customHeight="1">
+    <row r="45" spans="1:3" ht="16" customHeight="1">
       <c r="A45" s="2"/>
       <c r="B45" s="3"/>
       <c r="C45" s="3"/>
     </row>
-    <row r="46" spans="1:3" ht="15.95" customHeight="1">
+    <row r="46" spans="1:3" ht="16" customHeight="1">
       <c r="A46" s="2"/>
       <c r="B46" s="3"/>
       <c r="C46" s="3"/>
     </row>
-    <row r="47" spans="1:3" ht="15.95" customHeight="1">
+    <row r="47" spans="1:3" ht="16" customHeight="1">
       <c r="A47" s="2"/>
       <c r="B47" s="3"/>
       <c r="C47" s="3"/>
     </row>
-    <row r="48" spans="1:3" ht="15.95" customHeight="1">
+    <row r="48" spans="1:3" ht="16" customHeight="1">
       <c r="A48" s="2"/>
       <c r="B48" s="3"/>
       <c r="C48" s="3"/>
     </row>
-    <row r="49" spans="1:3" ht="15.95" customHeight="1">
+    <row r="49" spans="1:3" ht="16" customHeight="1">
       <c r="A49" s="2"/>
       <c r="B49" s="3"/>
       <c r="C49" s="3"/>
     </row>
-    <row r="50" spans="1:3" ht="15.95" customHeight="1">
+    <row r="50" spans="1:3" ht="16" customHeight="1">
       <c r="A50" s="2"/>
       <c r="B50" s="3"/>
       <c r="C50" s="3"/>
     </row>
-    <row r="51" spans="1:3" ht="15.95" customHeight="1">
+    <row r="51" spans="1:3" ht="16" customHeight="1">
       <c r="A51" s="2"/>
       <c r="B51" s="3"/>
       <c r="C51" s="3"/>
     </row>
-    <row r="52" spans="1:3" ht="15.95" customHeight="1">
+    <row r="52" spans="1:3" ht="16" customHeight="1">
       <c r="A52" s="2"/>
       <c r="B52" s="3"/>
       <c r="C52" s="3"/>
     </row>
-    <row r="53" spans="1:3" ht="15.95" customHeight="1">
+    <row r="53" spans="1:3" ht="16" customHeight="1">
       <c r="A53" s="2"/>
       <c r="B53" s="3"/>
       <c r="C53" s="3"/>
     </row>
-    <row r="54" spans="1:3" ht="15.95" customHeight="1">
+    <row r="54" spans="1:3" ht="16" customHeight="1">
       <c r="A54" s="2"/>
       <c r="B54" s="3"/>
       <c r="C54" s="3"/>
     </row>
-    <row r="55" spans="1:3" ht="15.95" customHeight="1">
+    <row r="55" spans="1:3" ht="16" customHeight="1">
       <c r="A55" s="2"/>
       <c r="B55" s="3"/>
       <c r="C55" s="3"/>
     </row>
-    <row r="56" spans="1:3" ht="15.95" customHeight="1">
+    <row r="56" spans="1:3" ht="16" customHeight="1">
       <c r="A56" s="2"/>
       <c r="B56" s="3"/>
       <c r="C56" s="3"/>
     </row>
-    <row r="57" spans="1:3" ht="15.95" customHeight="1">
+    <row r="57" spans="1:3" ht="16" customHeight="1">
       <c r="A57" s="2"/>
       <c r="B57" s="3"/>
       <c r="C57" s="3"/>
     </row>
-    <row r="58" spans="1:3" ht="15.95" customHeight="1">
+    <row r="58" spans="1:3" ht="16" customHeight="1">
       <c r="A58" s="2"/>
       <c r="B58" s="3"/>
       <c r="C58" s="3"/>
     </row>
-    <row r="59" spans="1:3" ht="15.95" customHeight="1">
+    <row r="59" spans="1:3" ht="16" customHeight="1">
       <c r="A59" s="2"/>
       <c r="B59" s="3"/>
       <c r="C59" s="3"/>
     </row>
-    <row r="60" spans="1:3" ht="15.95" customHeight="1">
+    <row r="60" spans="1:3" ht="16" customHeight="1">
       <c r="A60" s="2"/>
       <c r="B60" s="3"/>
       <c r="C60" s="3"/>
     </row>
-    <row r="61" spans="1:3" ht="15.95" customHeight="1">
+    <row r="61" spans="1:3" ht="16" customHeight="1">
       <c r="A61" s="2"/>
       <c r="B61" s="3"/>
       <c r="C61" s="3"/>
     </row>
-    <row r="62" spans="1:3" ht="15.95" customHeight="1">
+    <row r="62" spans="1:3" ht="16" customHeight="1">
       <c r="A62" s="2"/>
       <c r="B62" s="3"/>
       <c r="C62" s="3"/>
     </row>
-    <row r="63" spans="1:3" ht="15.95" customHeight="1">
+    <row r="63" spans="1:3" ht="16" customHeight="1">
       <c r="A63" s="2"/>
       <c r="B63" s="3"/>
       <c r="C63" s="3"/>
     </row>
-    <row r="64" spans="1:3" ht="15.95" customHeight="1">
+    <row r="64" spans="1:3" ht="16" customHeight="1">
       <c r="A64" s="2"/>
       <c r="B64" s="3"/>
       <c r="C64" s="3"/>
     </row>
-    <row r="65" spans="1:3" ht="15.95" customHeight="1">
+    <row r="65" spans="1:3" ht="16" customHeight="1">
       <c r="A65" s="2"/>
       <c r="B65" s="3"/>
       <c r="C65" s="3"/>
     </row>
-    <row r="66" spans="1:3" ht="15.95" customHeight="1">
+    <row r="66" spans="1:3" ht="16" customHeight="1">
       <c r="A66" s="2"/>
       <c r="B66" s="3"/>
       <c r="C66" s="3"/>
     </row>
-    <row r="67" spans="1:3" ht="15.95" customHeight="1">
+    <row r="67" spans="1:3" ht="16" customHeight="1">
       <c r="A67" s="2"/>
       <c r="B67" s="3"/>
       <c r="C67" s="3"/>
     </row>
-    <row r="68" spans="1:3" ht="15.95" customHeight="1">
+    <row r="68" spans="1:3" ht="16" customHeight="1">
       <c r="A68" s="2"/>
       <c r="B68" s="3"/>
       <c r="C68" s="3"/>
     </row>
-    <row r="69" spans="1:3" ht="15.95" customHeight="1">
+    <row r="69" spans="1:3" ht="16" customHeight="1">
       <c r="A69" s="2"/>
       <c r="B69" s="3"/>
       <c r="C69" s="3"/>
     </row>
-    <row r="70" spans="1:3" ht="15.95" customHeight="1">
+    <row r="70" spans="1:3" ht="16" customHeight="1">
       <c r="A70" s="2"/>
       <c r="B70" s="3"/>
       <c r="C70" s="3"/>
     </row>
-    <row r="71" spans="1:3" ht="15.95" customHeight="1">
+    <row r="71" spans="1:3" ht="16" customHeight="1">
       <c r="A71" s="2"/>
       <c r="B71" s="3"/>
       <c r="C71" s="3"/>
     </row>
-    <row r="72" spans="1:3" ht="15.95" customHeight="1">
+    <row r="72" spans="1:3" ht="16" customHeight="1">
       <c r="A72" s="2"/>
       <c r="B72" s="3"/>
       <c r="C72" s="3"/>
     </row>
-    <row r="73" spans="1:3" ht="15.95" customHeight="1">
+    <row r="73" spans="1:3" ht="16" customHeight="1">
       <c r="A73" s="2"/>
       <c r="B73" s="3"/>
       <c r="C73" s="3"/>
     </row>
-    <row r="74" spans="1:3" ht="15.95" customHeight="1">
+    <row r="74" spans="1:3" ht="16" customHeight="1">
       <c r="A74" s="2"/>
       <c r="B74" s="3"/>
       <c r="C74" s="3"/>
     </row>
-    <row r="75" spans="1:3" ht="15.95" customHeight="1">
+    <row r="75" spans="1:3" ht="16" customHeight="1">
       <c r="A75" s="2"/>
       <c r="B75" s="3"/>
       <c r="C75" s="3"/>
     </row>
-    <row r="76" spans="1:3" ht="15.95" customHeight="1">
+    <row r="76" spans="1:3" ht="16" customHeight="1">
       <c r="A76" s="2"/>
       <c r="B76" s="3"/>
       <c r="C76" s="3"/>
     </row>
-    <row r="77" spans="1:3" ht="15.95" customHeight="1">
+    <row r="77" spans="1:3" ht="16" customHeight="1">
       <c r="A77" s="2"/>
       <c r="B77" s="3"/>
       <c r="C77" s="3"/>
     </row>
-    <row r="78" spans="1:3" ht="15.95" customHeight="1">
+    <row r="78" spans="1:3" ht="16" customHeight="1">
       <c r="A78" s="2"/>
       <c r="B78" s="3"/>
       <c r="C78" s="3"/>
     </row>
-    <row r="79" spans="1:3" ht="15.95" customHeight="1">
+    <row r="79" spans="1:3" ht="16" customHeight="1">
       <c r="A79" s="2"/>
       <c r="B79" s="3"/>
       <c r="C79" s="3"/>
     </row>
-    <row r="80" spans="1:3" ht="15.95" customHeight="1">
+    <row r="80" spans="1:3" ht="16" customHeight="1">
       <c r="A80" s="2"/>
       <c r="B80" s="3"/>
       <c r="C80" s="3"/>
     </row>
-    <row r="81" spans="1:3" ht="15.95" customHeight="1">
+    <row r="81" spans="1:3" ht="16" customHeight="1">
       <c r="A81" s="2"/>
       <c r="B81" s="3"/>
       <c r="C81" s="3"/>
     </row>
-    <row r="82" spans="1:3" ht="15.95" customHeight="1">
+    <row r="82" spans="1:3" ht="16" customHeight="1">
       <c r="A82" s="2"/>
       <c r="B82" s="3"/>
       <c r="C82" s="3"/>
     </row>
-    <row r="83" spans="1:3" ht="15.95" customHeight="1">
+    <row r="83" spans="1:3" ht="16" customHeight="1">
       <c r="A83" s="2"/>
       <c r="B83" s="3"/>
       <c r="C83" s="3"/>
     </row>
-    <row r="84" spans="1:3" ht="15.95" customHeight="1">
+    <row r="84" spans="1:3" ht="16" customHeight="1">
       <c r="A84" s="2"/>
       <c r="B84" s="3"/>
       <c r="C84" s="3"/>
     </row>
-    <row r="85" spans="1:3" ht="15.95" customHeight="1">
+    <row r="85" spans="1:3" ht="16" customHeight="1">
       <c r="A85" s="2"/>
       <c r="B85" s="3"/>
       <c r="C85" s="3"/>
     </row>
-    <row r="86" spans="1:3" ht="15.95" customHeight="1">
+    <row r="86" spans="1:3" ht="16" customHeight="1">
       <c r="A86" s="2"/>
       <c r="B86" s="3"/>
       <c r="C86" s="3"/>
     </row>
-    <row r="87" spans="1:3" ht="15.95" customHeight="1">
+    <row r="87" spans="1:3" ht="16" customHeight="1">
       <c r="A87" s="2"/>
       <c r="B87" s="3"/>
       <c r="C87" s="3"/>
     </row>
-    <row r="88" spans="1:3" ht="15.95" customHeight="1">
+    <row r="88" spans="1:3" ht="16" customHeight="1">
       <c r="A88" s="2"/>
       <c r="B88" s="3"/>
       <c r="C88" s="3"/>
     </row>
-    <row r="89" spans="1:3" ht="15.95" customHeight="1">
+    <row r="89" spans="1:3" ht="16" customHeight="1">
       <c r="A89" s="2"/>
       <c r="B89" s="3"/>
       <c r="C89" s="3"/>
     </row>
-    <row r="90" spans="1:3" ht="15.95" customHeight="1">
+    <row r="90" spans="1:3" ht="16" customHeight="1">
       <c r="A90" s="2"/>
       <c r="B90" s="3"/>
       <c r="C90" s="3"/>
     </row>
-    <row r="91" spans="1:3" ht="15.95" customHeight="1">
+    <row r="91" spans="1:3" ht="16" customHeight="1">
       <c r="A91" s="2"/>
       <c r="B91" s="3"/>
       <c r="C91" s="3"/>
     </row>
-    <row r="92" spans="1:3" ht="15.95" customHeight="1">
+    <row r="92" spans="1:3" ht="16" customHeight="1">
       <c r="A92" s="2"/>
       <c r="B92" s="3"/>
       <c r="C92" s="3"/>
     </row>
-    <row r="93" spans="1:3" ht="15.95" customHeight="1">
+    <row r="93" spans="1:3" ht="16" customHeight="1">
       <c r="A93" s="2"/>
       <c r="B93" s="3"/>
       <c r="C93" s="3"/>
     </row>
-    <row r="94" spans="1:3" ht="15.95" customHeight="1">
+    <row r="94" spans="1:3" ht="16" customHeight="1">
       <c r="A94" s="2"/>
       <c r="B94" s="3"/>
       <c r="C94" s="3"/>
     </row>
-    <row r="95" spans="1:3" ht="15.95" customHeight="1">
+    <row r="95" spans="1:3" ht="16" customHeight="1">
       <c r="A95" s="2"/>
       <c r="B95" s="3"/>
       <c r="C95" s="3"/>
     </row>
-    <row r="96" spans="1:3" ht="15.95" customHeight="1">
+    <row r="96" spans="1:3" ht="16" customHeight="1">
       <c r="A96" s="2"/>
       <c r="B96" s="3"/>
       <c r="C96" s="3"/>
     </row>
-    <row r="97" spans="1:3" ht="15.95" customHeight="1">
+    <row r="97" spans="1:3" ht="16" customHeight="1">
       <c r="A97" s="2"/>
       <c r="B97" s="3"/>
       <c r="C97" s="3"/>
     </row>
-    <row r="98" spans="1:3" ht="15.95" customHeight="1">
+    <row r="98" spans="1:3" ht="16" customHeight="1">
       <c r="A98" s="2"/>
       <c r="B98" s="3"/>
       <c r="C98" s="3"/>
     </row>
-    <row r="99" spans="1:3" ht="15.95" customHeight="1">
+    <row r="99" spans="1:3" ht="16" customHeight="1">
       <c r="A99" s="2"/>
       <c r="B99" s="3"/>
       <c r="C99" s="3"/>
     </row>
-    <row r="100" spans="1:3" ht="15.95" customHeight="1">
+    <row r="100" spans="1:3" ht="16" customHeight="1">
       <c r="A100" s="2"/>
       <c r="B100" s="3"/>
       <c r="C100" s="3"/>
     </row>
-    <row r="101" spans="1:3" ht="15.95" customHeight="1">
+    <row r="101" spans="1:3" ht="16" customHeight="1">
       <c r="A101" s="2"/>
       <c r="B101" s="3"/>
       <c r="C101" s="3"/>
     </row>
-    <row r="102" spans="1:3" ht="15.95" customHeight="1">
+    <row r="102" spans="1:3" ht="16" customHeight="1">
       <c r="A102" s="2"/>
       <c r="B102" s="3"/>
       <c r="C102" s="3"/>
     </row>
-    <row r="103" spans="1:3" ht="15.95" customHeight="1">
+    <row r="103" spans="1:3" ht="16" customHeight="1">
       <c r="A103" s="2"/>
       <c r="B103" s="3"/>
       <c r="C103" s="3"/>
     </row>
-    <row r="104" spans="1:3" ht="15.95" customHeight="1">
+    <row r="104" spans="1:3" ht="16" customHeight="1">
       <c r="A104" s="2"/>
       <c r="B104" s="3"/>
       <c r="C104" s="3"/>
     </row>
-    <row r="105" spans="1:3" ht="15.95" customHeight="1">
+    <row r="105" spans="1:3" ht="16" customHeight="1">
       <c r="A105" s="2"/>
       <c r="B105" s="3"/>
       <c r="C105" s="3"/>
     </row>
-    <row r="106" spans="1:3" ht="15.95" customHeight="1">
+    <row r="106" spans="1:3" ht="16" customHeight="1">
       <c r="A106" s="2"/>
       <c r="B106" s="3"/>
       <c r="C106" s="3"/>
     </row>
-    <row r="107" spans="1:3" ht="15.95" customHeight="1">
+    <row r="107" spans="1:3" ht="16" customHeight="1">
       <c r="A107" s="2"/>
       <c r="B107" s="3"/>
       <c r="C107" s="3"/>
     </row>
-    <row r="108" spans="1:3" ht="15.95" customHeight="1">
+    <row r="108" spans="1:3" ht="16" customHeight="1">
       <c r="A108" s="2"/>
       <c r="B108" s="3"/>
       <c r="C108" s="3"/>
     </row>
-    <row r="109" spans="1:3" ht="15.95" customHeight="1">
+    <row r="109" spans="1:3" ht="16" customHeight="1">
       <c r="A109" s="2"/>
       <c r="B109" s="3"/>
       <c r="C109" s="3"/>
     </row>
-    <row r="110" spans="1:3" ht="15.95" customHeight="1">
+    <row r="110" spans="1:3" ht="16" customHeight="1">
       <c r="A110" s="2"/>
       <c r="B110" s="3"/>
       <c r="C110" s="3"/>
     </row>
-    <row r="111" spans="1:3" ht="15.95" customHeight="1">
+    <row r="111" spans="1:3" ht="16" customHeight="1">
       <c r="A111" s="2"/>
       <c r="B111" s="3"/>
       <c r="C111" s="3"/>
     </row>
-    <row r="112" spans="1:3" ht="15.95" customHeight="1">
+    <row r="112" spans="1:3" ht="16" customHeight="1">
       <c r="A112" s="2"/>
       <c r="B112" s="3"/>
       <c r="C112" s="3"/>
     </row>
-    <row r="113" spans="1:3" ht="15.95" customHeight="1">
+    <row r="113" spans="1:3" ht="16" customHeight="1">
       <c r="A113" s="2"/>
       <c r="B113" s="3"/>
       <c r="C113" s="3"/>
     </row>
-    <row r="114" spans="1:3" ht="15.95" customHeight="1">
+    <row r="114" spans="1:3" ht="16" customHeight="1">
       <c r="A114" s="2"/>
       <c r="B114" s="3"/>
       <c r="C114" s="3"/>
     </row>
-    <row r="115" spans="1:3" ht="15.95" customHeight="1">
+    <row r="115" spans="1:3" ht="16" customHeight="1">
       <c r="A115" s="2"/>
       <c r="B115" s="3"/>
       <c r="C115" s="3"/>
     </row>
-    <row r="116" spans="1:3" ht="15.95" customHeight="1">
+    <row r="116" spans="1:3" ht="16" customHeight="1">
       <c r="A116" s="2"/>
       <c r="B116" s="3"/>
       <c r="C116" s="3"/>
     </row>
-    <row r="117" spans="1:3" ht="15.95" customHeight="1">
+    <row r="117" spans="1:3" ht="16" customHeight="1">
       <c r="A117" s="2"/>
       <c r="B117" s="3"/>
       <c r="C117" s="3"/>
     </row>
-    <row r="118" spans="1:3" ht="15.95" customHeight="1">
+    <row r="118" spans="1:3" ht="16" customHeight="1">
       <c r="A118" s="2"/>
       <c r="B118" s="3"/>
       <c r="C118" s="3"/>
     </row>
-    <row r="119" spans="1:3" ht="15.95" customHeight="1">
+    <row r="119" spans="1:3" ht="16" customHeight="1">
       <c r="A119" s="2"/>
       <c r="B119" s="3"/>
       <c r="C119" s="3"/>
     </row>
-    <row r="120" spans="1:3" ht="15.95" customHeight="1">
+    <row r="120" spans="1:3" ht="16" customHeight="1">
       <c r="A120" s="2"/>
       <c r="B120" s="3"/>
       <c r="C120" s="3"/>
     </row>
-    <row r="121" spans="1:3" ht="15.95" customHeight="1">
+    <row r="121" spans="1:3" ht="16" customHeight="1">
       <c r="A121" s="2"/>
       <c r="B121" s="3"/>
       <c r="C121" s="3"/>
     </row>
-    <row r="122" spans="1:3" ht="15.95" customHeight="1">
+    <row r="122" spans="1:3" ht="16" customHeight="1">
       <c r="A122" s="2"/>
       <c r="B122" s="3"/>
       <c r="C122" s="3"/>
     </row>
-    <row r="123" spans="1:3" ht="15.95" customHeight="1">
+    <row r="123" spans="1:3" ht="16" customHeight="1">
       <c r="A123" s="2"/>
       <c r="B123" s="3"/>
       <c r="C123" s="3"/>
     </row>
-    <row r="124" spans="1:3" ht="15.95" customHeight="1">
+    <row r="124" spans="1:3" ht="16" customHeight="1">
       <c r="A124" s="2"/>
       <c r="B124" s="3"/>
       <c r="C124" s="3"/>
     </row>
-    <row r="125" spans="1:3" ht="15.95" customHeight="1">
+    <row r="125" spans="1:3" ht="16" customHeight="1">
       <c r="A125" s="2"/>
       <c r="B125" s="3"/>
       <c r="C125" s="3"/>
     </row>
-    <row r="126" spans="1:3" ht="15.95" customHeight="1">
+    <row r="126" spans="1:3" ht="16" customHeight="1">
       <c r="A126" s="2"/>
       <c r="B126" s="3"/>
       <c r="C126" s="3"/>
     </row>
-    <row r="127" spans="1:3" ht="15.95" customHeight="1">
+    <row r="127" spans="1:3" ht="16" customHeight="1">
       <c r="A127" s="2"/>
       <c r="B127" s="3"/>
       <c r="C127" s="3"/>
     </row>
-    <row r="128" spans="1:3" ht="15.95" customHeight="1">
+    <row r="128" spans="1:3" ht="16" customHeight="1">
       <c r="A128" s="2"/>
       <c r="B128" s="3"/>
       <c r="C128" s="3"/>
     </row>
-    <row r="129" spans="1:3" ht="15.95" customHeight="1">
+    <row r="129" spans="1:3" ht="16" customHeight="1">
       <c r="A129" s="2"/>
       <c r="B129" s="3"/>
       <c r="C129" s="3"/>
     </row>
-    <row r="130" spans="1:3" ht="15.95" customHeight="1">
+    <row r="130" spans="1:3" ht="16" customHeight="1">
       <c r="A130" s="2"/>
       <c r="B130" s="3"/>
       <c r="C130" s="3"/>
     </row>
-    <row r="131" spans="1:3" ht="15.95" customHeight="1">
+    <row r="131" spans="1:3" ht="16" customHeight="1">
       <c r="A131" s="2"/>
       <c r="B131" s="3"/>
       <c r="C131" s="3"/>
     </row>
-    <row r="132" spans="1:3" ht="15.95" customHeight="1">
+    <row r="132" spans="1:3" ht="16" customHeight="1">
       <c r="A132" s="2"/>
       <c r="B132" s="3"/>
       <c r="C132" s="3"/>
     </row>
-    <row r="133" spans="1:3" ht="15.95" customHeight="1">
+    <row r="133" spans="1:3" ht="16" customHeight="1">
       <c r="A133" s="2"/>
       <c r="B133" s="3"/>
       <c r="C133" s="3"/>
     </row>
-    <row r="134" spans="1:3" ht="15.95" customHeight="1">
+    <row r="134" spans="1:3" ht="16" customHeight="1">
       <c r="A134" s="2"/>
       <c r="B134" s="3"/>
       <c r="C134" s="3"/>
     </row>
-    <row r="135" spans="1:3" ht="15.95" customHeight="1">
+    <row r="135" spans="1:3" ht="16" customHeight="1">
       <c r="A135" s="2"/>
       <c r="B135" s="3"/>
       <c r="C135" s="3"/>
     </row>
-    <row r="136" spans="1:3" ht="15.95" customHeight="1">
+    <row r="136" spans="1:3" ht="16" customHeight="1">
       <c r="A136" s="2"/>
       <c r="B136" s="3"/>
       <c r="C136" s="3"/>
     </row>
-    <row r="137" spans="1:3" ht="15.95" customHeight="1">
+    <row r="137" spans="1:3" ht="16" customHeight="1">
       <c r="A137" s="2"/>
       <c r="B137" s="3"/>
       <c r="C137" s="3"/>
     </row>
-    <row r="138" spans="1:3" ht="15.95" customHeight="1">
+    <row r="138" spans="1:3" ht="16" customHeight="1">
       <c r="A138" s="2"/>
       <c r="B138" s="3"/>
       <c r="C138" s="3"/>
     </row>
-    <row r="139" spans="1:3" ht="15.95" customHeight="1">
+    <row r="139" spans="1:3" ht="16" customHeight="1">
       <c r="A139" s="2"/>
       <c r="B139" s="3"/>
       <c r="C139" s="3"/>
     </row>
-    <row r="140" spans="1:3" ht="15.95" customHeight="1">
+    <row r="140" spans="1:3" ht="16" customHeight="1">
       <c r="A140" s="2"/>
       <c r="B140" s="3"/>
       <c r="C140" s="3"/>
     </row>
-    <row r="141" spans="1:3" ht="15.95" customHeight="1">
+    <row r="141" spans="1:3" ht="16" customHeight="1">
       <c r="A141" s="2"/>
       <c r="B141" s="3"/>
       <c r="C141" s="3"/>
     </row>
-    <row r="142" spans="1:3" ht="15.95" customHeight="1">
+    <row r="142" spans="1:3" ht="16" customHeight="1">
       <c r="A142" s="2"/>
       <c r="B142" s="3"/>
       <c r="C142" s="3"/>
     </row>
-    <row r="143" spans="1:3" ht="15.95" customHeight="1">
+    <row r="143" spans="1:3" ht="16" customHeight="1">
       <c r="A143" s="2"/>
       <c r="B143" s="3"/>
       <c r="C143" s="3"/>
     </row>
-    <row r="144" spans="1:3" ht="15.95" customHeight="1">
+    <row r="144" spans="1:3" ht="16" customHeight="1">
       <c r="A144" s="2"/>
       <c r="B144" s="3"/>
       <c r="C144" s="3"/>
     </row>
-    <row r="145" spans="1:3" ht="15.95" customHeight="1">
+    <row r="145" spans="1:3" ht="16" customHeight="1">
       <c r="A145" s="2"/>
       <c r="B145" s="3"/>
       <c r="C145" s="3"/>
     </row>
-    <row r="146" spans="1:3" ht="15.95" customHeight="1">
+    <row r="146" spans="1:3" ht="16" customHeight="1">
       <c r="A146" s="2"/>
       <c r="B146" s="3"/>
       <c r="C146" s="3"/>
     </row>
-    <row r="147" spans="1:3" ht="15.95" customHeight="1">
+    <row r="147" spans="1:3" ht="16" customHeight="1">
       <c r="A147" s="2"/>
       <c r="B147" s="3"/>
       <c r="C147" s="3"/>
     </row>
-    <row r="148" spans="1:3" ht="15.95" customHeight="1">
+    <row r="148" spans="1:3" ht="16" customHeight="1">
       <c r="A148" s="2"/>
       <c r="B148" s="3"/>
       <c r="C148" s="3"/>
     </row>
-    <row r="149" spans="1:3" ht="15.95" customHeight="1">
+    <row r="149" spans="1:3" ht="16" customHeight="1">
       <c r="A149" s="2"/>
       <c r="B149" s="3"/>
       <c r="C149" s="3"/>
     </row>
-    <row r="150" spans="1:3" ht="15.95" customHeight="1">
+    <row r="150" spans="1:3" ht="16" customHeight="1">
       <c r="A150" s="2"/>
       <c r="B150" s="3"/>
       <c r="C150" s="3"/>
     </row>
-    <row r="151" spans="1:3" ht="15.95" customHeight="1">
+    <row r="151" spans="1:3" ht="16" customHeight="1">
       <c r="A151" s="2"/>
       <c r="B151" s="3"/>
       <c r="C151" s="3"/>
     </row>
-    <row r="152" spans="1:3" ht="15.95" customHeight="1">
+    <row r="152" spans="1:3" ht="16" customHeight="1">
       <c r="A152" s="2"/>
       <c r="B152" s="3"/>
       <c r="C152" s="3"/>
     </row>
-    <row r="153" spans="1:3" ht="15.95" customHeight="1">
+    <row r="153" spans="1:3" ht="16" customHeight="1">
       <c r="A153" s="2"/>
       <c r="B153" s="3"/>
       <c r="C153" s="3"/>
     </row>
-    <row r="154" spans="1:3" ht="15.95" customHeight="1">
+    <row r="154" spans="1:3" ht="16" customHeight="1">
       <c r="A154" s="2"/>
       <c r="B154" s="3"/>
       <c r="C154" s="3"/>
     </row>
-    <row r="155" spans="1:3" ht="15.95" customHeight="1">
+    <row r="155" spans="1:3" ht="16" customHeight="1">
       <c r="A155" s="2"/>
       <c r="B155" s="3"/>
       <c r="C155" s="3"/>
     </row>
-    <row r="156" spans="1:3" ht="15.95" customHeight="1">
+    <row r="156" spans="1:3" ht="16" customHeight="1">
       <c r="A156" s="2"/>
       <c r="B156" s="3"/>
       <c r="C156" s="3"/>
     </row>
-    <row r="157" spans="1:3" ht="15.95" customHeight="1">
+    <row r="157" spans="1:3" ht="16" customHeight="1">
       <c r="A157" s="2"/>
       <c r="B157" s="3"/>
       <c r="C157" s="3"/>
     </row>
-    <row r="158" spans="1:3" ht="15.95" customHeight="1">
+    <row r="158" spans="1:3" ht="16" customHeight="1">
       <c r="A158" s="2"/>
       <c r="B158" s="3"/>
       <c r="C158" s="3"/>
     </row>
-    <row r="159" spans="1:3" ht="15.95" customHeight="1">
+    <row r="159" spans="1:3" ht="16" customHeight="1">
       <c r="A159" s="2"/>
       <c r="B159" s="3"/>
       <c r="C159" s="3"/>
     </row>
-    <row r="160" spans="1:3" ht="15.95" customHeight="1">
+    <row r="160" spans="1:3" ht="16" customHeight="1">
       <c r="A160" s="2"/>
       <c r="B160" s="3"/>
       <c r="C160" s="3"/>
     </row>
-    <row r="161" spans="1:3" ht="15.95" customHeight="1">
+    <row r="161" spans="1:3" ht="16" customHeight="1">
       <c r="A161" s="2"/>
       <c r="B161" s="3"/>
       <c r="C161" s="3"/>
     </row>
-    <row r="162" spans="1:3" ht="15.95" customHeight="1">
+    <row r="162" spans="1:3" ht="16" customHeight="1">
       <c r="A162" s="2"/>
       <c r="B162" s="3"/>
       <c r="C162" s="3"/>
     </row>
-    <row r="163" spans="1:3" ht="15.95" customHeight="1">
+    <row r="163" spans="1:3" ht="16" customHeight="1">
       <c r="A163" s="2"/>
       <c r="B163" s="3"/>
       <c r="C163" s="3"/>
     </row>
-    <row r="164" spans="1:3" ht="15.95" customHeight="1">
+    <row r="164" spans="1:3" ht="16" customHeight="1">
       <c r="A164" s="2"/>
       <c r="B164" s="3"/>
       <c r="C164" s="3"/>
     </row>
-    <row r="165" spans="1:3" ht="15.95" customHeight="1">
+    <row r="165" spans="1:3" ht="16" customHeight="1">
       <c r="A165" s="2"/>
       <c r="B165" s="3"/>
       <c r="C165" s="3"/>
     </row>
-    <row r="166" spans="1:3" ht="15.95" customHeight="1">
+    <row r="166" spans="1:3" ht="16" customHeight="1">
       <c r="A166" s="2"/>
       <c r="B166" s="3"/>
       <c r="C166" s="3"/>
     </row>
-    <row r="167" spans="1:3" ht="15.95" customHeight="1">
+    <row r="167" spans="1:3" ht="16" customHeight="1">
       <c r="A167" s="2"/>
       <c r="B167" s="3"/>
       <c r="C167" s="3"/>
     </row>
-    <row r="168" spans="1:3" ht="15.95" customHeight="1">
+    <row r="168" spans="1:3" ht="16" customHeight="1">
       <c r="A168" s="2"/>
       <c r="B168" s="3"/>
       <c r="C168" s="3"/>
     </row>
-    <row r="169" spans="1:3" ht="15.95" customHeight="1">
+    <row r="169" spans="1:3" ht="16" customHeight="1">
       <c r="A169" s="2"/>
       <c r="B169" s="3"/>
       <c r="C169" s="3"/>
     </row>
-    <row r="170" spans="1:3" ht="15.95" customHeight="1">
+    <row r="170" spans="1:3" ht="16" customHeight="1">
       <c r="A170" s="2"/>
       <c r="B170" s="3"/>
       <c r="C170" s="3"/>
     </row>
-    <row r="171" spans="1:3" ht="15.95" customHeight="1">
+    <row r="171" spans="1:3" ht="16" customHeight="1">
       <c r="A171" s="2"/>
       <c r="B171" s="3"/>
       <c r="C171" s="3"/>
     </row>
-    <row r="172" spans="1:3" ht="15.95" customHeight="1">
+    <row r="172" spans="1:3" ht="16" customHeight="1">
       <c r="A172" s="2"/>
       <c r="B172" s="3"/>
       <c r="C172" s="3"/>
     </row>
-    <row r="173" spans="1:3" ht="15.95" customHeight="1">
+    <row r="173" spans="1:3" ht="16" customHeight="1">
       <c r="A173" s="2"/>
       <c r="B173" s="3"/>
       <c r="C173" s="3"/>
     </row>
-    <row r="174" spans="1:3" ht="15.95" customHeight="1">
+    <row r="174" spans="1:3" ht="16" customHeight="1">
       <c r="A174" s="2"/>
       <c r="B174" s="3"/>
       <c r="C174" s="3"/>
     </row>
-    <row r="175" spans="1:3" ht="15.95" customHeight="1">
+    <row r="175" spans="1:3" ht="16" customHeight="1">
       <c r="A175" s="2"/>
       <c r="B175" s="3"/>
       <c r="C175" s="3"/>
     </row>
-    <row r="176" spans="1:3" ht="15.95" customHeight="1">
+    <row r="176" spans="1:3" ht="16" customHeight="1">
       <c r="A176" s="2"/>
       <c r="B176" s="3"/>
       <c r="C176" s="3"/>
     </row>
-    <row r="177" spans="1:3" ht="15.95" customHeight="1">
+    <row r="177" spans="1:3" ht="16" customHeight="1">
       <c r="A177" s="2"/>
       <c r="B177" s="3"/>
       <c r="C177" s="3"/>
     </row>
-    <row r="178" spans="1:3" ht="15.95" customHeight="1">
+    <row r="178" spans="1:3" ht="16" customHeight="1">
       <c r="A178" s="2"/>
       <c r="B178" s="3"/>
       <c r="C178" s="3"/>
     </row>
-    <row r="179" spans="1:3" ht="15.95" customHeight="1">
+    <row r="179" spans="1:3" ht="16" customHeight="1">
       <c r="A179" s="2"/>
       <c r="B179" s="3"/>
       <c r="C179" s="3"/>
     </row>
-    <row r="180" spans="1:3" ht="15.95" customHeight="1">
+    <row r="180" spans="1:3" ht="16" customHeight="1">
       <c r="A180" s="2"/>
       <c r="B180" s="3"/>
       <c r="C180" s="3"/>
     </row>
-    <row r="181" spans="1:3" ht="15.95" customHeight="1">
+    <row r="181" spans="1:3" ht="16" customHeight="1">
       <c r="A181" s="2"/>
       <c r="B181" s="3"/>
       <c r="C181" s="3"/>
     </row>
-    <row r="182" spans="1:3" ht="15.95" customHeight="1">
+    <row r="182" spans="1:3" ht="16" customHeight="1">
       <c r="A182" s="2"/>
       <c r="B182" s="3"/>
       <c r="C182" s="3"/>
     </row>
-    <row r="183" spans="1:3" ht="15.95" customHeight="1">
+    <row r="183" spans="1:3" ht="16" customHeight="1">
       <c r="A183" s="2"/>
       <c r="B183" s="3"/>
       <c r="C183" s="3"/>
     </row>
-    <row r="184" spans="1:3" ht="15.95" customHeight="1">
+    <row r="184" spans="1:3" ht="16" customHeight="1">
       <c r="A184" s="2"/>
       <c r="B184" s="3"/>
       <c r="C184" s="3"/>
     </row>
-    <row r="185" spans="1:3" ht="15.95" customHeight="1">
+    <row r="185" spans="1:3" ht="16" customHeight="1">
       <c r="A185" s="2"/>
       <c r="B185" s="3"/>
       <c r="C185" s="3"/>
     </row>
-    <row r="186" spans="1:3" ht="15.95" customHeight="1">
+    <row r="186" spans="1:3" ht="16" customHeight="1">
       <c r="A186" s="2"/>
       <c r="B186" s="3"/>
       <c r="C186" s="3"/>
     </row>
-    <row r="187" spans="1:3" ht="15.95" customHeight="1">
+    <row r="187" spans="1:3" ht="16" customHeight="1">
       <c r="A187" s="2"/>
       <c r="B187" s="3"/>
       <c r="C187" s="3"/>
     </row>
-    <row r="188" spans="1:3" ht="15.95" customHeight="1">
+    <row r="188" spans="1:3" ht="16" customHeight="1">
       <c r="A188" s="2"/>
       <c r="B188" s="3"/>
       <c r="C188" s="3"/>
     </row>
-    <row r="189" spans="1:3" ht="15.95" customHeight="1">
+    <row r="189" spans="1:3" ht="16" customHeight="1">
       <c r="A189" s="2"/>
       <c r="B189" s="3"/>
       <c r="C189" s="3"/>
     </row>
-    <row r="190" spans="1:3" ht="15.95" customHeight="1">
+    <row r="190" spans="1:3" ht="16" customHeight="1">
       <c r="A190" s="2"/>
       <c r="B190" s="3"/>
       <c r="C190" s="3"/>
     </row>
-    <row r="191" spans="1:3" ht="15.95" customHeight="1">
+    <row r="191" spans="1:3" ht="16" customHeight="1">
       <c r="A191" s="2"/>
       <c r="B191" s="3"/>
       <c r="C191" s="3"/>
     </row>
-    <row r="192" spans="1:3" ht="15.95" customHeight="1">
+    <row r="192" spans="1:3" ht="16" customHeight="1">
       <c r="A192" s="2"/>
       <c r="B192" s="3"/>
       <c r="C192" s="3"/>
     </row>
-    <row r="193" spans="1:3" ht="15.95" customHeight="1">
+    <row r="193" spans="1:3" ht="16" customHeight="1">
       <c r="A193" s="2"/>
       <c r="B193" s="3"/>
       <c r="C193" s="3"/>
     </row>
-    <row r="194" spans="1:3" ht="15.95" customHeight="1">
+    <row r="194" spans="1:3" ht="16" customHeight="1">
       <c r="A194" s="2"/>
       <c r="B194" s="3"/>
       <c r="C194" s="3"/>
     </row>
-    <row r="195" spans="1:3" ht="15.95" customHeight="1">
+    <row r="195" spans="1:3" ht="16" customHeight="1">
       <c r="A195" s="2"/>
       <c r="B195" s="3"/>
       <c r="C195" s="3"/>
     </row>
-    <row r="196" spans="1:3" ht="15.95" customHeight="1">
+    <row r="196" spans="1:3" ht="16" customHeight="1">
       <c r="A196" s="2"/>
       <c r="B196" s="3"/>
       <c r="C196" s="3"/>
     </row>
-    <row r="197" spans="1:3" ht="15.95" customHeight="1">
+    <row r="197" spans="1:3" ht="16" customHeight="1">
       <c r="A197" s="2"/>
       <c r="B197" s="3"/>
       <c r="C197" s="3"/>
     </row>
-    <row r="198" spans="1:3" ht="15.95" customHeight="1">
+    <row r="198" spans="1:3" ht="16" customHeight="1">
       <c r="A198" s="2"/>
       <c r="B198" s="3"/>
       <c r="C198" s="3"/>
     </row>
-    <row r="199" spans="1:3" ht="15.95" customHeight="1">
+    <row r="199" spans="1:3" ht="16" customHeight="1">
       <c r="A199" s="2"/>
       <c r="B199" s="3"/>
       <c r="C199" s="3"/>
     </row>
-    <row r="200" spans="1:3" ht="15.95" customHeight="1">
+    <row r="200" spans="1:3" ht="16" customHeight="1">
       <c r="A200" s="2"/>
       <c r="B200" s="3"/>
       <c r="C200" s="3"/>
     </row>
-    <row r="201" spans="1:3" ht="15.95" customHeight="1">
+    <row r="201" spans="1:3" ht="16" customHeight="1">
       <c r="A201" s="2"/>
       <c r="B201" s="3"/>
       <c r="C201" s="3"/>
     </row>
-    <row r="202" spans="1:3" ht="15.95" customHeight="1">
+    <row r="202" spans="1:3" ht="16" customHeight="1">
       <c r="A202" s="2"/>
       <c r="B202" s="3"/>
       <c r="C202" s="3"/>
     </row>
-    <row r="203" spans="1:3" ht="15.95" customHeight="1">
+    <row r="203" spans="1:3" ht="16" customHeight="1">
       <c r="A203" s="2"/>
       <c r="B203" s="3"/>
       <c r="C203" s="3"/>
     </row>
-    <row r="204" spans="1:3" ht="15.95" customHeight="1">
+    <row r="204" spans="1:3" ht="16" customHeight="1">
       <c r="A204" s="2"/>
       <c r="B204" s="3"/>
       <c r="C204" s="3"/>
     </row>
-    <row r="205" spans="1:3" ht="15.95" customHeight="1">
+    <row r="205" spans="1:3" ht="16" customHeight="1">
       <c r="A205" s="2"/>
       <c r="B205" s="3"/>
       <c r="C205" s="3"/>
     </row>
-    <row r="206" spans="1:3" ht="15.95" customHeight="1">
+    <row r="206" spans="1:3" ht="16" customHeight="1">
       <c r="A206" s="2"/>
       <c r="B206" s="3"/>
       <c r="C206" s="3"/>
     </row>
-    <row r="207" spans="1:3" ht="15.95" customHeight="1">
+    <row r="207" spans="1:3" ht="16" customHeight="1">
       <c r="A207" s="2"/>
       <c r="B207" s="3"/>
       <c r="C207" s="3"/>
     </row>
-    <row r="208" spans="1:3" ht="15.95" customHeight="1">
+    <row r="208" spans="1:3" ht="16" customHeight="1">
       <c r="A208" s="2"/>
       <c r="B208" s="3"/>
       <c r="C208" s="3"/>
     </row>
-    <row r="209" spans="1:3" ht="15.95" customHeight="1">
+    <row r="209" spans="1:3" ht="16" customHeight="1">
       <c r="A209" s="2"/>
       <c r="B209" s="3"/>
       <c r="C209" s="3"/>
     </row>
-    <row r="210" spans="1:3" ht="15.95" customHeight="1">
+    <row r="210" spans="1:3" ht="16" customHeight="1">
       <c r="A210" s="2"/>
       <c r="B210" s="3"/>
       <c r="C210" s="3"/>
     </row>
-    <row r="211" spans="1:3" ht="15.95" customHeight="1">
+    <row r="211" spans="1:3" ht="16" customHeight="1">
       <c r="A211" s="2"/>
       <c r="B211" s="3"/>
       <c r="C211" s="3"/>
     </row>
-    <row r="212" spans="1:3" ht="15.95" customHeight="1">
+    <row r="212" spans="1:3" ht="16" customHeight="1">
       <c r="A212" s="2"/>
       <c r="B212" s="3"/>
       <c r="C212" s="3"/>
     </row>
-    <row r="213" spans="1:3" ht="15.95" customHeight="1">
+    <row r="213" spans="1:3" ht="16" customHeight="1">
       <c r="A213" s="2"/>
       <c r="B213" s="3"/>
       <c r="C213" s="3"/>
     </row>
-    <row r="214" spans="1:3" ht="15.95" customHeight="1">
+    <row r="214" spans="1:3" ht="16" customHeight="1">
       <c r="A214" s="2"/>
       <c r="B214" s="3"/>
       <c r="C214" s="3"/>
     </row>
-    <row r="215" spans="1:3" ht="15.95" customHeight="1">
+    <row r="215" spans="1:3" ht="16" customHeight="1">
       <c r="A215" s="2"/>
       <c r="B215" s="3"/>
       <c r="C215" s="3"/>
     </row>
-    <row r="216" spans="1:3" ht="15.95" customHeight="1">
+    <row r="216" spans="1:3" ht="16" customHeight="1">
       <c r="A216" s="2"/>
       <c r="B216" s="3"/>
       <c r="C216" s="3"/>
     </row>
-    <row r="217" spans="1:3" ht="15.95" customHeight="1">
+    <row r="217" spans="1:3" ht="16" customHeight="1">
       <c r="A217" s="2"/>
       <c r="B217" s="3"/>
       <c r="C217" s="3"/>
     </row>
-    <row r="218" spans="1:3" ht="15.95" customHeight="1">
+    <row r="218" spans="1:3" ht="16" customHeight="1">
       <c r="A218" s="2"/>
       <c r="B218" s="3"/>
       <c r="C218" s="3"/>
     </row>
-    <row r="219" spans="1:3" ht="15.95" customHeight="1">
+    <row r="219" spans="1:3" ht="16" customHeight="1">
       <c r="A219" s="2"/>
       <c r="B219" s="3"/>
       <c r="C219" s="3"/>
     </row>
-    <row r="220" spans="1:3" ht="15.95" customHeight="1">
+    <row r="220" spans="1:3" ht="16" customHeight="1">
       <c r="A220" s="2"/>
       <c r="B220" s="3"/>
       <c r="C220" s="3"/>
     </row>
-    <row r="221" spans="1:3" ht="15.95" customHeight="1">
+    <row r="221" spans="1:3" ht="16" customHeight="1">
       <c r="A221" s="2"/>
       <c r="B221" s="3"/>
       <c r="C221" s="3"/>
     </row>
-    <row r="222" spans="1:3" ht="15.95" customHeight="1">
+    <row r="222" spans="1:3" ht="16" customHeight="1">
       <c r="A222" s="2"/>
       <c r="B222" s="3"/>
       <c r="C222" s="3"/>
     </row>
-    <row r="223" spans="1:3" ht="15.95" customHeight="1">
+    <row r="223" spans="1:3" ht="16" customHeight="1">
       <c r="A223" s="2"/>
       <c r="B223" s="3"/>
       <c r="C223" s="3"/>
     </row>
-    <row r="224" spans="1:3" ht="15.95" customHeight="1">
+    <row r="224" spans="1:3" ht="16" customHeight="1">
       <c r="A224" s="2"/>
       <c r="B224" s="3"/>
       <c r="C224" s="3"/>
     </row>
-    <row r="225" spans="1:3" ht="15.95" customHeight="1">
+    <row r="225" spans="1:3" ht="16" customHeight="1">
       <c r="A225" s="2"/>
       <c r="B225" s="3"/>
       <c r="C225" s="3"/>
     </row>
-    <row r="226" spans="1:3" ht="15.95" customHeight="1">
+    <row r="226" spans="1:3" ht="16" customHeight="1">
       <c r="A226" s="2"/>
       <c r="B226" s="3"/>
       <c r="C226" s="3"/>
     </row>
-    <row r="227" spans="1:3" ht="15.95" customHeight="1">
+    <row r="227" spans="1:3" ht="16" customHeight="1">
       <c r="A227" s="2"/>
       <c r="B227" s="3"/>
       <c r="C227" s="3"/>
     </row>
-    <row r="228" spans="1:3" ht="15.95" customHeight="1">
+    <row r="228" spans="1:3" ht="16" customHeight="1">
       <c r="A228" s="2"/>
       <c r="B228" s="3"/>
       <c r="C228" s="3"/>
     </row>
-    <row r="229" spans="1:3" ht="15.95" customHeight="1">
+    <row r="229" spans="1:3" ht="16" customHeight="1">
       <c r="A229" s="2"/>
       <c r="B229" s="3"/>
       <c r="C229" s="3"/>
     </row>
-    <row r="230" spans="1:3" ht="15.95" customHeight="1">
+    <row r="230" spans="1:3" ht="16" customHeight="1">
       <c r="A230" s="2"/>
       <c r="B230" s="3"/>
       <c r="C230" s="3"/>
     </row>
-    <row r="231" spans="1:3" ht="15.95" customHeight="1">
+    <row r="231" spans="1:3" ht="16" customHeight="1">
       <c r="A231" s="2"/>
       <c r="B231" s="3"/>
       <c r="C231" s="3"/>
     </row>
-    <row r="232" spans="1:3" ht="15.95" customHeight="1">
+    <row r="232" spans="1:3" ht="16" customHeight="1">
       <c r="A232" s="2"/>
       <c r="B232" s="3"/>
       <c r="C232" s="3"/>
     </row>
-    <row r="233" spans="1:3" ht="15.95" customHeight="1">
+    <row r="233" spans="1:3" ht="16" customHeight="1">
       <c r="A233" s="2"/>
       <c r="B233" s="3"/>
       <c r="C233" s="3"/>
     </row>
-    <row r="234" spans="1:3" ht="15.95" customHeight="1">
+    <row r="234" spans="1:3" ht="16" customHeight="1">
       <c r="A234" s="2"/>
       <c r="B234" s="3"/>
       <c r="C234" s="3"/>
     </row>
-    <row r="235" spans="1:3" ht="15.95" customHeight="1">
+    <row r="235" spans="1:3" ht="16" customHeight="1">
       <c r="A235" s="2"/>
       <c r="B235" s="3"/>
       <c r="C235" s="3"/>
     </row>
-    <row r="236" spans="1:3" ht="15.95" customHeight="1">
+    <row r="236" spans="1:3" ht="16" customHeight="1">
       <c r="A236" s="2"/>
       <c r="B236" s="3"/>
       <c r="C236" s="3"/>
     </row>
-    <row r="237" spans="1:3" ht="15.95" customHeight="1">
+    <row r="237" spans="1:3" ht="16" customHeight="1">
       <c r="A237" s="2"/>
       <c r="B237" s="3"/>
       <c r="C237" s="3"/>
     </row>
-    <row r="238" spans="1:3" ht="15.95" customHeight="1">
+    <row r="238" spans="1:3" ht="16" customHeight="1">
       <c r="A238" s="2"/>
       <c r="B238" s="3"/>
       <c r="C238" s="3"/>
     </row>
-    <row r="239" spans="1:3" ht="15.95" customHeight="1">
+    <row r="239" spans="1:3" ht="16" customHeight="1">
       <c r="A239" s="2"/>
       <c r="B239" s="3"/>
       <c r="C239" s="3"/>
     </row>
-    <row r="240" spans="1:3" ht="15.95" customHeight="1">
+    <row r="240" spans="1:3" ht="16" customHeight="1">
       <c r="A240" s="2"/>
       <c r="B240" s="3"/>
       <c r="C240" s="3"/>
     </row>
-    <row r="241" spans="1:3" ht="15.95" customHeight="1">
+    <row r="241" spans="1:3" ht="16" customHeight="1">
       <c r="A241" s="2"/>
       <c r="B241" s="3"/>
       <c r="C241" s="3"/>
     </row>
-    <row r="242" spans="1:3" ht="15.95" customHeight="1">
+    <row r="242" spans="1:3" ht="16" customHeight="1">
       <c r="A242" s="2"/>
       <c r="B242" s="3"/>
       <c r="C242" s="3"/>
     </row>
-    <row r="243" spans="1:3" ht="15.95" customHeight="1">
+    <row r="243" spans="1:3" ht="16" customHeight="1">
       <c r="A243" s="2"/>
       <c r="B243" s="3"/>
       <c r="C243" s="3"/>
     </row>
-    <row r="244" spans="1:3" ht="15.95" customHeight="1">
+    <row r="244" spans="1:3" ht="16" customHeight="1">
       <c r="A244" s="2"/>
       <c r="B244" s="3"/>
       <c r="C244" s="3"/>
     </row>
-    <row r="245" spans="1:3" ht="15.95" customHeight="1">
+    <row r="245" spans="1:3" ht="16" customHeight="1">
       <c r="A245" s="2"/>
       <c r="B245" s="3"/>
       <c r="C245" s="3"/>
     </row>
-    <row r="246" spans="1:3" ht="15.95" customHeight="1">
+    <row r="246" spans="1:3" ht="16" customHeight="1">
       <c r="A246" s="2"/>
       <c r="B246" s="3"/>
       <c r="C246" s="3"/>
     </row>
-    <row r="247" spans="1:3" ht="15.95" customHeight="1">
+    <row r="247" spans="1:3" ht="16" customHeight="1">
       <c r="A247" s="2"/>
       <c r="B247" s="3"/>
       <c r="C247" s="3"/>
     </row>
-    <row r="248" spans="1:3" ht="15.95" customHeight="1">
+    <row r="248" spans="1:3" ht="16" customHeight="1">
       <c r="A248" s="2"/>
       <c r="B248" s="3"/>
       <c r="C248" s="3"/>
     </row>
-    <row r="249" spans="1:3" ht="15.95" customHeight="1">
+    <row r="249" spans="1:3" ht="16" customHeight="1">
       <c r="A249" s="2"/>
       <c r="B249" s="3"/>
       <c r="C249" s="3"/>
     </row>
-    <row r="250" spans="1:3" ht="15.95" customHeight="1">
+    <row r="250" spans="1:3" ht="16" customHeight="1">
       <c r="A250" s="2"/>
       <c r="B250" s="3"/>
       <c r="C250" s="3"/>
     </row>
-    <row r="251" spans="1:3" ht="15.95" customHeight="1">
+    <row r="251" spans="1:3" ht="16" customHeight="1">
       <c r="A251" s="2"/>
       <c r="B251" s="3"/>
       <c r="C251" s="3"/>
     </row>
-    <row r="252" spans="1:3" ht="15.95" customHeight="1">
+    <row r="252" spans="1:3" ht="16" customHeight="1">
       <c r="A252" s="2"/>
       <c r="B252" s="3"/>
       <c r="C252" s="3"/>
     </row>
-    <row r="253" spans="1:3" ht="15.95" customHeight="1">
+    <row r="253" spans="1:3" ht="16" customHeight="1">
       <c r="A253" s="2"/>
       <c r="B253" s="3"/>
       <c r="C253" s="3"/>
     </row>
-    <row r="254" spans="1:3" ht="15.95" customHeight="1">
+    <row r="254" spans="1:3" ht="16" customHeight="1">
       <c r="A254" s="2"/>
       <c r="B254" s="3"/>
       <c r="C254" s="3"/>
     </row>
-    <row r="255" spans="1:3" ht="15.95" customHeight="1">
+    <row r="255" spans="1:3" ht="16" customHeight="1">
       <c r="A255" s="2"/>
       <c r="B255" s="3"/>
       <c r="C255" s="3"/>
     </row>
-    <row r="256" spans="1:3" ht="15.95" customHeight="1">
+    <row r="256" spans="1:3" ht="16" customHeight="1">
       <c r="A256" s="2"/>
       <c r="B256" s="3"/>
       <c r="C256" s="3"/>
     </row>
-    <row r="257" spans="1:3" ht="15.95" customHeight="1">
+    <row r="257" spans="1:3" ht="16" customHeight="1">
       <c r="A257" s="2"/>
       <c r="B257" s="3"/>
       <c r="C257" s="3"/>
     </row>
-    <row r="258" spans="1:3" ht="15.95" customHeight="1">
+    <row r="258" spans="1:3" ht="16" customHeight="1">
       <c r="A258" s="2"/>
       <c r="B258" s="3"/>
       <c r="C258" s="3"/>
     </row>
-    <row r="259" spans="1:3" ht="15.95" customHeight="1">
+    <row r="259" spans="1:3" ht="16" customHeight="1">
       <c r="A259" s="2"/>
       <c r="B259" s="3"/>
       <c r="C259" s="3"/>
     </row>
-    <row r="260" spans="1:3" ht="15.95" customHeight="1">
+    <row r="260" spans="1:3" ht="16" customHeight="1">
       <c r="A260" s="2"/>
       <c r="B260" s="3"/>
       <c r="C260" s="3"/>
     </row>
-    <row r="261" spans="1:3" ht="15.95" customHeight="1">
+    <row r="261" spans="1:3" ht="16" customHeight="1">
       <c r="A261" s="2"/>
       <c r="B261" s="3"/>
       <c r="C261" s="3"/>
     </row>
-    <row r="262" spans="1:3" ht="15.95" customHeight="1">
+    <row r="262" spans="1:3" ht="16" customHeight="1">
       <c r="A262" s="2"/>
       <c r="B262" s="3"/>
       <c r="C262" s="3"/>
     </row>
-    <row r="263" spans="1:3" ht="15.95" customHeight="1">
+    <row r="263" spans="1:3" ht="16" customHeight="1">
       <c r="A263" s="2"/>
       <c r="B263" s="3"/>
       <c r="C263" s="3"/>
     </row>
-    <row r="264" spans="1:3" ht="15.95" customHeight="1">
+    <row r="264" spans="1:3" ht="16" customHeight="1">
       <c r="A264" s="2"/>
       <c r="B264" s="3"/>
       <c r="C264" s="3"/>
     </row>
-    <row r="265" spans="1:3" ht="15.95" customHeight="1">
+    <row r="265" spans="1:3" ht="16" customHeight="1">
       <c r="A265" s="2"/>
       <c r="B265" s="3"/>
       <c r="C265" s="3"/>
     </row>
-    <row r="266" spans="1:3" ht="15.95" customHeight="1">
+    <row r="266" spans="1:3" ht="16" customHeight="1">
       <c r="A266" s="2"/>
       <c r="B266" s="3"/>
       <c r="C266" s="3"/>
     </row>
-    <row r="267" spans="1:3" ht="15.95" customHeight="1">
+    <row r="267" spans="1:3" ht="16" customHeight="1">
       <c r="A267" s="2"/>
       <c r="B267" s="3"/>
       <c r="C267" s="3"/>
     </row>
-    <row r="268" spans="1:3" ht="15.95" customHeight="1">
+    <row r="268" spans="1:3" ht="16" customHeight="1">
       <c r="A268" s="2"/>
       <c r="B268" s="3"/>
       <c r="C268" s="3"/>
     </row>
-    <row r="269" spans="1:3" ht="15.95" customHeight="1">
+    <row r="269" spans="1:3" ht="16" customHeight="1">
       <c r="A269" s="2"/>
       <c r="B269" s="3"/>
       <c r="C269" s="3"/>
     </row>
-    <row r="270" spans="1:3" ht="15.95" customHeight="1">
+    <row r="270" spans="1:3" ht="16" customHeight="1">
       <c r="A270" s="2"/>
       <c r="B270" s="3"/>
       <c r="C270" s="3"/>
     </row>
-    <row r="271" spans="1:3" ht="15.95" customHeight="1">
+    <row r="271" spans="1:3" ht="16" customHeight="1">
       <c r="A271" s="2"/>
       <c r="B271" s="3"/>
       <c r="C271" s="3"/>
     </row>
-    <row r="272" spans="1:3" ht="15.95" customHeight="1">
+    <row r="272" spans="1:3" ht="16" customHeight="1">
       <c r="A272" s="2"/>
       <c r="B272" s="3"/>
       <c r="C272" s="3"/>
     </row>
-    <row r="273" spans="1:3" ht="15.95" customHeight="1">
+    <row r="273" spans="1:3" ht="16" customHeight="1">
       <c r="A273" s="2"/>
       <c r="B273" s="3"/>
       <c r="C273" s="3"/>
     </row>
-    <row r="274" spans="1:3" ht="15.95" customHeight="1">
+    <row r="274" spans="1:3" ht="16" customHeight="1">
       <c r="A274" s="2"/>
       <c r="B274" s="3"/>
       <c r="C274" s="3"/>
     </row>
-    <row r="275" spans="1:3" ht="15.95" customHeight="1">
+    <row r="275" spans="1:3" ht="16" customHeight="1">
       <c r="A275" s="2"/>
       <c r="B275" s="3"/>
       <c r="C275" s="3"/>
     </row>
-    <row r="276" spans="1:3" ht="15.95" customHeight="1">
+    <row r="276" spans="1:3" ht="16" customHeight="1">
       <c r="A276" s="2"/>
       <c r="B276" s="3"/>
       <c r="C276" s="3"/>
     </row>
-    <row r="277" spans="1:3" ht="15.95" customHeight="1">
+    <row r="277" spans="1:3" ht="16" customHeight="1">
       <c r="A277" s="2"/>
       <c r="B277" s="3"/>
       <c r="C277" s="3"/>
     </row>
-    <row r="278" spans="1:3" ht="15.95" customHeight="1">
+    <row r="278" spans="1:3" ht="16" customHeight="1">
       <c r="A278" s="2"/>
       <c r="B278" s="3"/>
       <c r="C278" s="3"/>
     </row>
-    <row r="279" spans="1:3" ht="15.95" customHeight="1">
+    <row r="279" spans="1:3" ht="16" customHeight="1">
       <c r="A279" s="2"/>
       <c r="B279" s="3"/>
       <c r="C279" s="3"/>
     </row>
-    <row r="280" spans="1:3" ht="15.95" customHeight="1">
+    <row r="280" spans="1:3" ht="16" customHeight="1">
       <c r="A280" s="2"/>
       <c r="B280" s="3"/>
       <c r="C280" s="3"/>
     </row>
-    <row r="281" spans="1:3" ht="15.95" customHeight="1">
+    <row r="281" spans="1:3" ht="16" customHeight="1">
       <c r="A281" s="2"/>
       <c r="B281" s="3"/>
       <c r="C281" s="3"/>
     </row>
-    <row r="282" spans="1:3" ht="15.95" customHeight="1">
+    <row r="282" spans="1:3" ht="16" customHeight="1">
       <c r="A282" s="2"/>
       <c r="B282" s="3"/>
       <c r="C282" s="3"/>
     </row>
-    <row r="283" spans="1:3" ht="15.95" customHeight="1">
+    <row r="283" spans="1:3" ht="16" customHeight="1">
       <c r="A283" s="2"/>
       <c r="B283" s="3"/>
       <c r="C283" s="3"/>
     </row>
-    <row r="284" spans="1:3" ht="15.95" customHeight="1">
+    <row r="284" spans="1:3" ht="16" customHeight="1">
       <c r="A284" s="2"/>
       <c r="B284" s="3"/>
       <c r="C284" s="3"/>
     </row>
-    <row r="285" spans="1:3" ht="15.95" customHeight="1">
+    <row r="285" spans="1:3" ht="16" customHeight="1">
       <c r="A285" s="2"/>
       <c r="B285" s="3"/>
       <c r="C285" s="3"/>
     </row>
-    <row r="286" spans="1:3" ht="15.95" customHeight="1">
+    <row r="286" spans="1:3" ht="16" customHeight="1">
       <c r="A286" s="2"/>
       <c r="B286" s="3"/>
       <c r="C286" s="3"/>
     </row>
-    <row r="287" spans="1:3" ht="15.95" customHeight="1">
+    <row r="287" spans="1:3" ht="16" customHeight="1">
       <c r="A287" s="2"/>
       <c r="B287" s="3"/>
       <c r="C287" s="3"/>
     </row>
-    <row r="288" spans="1:3" ht="15.95" customHeight="1">
+    <row r="288" spans="1:3" ht="16" customHeight="1">
       <c r="A288" s="2"/>
       <c r="B288" s="3"/>
       <c r="C288" s="3"/>
     </row>
-    <row r="289" spans="1:3" ht="15.95" customHeight="1">
+    <row r="289" spans="1:3" ht="16" customHeight="1">
       <c r="A289" s="2"/>
       <c r="B289" s="3"/>
       <c r="C289" s="3"/>
     </row>
-    <row r="290" spans="1:3" ht="15.95" customHeight="1">
+    <row r="290" spans="1:3" ht="16" customHeight="1">
       <c r="A290" s="2"/>
       <c r="B290" s="3"/>
       <c r="C290" s="3"/>
     </row>
-    <row r="291" spans="1:3" ht="15.95" customHeight="1">
+    <row r="291" spans="1:3" ht="16" customHeight="1">
       <c r="A291" s="2"/>
       <c r="B291" s="3"/>
       <c r="C291" s="3"/>
     </row>
-    <row r="292" spans="1:3" ht="15.95" customHeight="1">
+    <row r="292" spans="1:3" ht="16" customHeight="1">
       <c r="A292" s="2"/>
       <c r="B292" s="3"/>
       <c r="C292" s="3"/>
     </row>
-    <row r="293" spans="1:3" ht="15.95" customHeight="1">
+    <row r="293" spans="1:3" ht="16" customHeight="1">
       <c r="A293" s="2"/>
       <c r="B293" s="3"/>
       <c r="C293" s="3"/>
     </row>
-    <row r="294" spans="1:3" ht="15.95" customHeight="1">
+    <row r="294" spans="1:3" ht="16" customHeight="1">
       <c r="A294" s="2"/>
       <c r="B294" s="3"/>
       <c r="C294" s="3"/>
     </row>
-    <row r="295" spans="1:3" ht="15.95" customHeight="1">
+    <row r="295" spans="1:3" ht="16" customHeight="1">
       <c r="A295" s="2"/>
       <c r="B295" s="3"/>
       <c r="C295" s="3"/>
     </row>
-    <row r="296" spans="1:3" ht="15.95" customHeight="1">
+    <row r="296" spans="1:3" ht="16" customHeight="1">
       <c r="A296" s="2"/>
       <c r="B296" s="3"/>
       <c r="C296" s="3"/>
     </row>
-    <row r="297" spans="1:3" ht="15.95" customHeight="1">
+    <row r="297" spans="1:3" ht="16" customHeight="1">
       <c r="A297" s="2"/>
       <c r="B297" s="3"/>
       <c r="C297" s="3"/>
     </row>
-    <row r="298" spans="1:3" ht="15.95" customHeight="1">
+    <row r="298" spans="1:3" ht="16" customHeight="1">
       <c r="A298" s="2"/>
       <c r="B298" s="3"/>
       <c r="C298" s="3"/>
     </row>
-    <row r="299" spans="1:3" ht="15.95" customHeight="1">
+    <row r="299" spans="1:3" ht="16" customHeight="1">
       <c r="A299" s="2"/>
       <c r="B299" s="3"/>
       <c r="C299" s="3"/>
     </row>
-    <row r="300" spans="1:3" ht="15.95" customHeight="1">
+    <row r="300" spans="1:3" ht="16" customHeight="1">
       <c r="A300" s="2"/>
       <c r="B300" s="3"/>
       <c r="C300" s="3"/>
     </row>
-    <row r="301" spans="1:3" ht="15.95" customHeight="1">
+    <row r="301" spans="1:3" ht="16" customHeight="1">
       <c r="A301" s="2"/>
       <c r="B301" s="3"/>
       <c r="C301" s="3"/>
     </row>
-    <row r="302" spans="1:3" ht="15.95" customHeight="1">
+    <row r="302" spans="1:3" ht="16" customHeight="1">
       <c r="A302" s="2"/>
       <c r="B302" s="3"/>
       <c r="C302" s="3"/>
     </row>
-    <row r="303" spans="1:3" ht="15.95" customHeight="1">
+    <row r="303" spans="1:3" ht="16" customHeight="1">
       <c r="A303" s="2"/>
       <c r="B303" s="3"/>
       <c r="C303" s="3"/>
     </row>
-    <row r="304" spans="1:3" ht="15.95" customHeight="1">
+    <row r="304" spans="1:3" ht="16" customHeight="1">
       <c r="A304" s="2"/>
       <c r="B304" s="3"/>
       <c r="C304" s="3"/>
     </row>
-    <row r="305" spans="1:3" ht="15.95" customHeight="1">
+    <row r="305" spans="1:3" ht="16" customHeight="1">
       <c r="A305" s="2"/>
       <c r="B305" s="3"/>
       <c r="C305" s="3"/>
     </row>
-    <row r="306" spans="1:3" ht="15.95" customHeight="1">
+    <row r="306" spans="1:3" ht="16" customHeight="1">
       <c r="A306" s="2"/>
       <c r="B306" s="3"/>
       <c r="C306" s="3"/>
     </row>
-    <row r="307" spans="1:3" ht="15.95" customHeight="1">
+    <row r="307" spans="1:3" ht="16" customHeight="1">
       <c r="A307" s="2"/>
       <c r="B307" s="3"/>
       <c r="C307" s="3"/>
     </row>
-    <row r="308" spans="1:3" ht="15.95" customHeight="1">
+    <row r="308" spans="1:3" ht="16" customHeight="1">
       <c r="A308" s="2"/>
       <c r="B308" s="3"/>
       <c r="C308" s="3"/>
     </row>
-    <row r="309" spans="1:3" ht="15.95" customHeight="1">
+    <row r="309" spans="1:3" ht="16" customHeight="1">
       <c r="A309" s="2"/>
       <c r="B309" s="3"/>
       <c r="C309" s="3"/>
     </row>
-    <row r="310" spans="1:3" ht="15.95" customHeight="1">
+    <row r="310" spans="1:3" ht="16" customHeight="1">
       <c r="A310" s="2"/>
       <c r="B310" s="3"/>
       <c r="C310" s="3"/>
     </row>
-    <row r="311" spans="1:3" ht="15.95" customHeight="1">
+    <row r="311" spans="1:3" ht="16" customHeight="1">
       <c r="A311" s="2"/>
       <c r="B311" s="3"/>
       <c r="C311" s="3"/>
     </row>
-    <row r="312" spans="1:3" ht="15.95" customHeight="1">
+    <row r="312" spans="1:3" ht="16" customHeight="1">
       <c r="A312" s="2"/>
       <c r="B312" s="3"/>
       <c r="C312" s="3"/>
     </row>
-    <row r="313" spans="1:3" ht="15.95" customHeight="1">
+    <row r="313" spans="1:3" ht="16" customHeight="1">
       <c r="A313" s="2"/>
       <c r="B313" s="3"/>
       <c r="C313" s="3"/>
     </row>
-    <row r="314" spans="1:3" ht="15.95" customHeight="1">
+    <row r="314" spans="1:3" ht="16" customHeight="1">
       <c r="A314" s="2"/>
       <c r="B314" s="3"/>
       <c r="C314" s="3"/>
     </row>
-    <row r="315" spans="1:3" ht="15.95" customHeight="1">
+    <row r="315" spans="1:3" ht="16" customHeight="1">
       <c r="A315" s="2"/>
       <c r="B315" s="3"/>
       <c r="C315" s="3"/>
     </row>
-    <row r="316" spans="1:3" ht="15.95" customHeight="1">
+    <row r="316" spans="1:3" ht="16" customHeight="1">
       <c r="A316" s="2"/>
       <c r="B316" s="3"/>
       <c r="C316" s="3"/>
     </row>
-    <row r="317" spans="1:3" ht="15.95" customHeight="1">
+    <row r="317" spans="1:3" ht="16" customHeight="1">
       <c r="A317" s="2"/>
       <c r="B317" s="3"/>
       <c r="C317" s="3"/>
     </row>
-    <row r="318" spans="1:3" ht="15.95" customHeight="1">
+    <row r="318" spans="1:3" ht="16" customHeight="1">
       <c r="A318" s="2"/>
       <c r="B318" s="3"/>
       <c r="C318" s="3"/>
     </row>
-    <row r="319" spans="1:3" ht="15.95" customHeight="1">
+    <row r="319" spans="1:3" ht="16" customHeight="1">
       <c r="A319" s="2"/>
       <c r="B319" s="3"/>
       <c r="C319" s="3"/>
     </row>
-    <row r="320" spans="1:3" ht="15.95" customHeight="1">
+    <row r="320" spans="1:3" ht="16" customHeight="1">
       <c r="A320" s="2"/>
       <c r="B320" s="3"/>
       <c r="C320" s="3"/>
     </row>
-    <row r="321" spans="1:3" ht="15.95" customHeight="1">
+    <row r="321" spans="1:3" ht="16" customHeight="1">
       <c r="A321" s="2"/>
       <c r="B321" s="3"/>
       <c r="C321" s="3"/>
     </row>
-    <row r="322" spans="1:3" ht="15.95" customHeight="1">
+    <row r="322" spans="1:3" ht="16" customHeight="1">
       <c r="A322" s="2"/>
       <c r="B322" s="3"/>
       <c r="C322" s="3"/>
     </row>
-    <row r="323" spans="1:3" ht="15.95" customHeight="1">
+    <row r="323" spans="1:3" ht="16" customHeight="1">
       <c r="A323" s="2"/>
       <c r="B323" s="3"/>
       <c r="C323" s="3"/>
     </row>
-    <row r="324" spans="1:3" ht="15.95" customHeight="1">
+    <row r="324" spans="1:3" ht="16" customHeight="1">
       <c r="A324" s="2"/>
       <c r="B324" s="3"/>
       <c r="C324" s="3"/>
     </row>
-    <row r="325" spans="1:3" ht="15.95" customHeight="1">
+    <row r="325" spans="1:3" ht="16" customHeight="1">
       <c r="A325" s="2"/>
       <c r="B325" s="3"/>
       <c r="C325" s="3"/>
     </row>
-    <row r="326" spans="1:3" ht="15.95" customHeight="1">
+    <row r="326" spans="1:3" ht="16" customHeight="1">
       <c r="A326" s="2"/>
       <c r="B326" s="3"/>
       <c r="C326" s="3"/>
     </row>
-    <row r="327" spans="1:3" ht="15.95" customHeight="1">
+    <row r="327" spans="1:3" ht="16" customHeight="1">
       <c r="A327" s="2"/>
       <c r="B327" s="3"/>
       <c r="C327" s="3"/>
     </row>
-    <row r="328" spans="1:3" ht="15.95" customHeight="1">
+    <row r="328" spans="1:3" ht="16" customHeight="1">
       <c r="A328" s="2"/>
       <c r="B328" s="3"/>
       <c r="C328" s="3"/>
     </row>
-    <row r="329" spans="1:3" ht="15.95" customHeight="1">
+    <row r="329" spans="1:3" ht="16" customHeight="1">
       <c r="A329" s="2"/>
       <c r="B329" s="3"/>
       <c r="C329" s="3"/>
     </row>
-    <row r="330" spans="1:3" ht="15.95" customHeight="1">
+    <row r="330" spans="1:3" ht="16" customHeight="1">
       <c r="A330" s="2"/>
       <c r="B330" s="3"/>
       <c r="C330" s="3"/>
     </row>
-    <row r="331" spans="1:3" ht="15.95" customHeight="1">
+    <row r="331" spans="1:3" ht="16" customHeight="1">
       <c r="A331" s="2"/>
       <c r="B331" s="3"/>
       <c r="C331" s="3"/>
     </row>
-    <row r="332" spans="1:3" ht="15.95" customHeight="1">
+    <row r="332" spans="1:3" ht="16" customHeight="1">
       <c r="A332" s="2"/>
       <c r="B332" s="3"/>
       <c r="C332" s="3"/>
     </row>
-    <row r="333" spans="1:3" ht="15.95" customHeight="1">
+    <row r="333" spans="1:3" ht="16" customHeight="1">
       <c r="A333" s="2"/>
       <c r="B333" s="3"/>
       <c r="C333" s="3"/>
     </row>
-    <row r="334" spans="1:3" ht="15.95" customHeight="1">
+    <row r="334" spans="1:3" ht="16" customHeight="1">
       <c r="A334" s="2"/>
       <c r="B334" s="3"/>
       <c r="C334" s="3"/>
     </row>
-    <row r="335" spans="1:3" ht="15.95" customHeight="1">
+    <row r="335" spans="1:3" ht="16" customHeight="1">
       <c r="A335" s="2"/>
       <c r="B335" s="3"/>
       <c r="C335" s="3"/>
     </row>
-    <row r="336" spans="1:3" ht="15.95" customHeight="1">
+    <row r="336" spans="1:3" ht="16" customHeight="1">
       <c r="A336" s="2"/>
       <c r="B336" s="3"/>
       <c r="C336" s="3"/>
     </row>
-    <row r="337" spans="1:3" ht="15.95" customHeight="1">
+    <row r="337" spans="1:3" ht="16" customHeight="1">
       <c r="A337" s="2"/>
       <c r="B337" s="3"/>
       <c r="C337" s="3"/>
     </row>
-    <row r="338" spans="1:3" ht="15.95" customHeight="1">
+    <row r="338" spans="1:3" ht="16" customHeight="1">
       <c r="A338" s="2"/>
       <c r="B338" s="3"/>
       <c r="C338" s="3"/>
     </row>
-    <row r="339" spans="1:3" ht="15.95" customHeight="1">
+    <row r="339" spans="1:3" ht="16" customHeight="1">
       <c r="A339" s="2"/>
       <c r="B339" s="3"/>
       <c r="C339" s="3"/>
     </row>
-    <row r="340" spans="1:3" ht="15.95" customHeight="1">
+    <row r="340" spans="1:3" ht="16" customHeight="1">
       <c r="A340" s="2"/>
       <c r="B340" s="3"/>
       <c r="C340" s="3"/>
     </row>
-    <row r="341" spans="1:3" ht="15.95" customHeight="1">
+    <row r="341" spans="1:3" ht="16" customHeight="1">
       <c r="A341" s="2"/>
       <c r="B341" s="3"/>
       <c r="C341" s="3"/>
     </row>
-    <row r="342" spans="1:3" ht="15.95" customHeight="1">
+    <row r="342" spans="1:3" ht="16" customHeight="1">
       <c r="A342" s="2"/>
       <c r="B342" s="3"/>
       <c r="C342" s="3"/>
     </row>
-    <row r="343" spans="1:3" ht="15.95" customHeight="1">
+    <row r="343" spans="1:3" ht="16" customHeight="1">
       <c r="A343" s="2"/>
       <c r="B343" s="3"/>
       <c r="C343" s="3"/>
     </row>
-    <row r="344" spans="1:3" ht="15.95" customHeight="1">
+    <row r="344" spans="1:3" ht="16" customHeight="1">
       <c r="A344" s="2"/>
       <c r="B344" s="3"/>
       <c r="C344" s="3"/>
     </row>
-    <row r="345" spans="1:3" ht="15.95" customHeight="1">
+    <row r="345" spans="1:3" ht="16" customHeight="1">
       <c r="A345" s="2"/>
       <c r="B345" s="3"/>
       <c r="C345" s="3"/>
     </row>
-    <row r="346" spans="1:3" ht="15.95" customHeight="1">
+    <row r="346" spans="1:3" ht="16" customHeight="1">
       <c r="A346" s="2"/>
       <c r="B346" s="3"/>
       <c r="C346" s="3"/>
     </row>
-    <row r="347" spans="1:3" ht="15.95" customHeight="1">
+    <row r="347" spans="1:3" ht="16" customHeight="1">
       <c r="A347" s="2"/>
       <c r="B347" s="3"/>
       <c r="C347" s="3"/>
     </row>
-    <row r="348" spans="1:3" ht="15.95" customHeight="1">
+    <row r="348" spans="1:3" ht="16" customHeight="1">
       <c r="A348" s="2"/>
       <c r="B348" s="3"/>
       <c r="C348" s="3"/>
     </row>
-    <row r="349" spans="1:3" ht="15.95" customHeight="1">
+    <row r="349" spans="1:3" ht="16" customHeight="1">
       <c r="A349" s="2"/>
       <c r="B349" s="3"/>
       <c r="C349" s="3"/>
     </row>
-    <row r="350" spans="1:3" ht="15.95" customHeight="1">
+    <row r="350" spans="1:3" ht="16" customHeight="1">
       <c r="A350" s="2"/>
       <c r="B350" s="3"/>
       <c r="C350" s="3"/>
     </row>
-    <row r="351" spans="1:3" ht="15.95" customHeight="1">
+    <row r="351" spans="1:3" ht="16" customHeight="1">
       <c r="A351" s="2"/>
       <c r="B351" s="3"/>
       <c r="C351" s="3"/>
     </row>
-    <row r="352" spans="1:3" ht="14.1" customHeight="1">
+    <row r="352" spans="1:3" ht="14" customHeight="1">
       <c r="A352" s="4"/>
     </row>
   </sheetData>
   <printOptions verticalCentered="1" gridLines="1"/>
   <pageMargins left="0.08" right="0.08" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" blackAndWhite="1" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup orientation="portrait" blackAndWhite="1" horizontalDpi="300" verticalDpi="300"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -3131,35 +3147,35 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="18.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="31.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="38.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="18.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="12.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="31.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="38.5" style="1" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="30" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="27.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="28.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="18" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="22.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="16384" width="8.85546875" style="1"/>
+    <col min="15" max="15" width="27.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="28.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="18" width="11.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="22.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="14.1" customHeight="1">
+    <row r="1" spans="1:19" ht="14" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>53</v>
       </c>
@@ -3218,7 +3234,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:19" ht="15.95" customHeight="1">
+    <row r="2" spans="1:19" ht="16" customHeight="1">
       <c r="A2" s="2">
         <v>1000121</v>
       </c>
@@ -3277,7 +3293,7 @@
         <v>854.88</v>
       </c>
     </row>
-    <row r="3" spans="1:19" ht="15.95" customHeight="1">
+    <row r="3" spans="1:19" ht="16" customHeight="1">
       <c r="A3" s="2">
         <v>1000122</v>
       </c>
@@ -3336,7 +3352,7 @@
         <v>4346.07</v>
       </c>
     </row>
-    <row r="4" spans="1:19" ht="15.95" customHeight="1">
+    <row r="4" spans="1:19" ht="16" customHeight="1">
       <c r="A4" s="2">
         <v>1000123</v>
       </c>
@@ -3395,7 +3411,7 @@
         <v>15355.88</v>
       </c>
     </row>
-    <row r="5" spans="1:19" ht="15.95" customHeight="1">
+    <row r="5" spans="1:19" ht="16" customHeight="1">
       <c r="A5" s="2">
         <v>1000124</v>
       </c>
@@ -3454,7 +3470,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:19" ht="15.95" customHeight="1">
+    <row r="6" spans="1:19" ht="16" customHeight="1">
       <c r="A6" s="2">
         <v>1000125</v>
       </c>
@@ -3513,7 +3529,7 @@
         <v>182.58</v>
       </c>
     </row>
-    <row r="7" spans="1:19" ht="15.95" customHeight="1">
+    <row r="7" spans="1:19" ht="16" customHeight="1">
       <c r="A7" s="2">
         <v>1000126</v>
       </c>
@@ -3572,7 +3588,7 @@
         <v>405.46</v>
       </c>
     </row>
-    <row r="8" spans="1:19" ht="15.95" customHeight="1">
+    <row r="8" spans="1:19" ht="16" customHeight="1">
       <c r="A8" s="2">
         <v>1000127</v>
       </c>
@@ -3631,7 +3647,7 @@
         <v>935.81</v>
       </c>
     </row>
-    <row r="9" spans="1:19" ht="15.95" customHeight="1">
+    <row r="9" spans="1:19" ht="16" customHeight="1">
       <c r="A9" s="2">
         <v>1000128</v>
       </c>
@@ -3690,7 +3706,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:19" ht="15.95" customHeight="1">
+    <row r="10" spans="1:19" ht="16" customHeight="1">
       <c r="A10" s="2">
         <v>1000129</v>
       </c>
@@ -3749,7 +3765,7 @@
         <v>163.47999999999999</v>
       </c>
     </row>
-    <row r="11" spans="1:19" ht="15.95" customHeight="1">
+    <row r="11" spans="1:19" ht="16" customHeight="1">
       <c r="A11" s="2">
         <v>1000130</v>
       </c>
@@ -3808,7 +3824,7 @@
         <v>924.71</v>
       </c>
     </row>
-    <row r="12" spans="1:19" ht="15.95" customHeight="1">
+    <row r="12" spans="1:19" ht="16" customHeight="1">
       <c r="A12" s="2">
         <v>1000131</v>
       </c>
@@ -3867,7 +3883,7 @@
         <v>794.82</v>
       </c>
     </row>
-    <row r="13" spans="1:19" ht="15.95" customHeight="1">
+    <row r="13" spans="1:19" ht="16" customHeight="1">
       <c r="A13" s="2">
         <v>1000132</v>
       </c>
@@ -3926,7 +3942,7 @@
         <v>41.74</v>
       </c>
     </row>
-    <row r="14" spans="1:19" ht="15.95" customHeight="1">
+    <row r="14" spans="1:19" ht="16" customHeight="1">
       <c r="A14" s="2">
         <v>1000133</v>
       </c>
@@ -3985,7 +4001,7 @@
         <v>196.24</v>
       </c>
     </row>
-    <row r="15" spans="1:19" ht="15.95" customHeight="1">
+    <row r="15" spans="1:19" ht="16" customHeight="1">
       <c r="A15" s="2">
         <v>1000134</v>
       </c>
@@ -4044,7 +4060,7 @@
         <v>65.25</v>
       </c>
     </row>
-    <row r="16" spans="1:19" ht="15.95" customHeight="1">
+    <row r="16" spans="1:19" ht="16" customHeight="1">
       <c r="A16" s="2">
         <v>1000135</v>
       </c>
@@ -4103,7 +4119,7 @@
         <v>128.57</v>
       </c>
     </row>
-    <row r="17" spans="1:19" ht="15.95" customHeight="1">
+    <row r="17" spans="1:19" ht="16" customHeight="1">
       <c r="A17" s="2">
         <v>1000136</v>
       </c>
@@ -4162,7 +4178,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:19" ht="15.95" customHeight="1">
+    <row r="18" spans="1:19" ht="16" customHeight="1">
       <c r="A18" s="2">
         <v>1000137</v>
       </c>
@@ -4221,7 +4237,7 @@
         <v>121.37</v>
       </c>
     </row>
-    <row r="19" spans="1:19" ht="15.95" customHeight="1">
+    <row r="19" spans="1:19" ht="16" customHeight="1">
       <c r="A19" s="2">
         <v>1000138</v>
       </c>
@@ -4280,7 +4296,7 @@
         <v>47.19</v>
       </c>
     </row>
-    <row r="20" spans="1:19" ht="15.95" customHeight="1">
+    <row r="20" spans="1:19" ht="16" customHeight="1">
       <c r="A20" s="2">
         <v>1000139</v>
       </c>
@@ -4352,27 +4368,27 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.28515625" style="1" customWidth="1"/>
-    <col min="3" max="4" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.85546875" style="1"/>
+    <col min="1" max="1" width="14.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.33203125" style="1" customWidth="1"/>
+    <col min="3" max="4" width="11.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="14.1" customHeight="1">
+    <row r="1" spans="1:4" ht="14" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>53</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C1" s="5" t="s">
         <v>54</v>
@@ -4381,7 +4397,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15.95" customHeight="1">
+    <row r="2" spans="1:4" ht="16" customHeight="1">
       <c r="A2" s="2">
         <v>1000121</v>
       </c>
@@ -4395,7 +4411,7 @@
         <v>26.8</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15.95" customHeight="1">
+    <row r="3" spans="1:4" ht="16" customHeight="1">
       <c r="A3" s="2">
         <v>1000122</v>
       </c>
@@ -4409,7 +4425,7 @@
         <v>32.4</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15.95" customHeight="1">
+    <row r="4" spans="1:4" ht="16" customHeight="1">
       <c r="A4" s="2">
         <v>1000123</v>
       </c>
@@ -4423,7 +4439,7 @@
         <v>33.4</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="15.95" customHeight="1">
+    <row r="5" spans="1:4" ht="16" customHeight="1">
       <c r="A5" s="2">
         <v>1000124</v>
       </c>
@@ -4437,7 +4453,7 @@
         <v>29.7</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="15.95" customHeight="1">
+    <row r="6" spans="1:4" ht="16" customHeight="1">
       <c r="A6" s="2">
         <v>1000125</v>
       </c>
@@ -4451,7 +4467,7 @@
         <v>22.7</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="15.95" customHeight="1">
+    <row r="7" spans="1:4" ht="16" customHeight="1">
       <c r="A7" s="2">
         <v>1000126</v>
       </c>
@@ -4465,7 +4481,7 @@
         <v>26.4</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="15.95" customHeight="1">
+    <row r="8" spans="1:4" ht="16" customHeight="1">
       <c r="A8" s="2">
         <v>1000127</v>
       </c>
@@ -4479,7 +4495,7 @@
         <v>24.9</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="15.95" customHeight="1">
+    <row r="9" spans="1:4" ht="16" customHeight="1">
       <c r="A9" s="2">
         <v>1000128</v>
       </c>
@@ -4493,7 +4509,7 @@
         <v>22.4</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="15.95" customHeight="1">
+    <row r="10" spans="1:4" ht="16" customHeight="1">
       <c r="A10" s="2">
         <v>1000129</v>
       </c>
@@ -4507,7 +4523,7 @@
         <v>28.6</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="15.95" customHeight="1">
+    <row r="11" spans="1:4" ht="16" customHeight="1">
       <c r="A11" s="2">
         <v>1000130</v>
       </c>
@@ -4521,7 +4537,7 @@
         <v>21.4</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="15.95" customHeight="1">
+    <row r="12" spans="1:4" ht="16" customHeight="1">
       <c r="A12" s="2">
         <v>1000131</v>
       </c>
@@ -4535,7 +4551,7 @@
         <v>20.7</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="15.95" customHeight="1">
+    <row r="13" spans="1:4" ht="16" customHeight="1">
       <c r="A13" s="2">
         <v>1000132</v>
       </c>
@@ -4549,7 +4565,7 @@
         <v>29.4</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="15.95" customHeight="1">
+    <row r="14" spans="1:4" ht="16" customHeight="1">
       <c r="A14" s="2">
         <v>1000133</v>
       </c>
@@ -4563,7 +4579,7 @@
         <v>28.7</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="15.95" customHeight="1">
+    <row r="15" spans="1:4" ht="16" customHeight="1">
       <c r="A15" s="2">
         <v>1000134</v>
       </c>
@@ -4577,7 +4593,7 @@
         <v>26.8</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="15.95" customHeight="1">
+    <row r="16" spans="1:4" ht="16" customHeight="1">
       <c r="A16" s="2">
         <v>1000135</v>
       </c>
@@ -4591,7 +4607,7 @@
         <v>27.3</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="15.95" customHeight="1">
+    <row r="17" spans="1:4" ht="16" customHeight="1">
       <c r="A17" s="2">
         <v>1000136</v>
       </c>
@@ -4605,7 +4621,7 @@
         <v>22.4</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="15.95" customHeight="1">
+    <row r="18" spans="1:4" ht="16" customHeight="1">
       <c r="A18" s="2">
         <v>1000137</v>
       </c>
@@ -4619,7 +4635,7 @@
         <v>21.6</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="15.95" customHeight="1">
+    <row r="19" spans="1:4" ht="16" customHeight="1">
       <c r="A19" s="2">
         <v>1000138</v>
       </c>
@@ -4633,7 +4649,7 @@
         <v>23.4</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="15.95" customHeight="1">
+    <row r="20" spans="1:4" ht="16" customHeight="1">
       <c r="A20" s="2">
         <v>1000139</v>
       </c>
@@ -4660,22 +4676,22 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="39.85546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="43.42578125" style="1" customWidth="1"/>
-    <col min="3" max="4" width="57.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.85546875" style="1"/>
+    <col min="1" max="1" width="26.1640625" customWidth="1"/>
+    <col min="2" max="2" width="51.1640625" customWidth="1"/>
+    <col min="3" max="3" width="28.6640625" customWidth="1"/>
+    <col min="4" max="4" width="52.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="14.1" customHeight="1">
+    <row r="1" spans="1:4">
       <c r="A1" s="2" t="s">
         <v>56</v>
       </c>
@@ -4689,7 +4705,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15.95" customHeight="1">
+    <row r="2" spans="1:4">
       <c r="A2" s="2" t="s">
         <v>60</v>
       </c>
@@ -4703,7 +4719,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15.95" customHeight="1">
+    <row r="3" spans="1:4">
       <c r="A3" s="2" t="s">
         <v>63</v>
       </c>
@@ -4717,7 +4733,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15.95" customHeight="1">
+    <row r="4" spans="1:4">
       <c r="A4" s="2" t="s">
         <v>66</v>
       </c>
@@ -4731,7 +4747,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="15.95" customHeight="1">
+    <row r="5" spans="1:4">
       <c r="A5" s="2" t="s">
         <v>70</v>
       </c>
@@ -4739,17 +4755,22 @@
         <v>69</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>80</v>
+        <v>79</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>85</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection password="AAAF" sheet="1" objects="1" scenarios="1"/>
-  <printOptions verticalCentered="1" gridLines="1"/>
-  <pageMargins left="0.08" right="0.08" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" blackAndWhite="1" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -4759,57 +4780,55 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B15" sqref="A14:B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="4" width="42.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="36.28515625" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.85546875" style="1"/>
+    <col min="1" max="4" width="42.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="36.33203125" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="14.1" customHeight="1">
+    <row r="1" spans="1:5" ht="14" customHeight="1">
       <c r="A1" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="8" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="16" customHeight="1">
+      <c r="A2" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="E1" s="8" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="15.95" customHeight="1">
-      <c r="A2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>76</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>77</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="15.95" customHeight="1">
+      <c r="D2" s="3"/>
+    </row>
+    <row r="3" spans="1:5" ht="16" customHeight="1">
       <c r="A3" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>63</v>
@@ -4818,7 +4837,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="14.1" customHeight="1">
+    <row r="4" spans="1:5" ht="14" customHeight="1">
       <c r="A4" s="4"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated the input files to reflect the decision to fix the metabolte id and subjectid rows in varmap. Unable to test in comets-analytics because calls are incorrect to corr
</commit_message>
<xml_diff>
--- a/inst/extdata/cometsInputAge.xlsx
+++ b/inst/extdata/cometsInputAge.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="27729"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1320" yWindow="640" windowWidth="25200" windowHeight="14760" activeTab="4"/>
+    <workbookView xWindow="1320" yWindow="645" windowWidth="24240" windowHeight="13740" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Metabolites" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="88">
   <si>
     <t>METABOLITE_NAME</t>
   </si>
@@ -211,27 +211,12 @@
     <t>cohort subject id</t>
   </si>
   <si>
-    <t>Sample Identifier</t>
-  </si>
-  <si>
     <t>age</t>
   </si>
   <si>
-    <t>Age at Entry</t>
-  </si>
-  <si>
-    <t>measured during year 1</t>
-  </si>
-  <si>
     <t>bmi</t>
   </si>
   <si>
-    <t>BMI at Baseline (In kg/m2)</t>
-  </si>
-  <si>
-    <t>measured at baseline</t>
-  </si>
-  <si>
     <t>metabolite identifier / variable name</t>
   </si>
   <si>
@@ -262,9 +247,6 @@
     <t>METABID</t>
   </si>
   <si>
-    <t>column header in metabolites sheet</t>
-  </si>
-  <si>
     <t>RT</t>
   </si>
   <si>
@@ -281,13 +263,37 @@
   </si>
   <si>
     <t>site</t>
+  </si>
+  <si>
+    <t>column header in metabolites sheet. Always keep as 1st row</t>
+  </si>
+  <si>
+    <t>Subject Identifier. Always keep as 2nd row.</t>
+  </si>
+  <si>
+    <t>age at the time of metabolite measurement</t>
+  </si>
+  <si>
+    <t>BMI (In kg/m2)</t>
+  </si>
+  <si>
+    <t>Age (y)</t>
+  </si>
+  <si>
+    <t>clinic</t>
+  </si>
+  <si>
+    <t>BMI at the time of metabolite measurement</t>
+  </si>
+  <si>
+    <t>site identifier.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="22" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -828,7 +834,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="19" fillId="34" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -857,6 +863,9 @@
     <xf numFmtId="0" fontId="18" fillId="35" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" wrapText="1"/>
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="35" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1171,31 +1180,31 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E352"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="36.5" style="1" customWidth="1"/>
-    <col min="2" max="2" width="38.5" style="1" customWidth="1"/>
-    <col min="3" max="3" width="12.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="8.83203125" style="1"/>
+    <col min="1" max="1" width="36.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="38.42578125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="14" customHeight="1">
+    <row r="1" spans="1:5" ht="14.1" customHeight="1">
       <c r="A1" s="2" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -1204,13 +1213,13 @@
         <v>1</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="16" customHeight="1">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="15.95" customHeight="1">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -1227,7 +1236,7 @@
         <v>146.11689999999999</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="16" customHeight="1">
+    <row r="3" spans="1:5" ht="15.95" customHeight="1">
       <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
@@ -1241,7 +1250,7 @@
         <v>117.04259999999999</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="16" customHeight="1">
+    <row r="4" spans="1:5" ht="15.95" customHeight="1">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
@@ -1255,7 +1264,7 @@
         <v>188.03210000000001</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="16" customHeight="1">
+    <row r="5" spans="1:5" ht="15.95" customHeight="1">
       <c r="A5" s="2" t="s">
         <v>11</v>
       </c>
@@ -1269,7 +1278,7 @@
         <v>135.05449999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="16" customHeight="1">
+    <row r="6" spans="1:5" ht="15.95" customHeight="1">
       <c r="A6" s="2" t="s">
         <v>14</v>
       </c>
@@ -1283,7 +1292,7 @@
         <v>267.09675499999997</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="16" customHeight="1">
+    <row r="7" spans="1:5" ht="15.95" customHeight="1">
       <c r="A7" s="2" t="s">
         <v>17</v>
       </c>
@@ -1297,7 +1306,7 @@
         <v>145.1</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="16" customHeight="1">
+    <row r="8" spans="1:5" ht="15.95" customHeight="1">
       <c r="A8" s="2" t="s">
         <v>20</v>
       </c>
@@ -1314,7 +1323,7 @@
         <v>203.15</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="16" customHeight="1">
+    <row r="9" spans="1:5" ht="15.95" customHeight="1">
       <c r="A9" s="2" t="s">
         <v>22</v>
       </c>
@@ -1328,7 +1337,7 @@
         <v>462.2</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="16" customHeight="1">
+    <row r="10" spans="1:5" ht="15.95" customHeight="1">
       <c r="A10" s="2" t="s">
         <v>24</v>
       </c>
@@ -1345,7 +1354,7 @@
         <v>90.06</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="16" customHeight="1">
+    <row r="11" spans="1:5" ht="15.95" customHeight="1">
       <c r="A11" s="2" t="s">
         <v>27</v>
       </c>
@@ -1359,7 +1368,7 @@
         <v>157.1</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="16" customHeight="1">
+    <row r="12" spans="1:5" ht="15.95" customHeight="1">
       <c r="A12" s="2" t="s">
         <v>30</v>
       </c>
@@ -1370,7 +1379,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="16" customHeight="1">
+    <row r="13" spans="1:5" ht="15.95" customHeight="1">
       <c r="A13" s="2" t="s">
         <v>33</v>
       </c>
@@ -1387,7 +1396,7 @@
         <v>258.1105</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="16" customHeight="1">
+    <row r="14" spans="1:5" ht="15.95" customHeight="1">
       <c r="A14" s="2" t="s">
         <v>36</v>
       </c>
@@ -1398,7 +1407,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="16" customHeight="1">
+    <row r="15" spans="1:5" ht="15.95" customHeight="1">
       <c r="A15" s="2" t="s">
         <v>39</v>
       </c>
@@ -1409,7 +1418,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="16" customHeight="1">
+    <row r="16" spans="1:5" ht="15.95" customHeight="1">
       <c r="A16" s="2" t="s">
         <v>42</v>
       </c>
@@ -1426,7 +1435,7 @@
         <v>104.07</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="16" customHeight="1">
+    <row r="17" spans="1:5" ht="15.95" customHeight="1">
       <c r="A17" s="2" t="s">
         <v>45</v>
       </c>
@@ -1440,7 +1449,7 @@
         <v>346.2</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="16" customHeight="1">
+    <row r="18" spans="1:5" ht="15.95" customHeight="1">
       <c r="A18" s="2" t="s">
         <v>47</v>
       </c>
@@ -1457,7 +1466,7 @@
         <v>241.13</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="16" customHeight="1">
+    <row r="19" spans="1:5" ht="15.95" customHeight="1">
       <c r="A19" s="2" t="s">
         <v>50</v>
       </c>
@@ -1471,1667 +1480,1667 @@
         <v>136.1</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="16" customHeight="1">
+    <row r="20" spans="1:5" ht="15.95" customHeight="1">
       <c r="A20" s="2"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
     </row>
-    <row r="21" spans="1:5" ht="16" customHeight="1">
+    <row r="21" spans="1:5" ht="15.95" customHeight="1">
       <c r="A21" s="2"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
     </row>
-    <row r="22" spans="1:5" ht="16" customHeight="1">
+    <row r="22" spans="1:5" ht="15.95" customHeight="1">
       <c r="A22" s="2"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
     </row>
-    <row r="23" spans="1:5" ht="16" customHeight="1">
+    <row r="23" spans="1:5" ht="15.95" customHeight="1">
       <c r="A23" s="2"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
     </row>
-    <row r="24" spans="1:5" ht="16" customHeight="1">
+    <row r="24" spans="1:5" ht="15.95" customHeight="1">
       <c r="A24" s="2"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
     </row>
-    <row r="25" spans="1:5" ht="16" customHeight="1">
+    <row r="25" spans="1:5" ht="15.95" customHeight="1">
       <c r="A25" s="2"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
     </row>
-    <row r="26" spans="1:5" ht="16" customHeight="1">
+    <row r="26" spans="1:5" ht="15.95" customHeight="1">
       <c r="A26" s="2"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
     </row>
-    <row r="27" spans="1:5" ht="16" customHeight="1">
+    <row r="27" spans="1:5" ht="15.95" customHeight="1">
       <c r="A27" s="2"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
     </row>
-    <row r="28" spans="1:5" ht="16" customHeight="1">
+    <row r="28" spans="1:5" ht="15.95" customHeight="1">
       <c r="A28" s="2"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
     </row>
-    <row r="29" spans="1:5" ht="16" customHeight="1">
+    <row r="29" spans="1:5" ht="15.95" customHeight="1">
       <c r="A29" s="2"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
     </row>
-    <row r="30" spans="1:5" ht="16" customHeight="1">
+    <row r="30" spans="1:5" ht="15.95" customHeight="1">
       <c r="A30" s="2"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
     </row>
-    <row r="31" spans="1:5" ht="16" customHeight="1">
+    <row r="31" spans="1:5" ht="15.95" customHeight="1">
       <c r="A31" s="2"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
     </row>
-    <row r="32" spans="1:5" ht="16" customHeight="1">
+    <row r="32" spans="1:5" ht="15.95" customHeight="1">
       <c r="A32" s="2"/>
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
     </row>
-    <row r="33" spans="1:3" ht="16" customHeight="1">
+    <row r="33" spans="1:3" ht="15.95" customHeight="1">
       <c r="A33" s="2"/>
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
     </row>
-    <row r="34" spans="1:3" ht="16" customHeight="1">
+    <row r="34" spans="1:3" ht="15.95" customHeight="1">
       <c r="A34" s="2"/>
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
     </row>
-    <row r="35" spans="1:3" ht="16" customHeight="1">
+    <row r="35" spans="1:3" ht="15.95" customHeight="1">
       <c r="A35" s="2"/>
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
     </row>
-    <row r="36" spans="1:3" ht="16" customHeight="1">
+    <row r="36" spans="1:3" ht="15.95" customHeight="1">
       <c r="A36" s="2"/>
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
     </row>
-    <row r="37" spans="1:3" ht="16" customHeight="1">
+    <row r="37" spans="1:3" ht="15.95" customHeight="1">
       <c r="A37" s="2"/>
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
     </row>
-    <row r="38" spans="1:3" ht="16" customHeight="1">
+    <row r="38" spans="1:3" ht="15.95" customHeight="1">
       <c r="A38" s="2"/>
       <c r="B38" s="3"/>
       <c r="C38" s="3"/>
     </row>
-    <row r="39" spans="1:3" ht="16" customHeight="1">
+    <row r="39" spans="1:3" ht="15.95" customHeight="1">
       <c r="A39" s="2"/>
       <c r="B39" s="3"/>
       <c r="C39" s="3"/>
     </row>
-    <row r="40" spans="1:3" ht="16" customHeight="1">
+    <row r="40" spans="1:3" ht="15.95" customHeight="1">
       <c r="A40" s="2"/>
       <c r="B40" s="3"/>
       <c r="C40" s="3"/>
     </row>
-    <row r="41" spans="1:3" ht="16" customHeight="1">
+    <row r="41" spans="1:3" ht="15.95" customHeight="1">
       <c r="A41" s="2"/>
       <c r="B41" s="3"/>
       <c r="C41" s="3"/>
     </row>
-    <row r="42" spans="1:3" ht="16" customHeight="1">
+    <row r="42" spans="1:3" ht="15.95" customHeight="1">
       <c r="A42" s="2"/>
       <c r="B42" s="3"/>
       <c r="C42" s="3"/>
     </row>
-    <row r="43" spans="1:3" ht="16" customHeight="1">
+    <row r="43" spans="1:3" ht="15.95" customHeight="1">
       <c r="A43" s="2"/>
       <c r="B43" s="3"/>
       <c r="C43" s="3"/>
     </row>
-    <row r="44" spans="1:3" ht="16" customHeight="1">
+    <row r="44" spans="1:3" ht="15.95" customHeight="1">
       <c r="A44" s="2"/>
       <c r="B44" s="3"/>
       <c r="C44" s="3"/>
     </row>
-    <row r="45" spans="1:3" ht="16" customHeight="1">
+    <row r="45" spans="1:3" ht="15.95" customHeight="1">
       <c r="A45" s="2"/>
       <c r="B45" s="3"/>
       <c r="C45" s="3"/>
     </row>
-    <row r="46" spans="1:3" ht="16" customHeight="1">
+    <row r="46" spans="1:3" ht="15.95" customHeight="1">
       <c r="A46" s="2"/>
       <c r="B46" s="3"/>
       <c r="C46" s="3"/>
     </row>
-    <row r="47" spans="1:3" ht="16" customHeight="1">
+    <row r="47" spans="1:3" ht="15.95" customHeight="1">
       <c r="A47" s="2"/>
       <c r="B47" s="3"/>
       <c r="C47" s="3"/>
     </row>
-    <row r="48" spans="1:3" ht="16" customHeight="1">
+    <row r="48" spans="1:3" ht="15.95" customHeight="1">
       <c r="A48" s="2"/>
       <c r="B48" s="3"/>
       <c r="C48" s="3"/>
     </row>
-    <row r="49" spans="1:3" ht="16" customHeight="1">
+    <row r="49" spans="1:3" ht="15.95" customHeight="1">
       <c r="A49" s="2"/>
       <c r="B49" s="3"/>
       <c r="C49" s="3"/>
     </row>
-    <row r="50" spans="1:3" ht="16" customHeight="1">
+    <row r="50" spans="1:3" ht="15.95" customHeight="1">
       <c r="A50" s="2"/>
       <c r="B50" s="3"/>
       <c r="C50" s="3"/>
     </row>
-    <row r="51" spans="1:3" ht="16" customHeight="1">
+    <row r="51" spans="1:3" ht="15.95" customHeight="1">
       <c r="A51" s="2"/>
       <c r="B51" s="3"/>
       <c r="C51" s="3"/>
     </row>
-    <row r="52" spans="1:3" ht="16" customHeight="1">
+    <row r="52" spans="1:3" ht="15.95" customHeight="1">
       <c r="A52" s="2"/>
       <c r="B52" s="3"/>
       <c r="C52" s="3"/>
     </row>
-    <row r="53" spans="1:3" ht="16" customHeight="1">
+    <row r="53" spans="1:3" ht="15.95" customHeight="1">
       <c r="A53" s="2"/>
       <c r="B53" s="3"/>
       <c r="C53" s="3"/>
     </row>
-    <row r="54" spans="1:3" ht="16" customHeight="1">
+    <row r="54" spans="1:3" ht="15.95" customHeight="1">
       <c r="A54" s="2"/>
       <c r="B54" s="3"/>
       <c r="C54" s="3"/>
     </row>
-    <row r="55" spans="1:3" ht="16" customHeight="1">
+    <row r="55" spans="1:3" ht="15.95" customHeight="1">
       <c r="A55" s="2"/>
       <c r="B55" s="3"/>
       <c r="C55" s="3"/>
     </row>
-    <row r="56" spans="1:3" ht="16" customHeight="1">
+    <row r="56" spans="1:3" ht="15.95" customHeight="1">
       <c r="A56" s="2"/>
       <c r="B56" s="3"/>
       <c r="C56" s="3"/>
     </row>
-    <row r="57" spans="1:3" ht="16" customHeight="1">
+    <row r="57" spans="1:3" ht="15.95" customHeight="1">
       <c r="A57" s="2"/>
       <c r="B57" s="3"/>
       <c r="C57" s="3"/>
     </row>
-    <row r="58" spans="1:3" ht="16" customHeight="1">
+    <row r="58" spans="1:3" ht="15.95" customHeight="1">
       <c r="A58" s="2"/>
       <c r="B58" s="3"/>
       <c r="C58" s="3"/>
     </row>
-    <row r="59" spans="1:3" ht="16" customHeight="1">
+    <row r="59" spans="1:3" ht="15.95" customHeight="1">
       <c r="A59" s="2"/>
       <c r="B59" s="3"/>
       <c r="C59" s="3"/>
     </row>
-    <row r="60" spans="1:3" ht="16" customHeight="1">
+    <row r="60" spans="1:3" ht="15.95" customHeight="1">
       <c r="A60" s="2"/>
       <c r="B60" s="3"/>
       <c r="C60" s="3"/>
     </row>
-    <row r="61" spans="1:3" ht="16" customHeight="1">
+    <row r="61" spans="1:3" ht="15.95" customHeight="1">
       <c r="A61" s="2"/>
       <c r="B61" s="3"/>
       <c r="C61" s="3"/>
     </row>
-    <row r="62" spans="1:3" ht="16" customHeight="1">
+    <row r="62" spans="1:3" ht="15.95" customHeight="1">
       <c r="A62" s="2"/>
       <c r="B62" s="3"/>
       <c r="C62" s="3"/>
     </row>
-    <row r="63" spans="1:3" ht="16" customHeight="1">
+    <row r="63" spans="1:3" ht="15.95" customHeight="1">
       <c r="A63" s="2"/>
       <c r="B63" s="3"/>
       <c r="C63" s="3"/>
     </row>
-    <row r="64" spans="1:3" ht="16" customHeight="1">
+    <row r="64" spans="1:3" ht="15.95" customHeight="1">
       <c r="A64" s="2"/>
       <c r="B64" s="3"/>
       <c r="C64" s="3"/>
     </row>
-    <row r="65" spans="1:3" ht="16" customHeight="1">
+    <row r="65" spans="1:3" ht="15.95" customHeight="1">
       <c r="A65" s="2"/>
       <c r="B65" s="3"/>
       <c r="C65" s="3"/>
     </row>
-    <row r="66" spans="1:3" ht="16" customHeight="1">
+    <row r="66" spans="1:3" ht="15.95" customHeight="1">
       <c r="A66" s="2"/>
       <c r="B66" s="3"/>
       <c r="C66" s="3"/>
     </row>
-    <row r="67" spans="1:3" ht="16" customHeight="1">
+    <row r="67" spans="1:3" ht="15.95" customHeight="1">
       <c r="A67" s="2"/>
       <c r="B67" s="3"/>
       <c r="C67" s="3"/>
     </row>
-    <row r="68" spans="1:3" ht="16" customHeight="1">
+    <row r="68" spans="1:3" ht="15.95" customHeight="1">
       <c r="A68" s="2"/>
       <c r="B68" s="3"/>
       <c r="C68" s="3"/>
     </row>
-    <row r="69" spans="1:3" ht="16" customHeight="1">
+    <row r="69" spans="1:3" ht="15.95" customHeight="1">
       <c r="A69" s="2"/>
       <c r="B69" s="3"/>
       <c r="C69" s="3"/>
     </row>
-    <row r="70" spans="1:3" ht="16" customHeight="1">
+    <row r="70" spans="1:3" ht="15.95" customHeight="1">
       <c r="A70" s="2"/>
       <c r="B70" s="3"/>
       <c r="C70" s="3"/>
     </row>
-    <row r="71" spans="1:3" ht="16" customHeight="1">
+    <row r="71" spans="1:3" ht="15.95" customHeight="1">
       <c r="A71" s="2"/>
       <c r="B71" s="3"/>
       <c r="C71" s="3"/>
     </row>
-    <row r="72" spans="1:3" ht="16" customHeight="1">
+    <row r="72" spans="1:3" ht="15.95" customHeight="1">
       <c r="A72" s="2"/>
       <c r="B72" s="3"/>
       <c r="C72" s="3"/>
     </row>
-    <row r="73" spans="1:3" ht="16" customHeight="1">
+    <row r="73" spans="1:3" ht="15.95" customHeight="1">
       <c r="A73" s="2"/>
       <c r="B73" s="3"/>
       <c r="C73" s="3"/>
     </row>
-    <row r="74" spans="1:3" ht="16" customHeight="1">
+    <row r="74" spans="1:3" ht="15.95" customHeight="1">
       <c r="A74" s="2"/>
       <c r="B74" s="3"/>
       <c r="C74" s="3"/>
     </row>
-    <row r="75" spans="1:3" ht="16" customHeight="1">
+    <row r="75" spans="1:3" ht="15.95" customHeight="1">
       <c r="A75" s="2"/>
       <c r="B75" s="3"/>
       <c r="C75" s="3"/>
     </row>
-    <row r="76" spans="1:3" ht="16" customHeight="1">
+    <row r="76" spans="1:3" ht="15.95" customHeight="1">
       <c r="A76" s="2"/>
       <c r="B76" s="3"/>
       <c r="C76" s="3"/>
     </row>
-    <row r="77" spans="1:3" ht="16" customHeight="1">
+    <row r="77" spans="1:3" ht="15.95" customHeight="1">
       <c r="A77" s="2"/>
       <c r="B77" s="3"/>
       <c r="C77" s="3"/>
     </row>
-    <row r="78" spans="1:3" ht="16" customHeight="1">
+    <row r="78" spans="1:3" ht="15.95" customHeight="1">
       <c r="A78" s="2"/>
       <c r="B78" s="3"/>
       <c r="C78" s="3"/>
     </row>
-    <row r="79" spans="1:3" ht="16" customHeight="1">
+    <row r="79" spans="1:3" ht="15.95" customHeight="1">
       <c r="A79" s="2"/>
       <c r="B79" s="3"/>
       <c r="C79" s="3"/>
     </row>
-    <row r="80" spans="1:3" ht="16" customHeight="1">
+    <row r="80" spans="1:3" ht="15.95" customHeight="1">
       <c r="A80" s="2"/>
       <c r="B80" s="3"/>
       <c r="C80" s="3"/>
     </row>
-    <row r="81" spans="1:3" ht="16" customHeight="1">
+    <row r="81" spans="1:3" ht="15.95" customHeight="1">
       <c r="A81" s="2"/>
       <c r="B81" s="3"/>
       <c r="C81" s="3"/>
     </row>
-    <row r="82" spans="1:3" ht="16" customHeight="1">
+    <row r="82" spans="1:3" ht="15.95" customHeight="1">
       <c r="A82" s="2"/>
       <c r="B82" s="3"/>
       <c r="C82" s="3"/>
     </row>
-    <row r="83" spans="1:3" ht="16" customHeight="1">
+    <row r="83" spans="1:3" ht="15.95" customHeight="1">
       <c r="A83" s="2"/>
       <c r="B83" s="3"/>
       <c r="C83" s="3"/>
     </row>
-    <row r="84" spans="1:3" ht="16" customHeight="1">
+    <row r="84" spans="1:3" ht="15.95" customHeight="1">
       <c r="A84" s="2"/>
       <c r="B84" s="3"/>
       <c r="C84" s="3"/>
     </row>
-    <row r="85" spans="1:3" ht="16" customHeight="1">
+    <row r="85" spans="1:3" ht="15.95" customHeight="1">
       <c r="A85" s="2"/>
       <c r="B85" s="3"/>
       <c r="C85" s="3"/>
     </row>
-    <row r="86" spans="1:3" ht="16" customHeight="1">
+    <row r="86" spans="1:3" ht="15.95" customHeight="1">
       <c r="A86" s="2"/>
       <c r="B86" s="3"/>
       <c r="C86" s="3"/>
     </row>
-    <row r="87" spans="1:3" ht="16" customHeight="1">
+    <row r="87" spans="1:3" ht="15.95" customHeight="1">
       <c r="A87" s="2"/>
       <c r="B87" s="3"/>
       <c r="C87" s="3"/>
     </row>
-    <row r="88" spans="1:3" ht="16" customHeight="1">
+    <row r="88" spans="1:3" ht="15.95" customHeight="1">
       <c r="A88" s="2"/>
       <c r="B88" s="3"/>
       <c r="C88" s="3"/>
     </row>
-    <row r="89" spans="1:3" ht="16" customHeight="1">
+    <row r="89" spans="1:3" ht="15.95" customHeight="1">
       <c r="A89" s="2"/>
       <c r="B89" s="3"/>
       <c r="C89" s="3"/>
     </row>
-    <row r="90" spans="1:3" ht="16" customHeight="1">
+    <row r="90" spans="1:3" ht="15.95" customHeight="1">
       <c r="A90" s="2"/>
       <c r="B90" s="3"/>
       <c r="C90" s="3"/>
     </row>
-    <row r="91" spans="1:3" ht="16" customHeight="1">
+    <row r="91" spans="1:3" ht="15.95" customHeight="1">
       <c r="A91" s="2"/>
       <c r="B91" s="3"/>
       <c r="C91" s="3"/>
     </row>
-    <row r="92" spans="1:3" ht="16" customHeight="1">
+    <row r="92" spans="1:3" ht="15.95" customHeight="1">
       <c r="A92" s="2"/>
       <c r="B92" s="3"/>
       <c r="C92" s="3"/>
     </row>
-    <row r="93" spans="1:3" ht="16" customHeight="1">
+    <row r="93" spans="1:3" ht="15.95" customHeight="1">
       <c r="A93" s="2"/>
       <c r="B93" s="3"/>
       <c r="C93" s="3"/>
     </row>
-    <row r="94" spans="1:3" ht="16" customHeight="1">
+    <row r="94" spans="1:3" ht="15.95" customHeight="1">
       <c r="A94" s="2"/>
       <c r="B94" s="3"/>
       <c r="C94" s="3"/>
     </row>
-    <row r="95" spans="1:3" ht="16" customHeight="1">
+    <row r="95" spans="1:3" ht="15.95" customHeight="1">
       <c r="A95" s="2"/>
       <c r="B95" s="3"/>
       <c r="C95" s="3"/>
     </row>
-    <row r="96" spans="1:3" ht="16" customHeight="1">
+    <row r="96" spans="1:3" ht="15.95" customHeight="1">
       <c r="A96" s="2"/>
       <c r="B96" s="3"/>
       <c r="C96" s="3"/>
     </row>
-    <row r="97" spans="1:3" ht="16" customHeight="1">
+    <row r="97" spans="1:3" ht="15.95" customHeight="1">
       <c r="A97" s="2"/>
       <c r="B97" s="3"/>
       <c r="C97" s="3"/>
     </row>
-    <row r="98" spans="1:3" ht="16" customHeight="1">
+    <row r="98" spans="1:3" ht="15.95" customHeight="1">
       <c r="A98" s="2"/>
       <c r="B98" s="3"/>
       <c r="C98" s="3"/>
     </row>
-    <row r="99" spans="1:3" ht="16" customHeight="1">
+    <row r="99" spans="1:3" ht="15.95" customHeight="1">
       <c r="A99" s="2"/>
       <c r="B99" s="3"/>
       <c r="C99" s="3"/>
     </row>
-    <row r="100" spans="1:3" ht="16" customHeight="1">
+    <row r="100" spans="1:3" ht="15.95" customHeight="1">
       <c r="A100" s="2"/>
       <c r="B100" s="3"/>
       <c r="C100" s="3"/>
     </row>
-    <row r="101" spans="1:3" ht="16" customHeight="1">
+    <row r="101" spans="1:3" ht="15.95" customHeight="1">
       <c r="A101" s="2"/>
       <c r="B101" s="3"/>
       <c r="C101" s="3"/>
     </row>
-    <row r="102" spans="1:3" ht="16" customHeight="1">
+    <row r="102" spans="1:3" ht="15.95" customHeight="1">
       <c r="A102" s="2"/>
       <c r="B102" s="3"/>
       <c r="C102" s="3"/>
     </row>
-    <row r="103" spans="1:3" ht="16" customHeight="1">
+    <row r="103" spans="1:3" ht="15.95" customHeight="1">
       <c r="A103" s="2"/>
       <c r="B103" s="3"/>
       <c r="C103" s="3"/>
     </row>
-    <row r="104" spans="1:3" ht="16" customHeight="1">
+    <row r="104" spans="1:3" ht="15.95" customHeight="1">
       <c r="A104" s="2"/>
       <c r="B104" s="3"/>
       <c r="C104" s="3"/>
     </row>
-    <row r="105" spans="1:3" ht="16" customHeight="1">
+    <row r="105" spans="1:3" ht="15.95" customHeight="1">
       <c r="A105" s="2"/>
       <c r="B105" s="3"/>
       <c r="C105" s="3"/>
     </row>
-    <row r="106" spans="1:3" ht="16" customHeight="1">
+    <row r="106" spans="1:3" ht="15.95" customHeight="1">
       <c r="A106" s="2"/>
       <c r="B106" s="3"/>
       <c r="C106" s="3"/>
     </row>
-    <row r="107" spans="1:3" ht="16" customHeight="1">
+    <row r="107" spans="1:3" ht="15.95" customHeight="1">
       <c r="A107" s="2"/>
       <c r="B107" s="3"/>
       <c r="C107" s="3"/>
     </row>
-    <row r="108" spans="1:3" ht="16" customHeight="1">
+    <row r="108" spans="1:3" ht="15.95" customHeight="1">
       <c r="A108" s="2"/>
       <c r="B108" s="3"/>
       <c r="C108" s="3"/>
     </row>
-    <row r="109" spans="1:3" ht="16" customHeight="1">
+    <row r="109" spans="1:3" ht="15.95" customHeight="1">
       <c r="A109" s="2"/>
       <c r="B109" s="3"/>
       <c r="C109" s="3"/>
     </row>
-    <row r="110" spans="1:3" ht="16" customHeight="1">
+    <row r="110" spans="1:3" ht="15.95" customHeight="1">
       <c r="A110" s="2"/>
       <c r="B110" s="3"/>
       <c r="C110" s="3"/>
     </row>
-    <row r="111" spans="1:3" ht="16" customHeight="1">
+    <row r="111" spans="1:3" ht="15.95" customHeight="1">
       <c r="A111" s="2"/>
       <c r="B111" s="3"/>
       <c r="C111" s="3"/>
     </row>
-    <row r="112" spans="1:3" ht="16" customHeight="1">
+    <row r="112" spans="1:3" ht="15.95" customHeight="1">
       <c r="A112" s="2"/>
       <c r="B112" s="3"/>
       <c r="C112" s="3"/>
     </row>
-    <row r="113" spans="1:3" ht="16" customHeight="1">
+    <row r="113" spans="1:3" ht="15.95" customHeight="1">
       <c r="A113" s="2"/>
       <c r="B113" s="3"/>
       <c r="C113" s="3"/>
     </row>
-    <row r="114" spans="1:3" ht="16" customHeight="1">
+    <row r="114" spans="1:3" ht="15.95" customHeight="1">
       <c r="A114" s="2"/>
       <c r="B114" s="3"/>
       <c r="C114" s="3"/>
     </row>
-    <row r="115" spans="1:3" ht="16" customHeight="1">
+    <row r="115" spans="1:3" ht="15.95" customHeight="1">
       <c r="A115" s="2"/>
       <c r="B115" s="3"/>
       <c r="C115" s="3"/>
     </row>
-    <row r="116" spans="1:3" ht="16" customHeight="1">
+    <row r="116" spans="1:3" ht="15.95" customHeight="1">
       <c r="A116" s="2"/>
       <c r="B116" s="3"/>
       <c r="C116" s="3"/>
     </row>
-    <row r="117" spans="1:3" ht="16" customHeight="1">
+    <row r="117" spans="1:3" ht="15.95" customHeight="1">
       <c r="A117" s="2"/>
       <c r="B117" s="3"/>
       <c r="C117" s="3"/>
     </row>
-    <row r="118" spans="1:3" ht="16" customHeight="1">
+    <row r="118" spans="1:3" ht="15.95" customHeight="1">
       <c r="A118" s="2"/>
       <c r="B118" s="3"/>
       <c r="C118" s="3"/>
     </row>
-    <row r="119" spans="1:3" ht="16" customHeight="1">
+    <row r="119" spans="1:3" ht="15.95" customHeight="1">
       <c r="A119" s="2"/>
       <c r="B119" s="3"/>
       <c r="C119" s="3"/>
     </row>
-    <row r="120" spans="1:3" ht="16" customHeight="1">
+    <row r="120" spans="1:3" ht="15.95" customHeight="1">
       <c r="A120" s="2"/>
       <c r="B120" s="3"/>
       <c r="C120" s="3"/>
     </row>
-    <row r="121" spans="1:3" ht="16" customHeight="1">
+    <row r="121" spans="1:3" ht="15.95" customHeight="1">
       <c r="A121" s="2"/>
       <c r="B121" s="3"/>
       <c r="C121" s="3"/>
     </row>
-    <row r="122" spans="1:3" ht="16" customHeight="1">
+    <row r="122" spans="1:3" ht="15.95" customHeight="1">
       <c r="A122" s="2"/>
       <c r="B122" s="3"/>
       <c r="C122" s="3"/>
     </row>
-    <row r="123" spans="1:3" ht="16" customHeight="1">
+    <row r="123" spans="1:3" ht="15.95" customHeight="1">
       <c r="A123" s="2"/>
       <c r="B123" s="3"/>
       <c r="C123" s="3"/>
     </row>
-    <row r="124" spans="1:3" ht="16" customHeight="1">
+    <row r="124" spans="1:3" ht="15.95" customHeight="1">
       <c r="A124" s="2"/>
       <c r="B124" s="3"/>
       <c r="C124" s="3"/>
     </row>
-    <row r="125" spans="1:3" ht="16" customHeight="1">
+    <row r="125" spans="1:3" ht="15.95" customHeight="1">
       <c r="A125" s="2"/>
       <c r="B125" s="3"/>
       <c r="C125" s="3"/>
     </row>
-    <row r="126" spans="1:3" ht="16" customHeight="1">
+    <row r="126" spans="1:3" ht="15.95" customHeight="1">
       <c r="A126" s="2"/>
       <c r="B126" s="3"/>
       <c r="C126" s="3"/>
     </row>
-    <row r="127" spans="1:3" ht="16" customHeight="1">
+    <row r="127" spans="1:3" ht="15.95" customHeight="1">
       <c r="A127" s="2"/>
       <c r="B127" s="3"/>
       <c r="C127" s="3"/>
     </row>
-    <row r="128" spans="1:3" ht="16" customHeight="1">
+    <row r="128" spans="1:3" ht="15.95" customHeight="1">
       <c r="A128" s="2"/>
       <c r="B128" s="3"/>
       <c r="C128" s="3"/>
     </row>
-    <row r="129" spans="1:3" ht="16" customHeight="1">
+    <row r="129" spans="1:3" ht="15.95" customHeight="1">
       <c r="A129" s="2"/>
       <c r="B129" s="3"/>
       <c r="C129" s="3"/>
     </row>
-    <row r="130" spans="1:3" ht="16" customHeight="1">
+    <row r="130" spans="1:3" ht="15.95" customHeight="1">
       <c r="A130" s="2"/>
       <c r="B130" s="3"/>
       <c r="C130" s="3"/>
     </row>
-    <row r="131" spans="1:3" ht="16" customHeight="1">
+    <row r="131" spans="1:3" ht="15.95" customHeight="1">
       <c r="A131" s="2"/>
       <c r="B131" s="3"/>
       <c r="C131" s="3"/>
     </row>
-    <row r="132" spans="1:3" ht="16" customHeight="1">
+    <row r="132" spans="1:3" ht="15.95" customHeight="1">
       <c r="A132" s="2"/>
       <c r="B132" s="3"/>
       <c r="C132" s="3"/>
     </row>
-    <row r="133" spans="1:3" ht="16" customHeight="1">
+    <row r="133" spans="1:3" ht="15.95" customHeight="1">
       <c r="A133" s="2"/>
       <c r="B133" s="3"/>
       <c r="C133" s="3"/>
     </row>
-    <row r="134" spans="1:3" ht="16" customHeight="1">
+    <row r="134" spans="1:3" ht="15.95" customHeight="1">
       <c r="A134" s="2"/>
       <c r="B134" s="3"/>
       <c r="C134" s="3"/>
     </row>
-    <row r="135" spans="1:3" ht="16" customHeight="1">
+    <row r="135" spans="1:3" ht="15.95" customHeight="1">
       <c r="A135" s="2"/>
       <c r="B135" s="3"/>
       <c r="C135" s="3"/>
     </row>
-    <row r="136" spans="1:3" ht="16" customHeight="1">
+    <row r="136" spans="1:3" ht="15.95" customHeight="1">
       <c r="A136" s="2"/>
       <c r="B136" s="3"/>
       <c r="C136" s="3"/>
     </row>
-    <row r="137" spans="1:3" ht="16" customHeight="1">
+    <row r="137" spans="1:3" ht="15.95" customHeight="1">
       <c r="A137" s="2"/>
       <c r="B137" s="3"/>
       <c r="C137" s="3"/>
     </row>
-    <row r="138" spans="1:3" ht="16" customHeight="1">
+    <row r="138" spans="1:3" ht="15.95" customHeight="1">
       <c r="A138" s="2"/>
       <c r="B138" s="3"/>
       <c r="C138" s="3"/>
     </row>
-    <row r="139" spans="1:3" ht="16" customHeight="1">
+    <row r="139" spans="1:3" ht="15.95" customHeight="1">
       <c r="A139" s="2"/>
       <c r="B139" s="3"/>
       <c r="C139" s="3"/>
     </row>
-    <row r="140" spans="1:3" ht="16" customHeight="1">
+    <row r="140" spans="1:3" ht="15.95" customHeight="1">
       <c r="A140" s="2"/>
       <c r="B140" s="3"/>
       <c r="C140" s="3"/>
     </row>
-    <row r="141" spans="1:3" ht="16" customHeight="1">
+    <row r="141" spans="1:3" ht="15.95" customHeight="1">
       <c r="A141" s="2"/>
       <c r="B141" s="3"/>
       <c r="C141" s="3"/>
     </row>
-    <row r="142" spans="1:3" ht="16" customHeight="1">
+    <row r="142" spans="1:3" ht="15.95" customHeight="1">
       <c r="A142" s="2"/>
       <c r="B142" s="3"/>
       <c r="C142" s="3"/>
     </row>
-    <row r="143" spans="1:3" ht="16" customHeight="1">
+    <row r="143" spans="1:3" ht="15.95" customHeight="1">
       <c r="A143" s="2"/>
       <c r="B143" s="3"/>
       <c r="C143" s="3"/>
     </row>
-    <row r="144" spans="1:3" ht="16" customHeight="1">
+    <row r="144" spans="1:3" ht="15.95" customHeight="1">
       <c r="A144" s="2"/>
       <c r="B144" s="3"/>
       <c r="C144" s="3"/>
     </row>
-    <row r="145" spans="1:3" ht="16" customHeight="1">
+    <row r="145" spans="1:3" ht="15.95" customHeight="1">
       <c r="A145" s="2"/>
       <c r="B145" s="3"/>
       <c r="C145" s="3"/>
     </row>
-    <row r="146" spans="1:3" ht="16" customHeight="1">
+    <row r="146" spans="1:3" ht="15.95" customHeight="1">
       <c r="A146" s="2"/>
       <c r="B146" s="3"/>
       <c r="C146" s="3"/>
     </row>
-    <row r="147" spans="1:3" ht="16" customHeight="1">
+    <row r="147" spans="1:3" ht="15.95" customHeight="1">
       <c r="A147" s="2"/>
       <c r="B147" s="3"/>
       <c r="C147" s="3"/>
     </row>
-    <row r="148" spans="1:3" ht="16" customHeight="1">
+    <row r="148" spans="1:3" ht="15.95" customHeight="1">
       <c r="A148" s="2"/>
       <c r="B148" s="3"/>
       <c r="C148" s="3"/>
     </row>
-    <row r="149" spans="1:3" ht="16" customHeight="1">
+    <row r="149" spans="1:3" ht="15.95" customHeight="1">
       <c r="A149" s="2"/>
       <c r="B149" s="3"/>
       <c r="C149" s="3"/>
     </row>
-    <row r="150" spans="1:3" ht="16" customHeight="1">
+    <row r="150" spans="1:3" ht="15.95" customHeight="1">
       <c r="A150" s="2"/>
       <c r="B150" s="3"/>
       <c r="C150" s="3"/>
     </row>
-    <row r="151" spans="1:3" ht="16" customHeight="1">
+    <row r="151" spans="1:3" ht="15.95" customHeight="1">
       <c r="A151" s="2"/>
       <c r="B151" s="3"/>
       <c r="C151" s="3"/>
     </row>
-    <row r="152" spans="1:3" ht="16" customHeight="1">
+    <row r="152" spans="1:3" ht="15.95" customHeight="1">
       <c r="A152" s="2"/>
       <c r="B152" s="3"/>
       <c r="C152" s="3"/>
     </row>
-    <row r="153" spans="1:3" ht="16" customHeight="1">
+    <row r="153" spans="1:3" ht="15.95" customHeight="1">
       <c r="A153" s="2"/>
       <c r="B153" s="3"/>
       <c r="C153" s="3"/>
     </row>
-    <row r="154" spans="1:3" ht="16" customHeight="1">
+    <row r="154" spans="1:3" ht="15.95" customHeight="1">
       <c r="A154" s="2"/>
       <c r="B154" s="3"/>
       <c r="C154" s="3"/>
     </row>
-    <row r="155" spans="1:3" ht="16" customHeight="1">
+    <row r="155" spans="1:3" ht="15.95" customHeight="1">
       <c r="A155" s="2"/>
       <c r="B155" s="3"/>
       <c r="C155" s="3"/>
     </row>
-    <row r="156" spans="1:3" ht="16" customHeight="1">
+    <row r="156" spans="1:3" ht="15.95" customHeight="1">
       <c r="A156" s="2"/>
       <c r="B156" s="3"/>
       <c r="C156" s="3"/>
     </row>
-    <row r="157" spans="1:3" ht="16" customHeight="1">
+    <row r="157" spans="1:3" ht="15.95" customHeight="1">
       <c r="A157" s="2"/>
       <c r="B157" s="3"/>
       <c r="C157" s="3"/>
     </row>
-    <row r="158" spans="1:3" ht="16" customHeight="1">
+    <row r="158" spans="1:3" ht="15.95" customHeight="1">
       <c r="A158" s="2"/>
       <c r="B158" s="3"/>
       <c r="C158" s="3"/>
     </row>
-    <row r="159" spans="1:3" ht="16" customHeight="1">
+    <row r="159" spans="1:3" ht="15.95" customHeight="1">
       <c r="A159" s="2"/>
       <c r="B159" s="3"/>
       <c r="C159" s="3"/>
     </row>
-    <row r="160" spans="1:3" ht="16" customHeight="1">
+    <row r="160" spans="1:3" ht="15.95" customHeight="1">
       <c r="A160" s="2"/>
       <c r="B160" s="3"/>
       <c r="C160" s="3"/>
     </row>
-    <row r="161" spans="1:3" ht="16" customHeight="1">
+    <row r="161" spans="1:3" ht="15.95" customHeight="1">
       <c r="A161" s="2"/>
       <c r="B161" s="3"/>
       <c r="C161" s="3"/>
     </row>
-    <row r="162" spans="1:3" ht="16" customHeight="1">
+    <row r="162" spans="1:3" ht="15.95" customHeight="1">
       <c r="A162" s="2"/>
       <c r="B162" s="3"/>
       <c r="C162" s="3"/>
     </row>
-    <row r="163" spans="1:3" ht="16" customHeight="1">
+    <row r="163" spans="1:3" ht="15.95" customHeight="1">
       <c r="A163" s="2"/>
       <c r="B163" s="3"/>
       <c r="C163" s="3"/>
     </row>
-    <row r="164" spans="1:3" ht="16" customHeight="1">
+    <row r="164" spans="1:3" ht="15.95" customHeight="1">
       <c r="A164" s="2"/>
       <c r="B164" s="3"/>
       <c r="C164" s="3"/>
     </row>
-    <row r="165" spans="1:3" ht="16" customHeight="1">
+    <row r="165" spans="1:3" ht="15.95" customHeight="1">
       <c r="A165" s="2"/>
       <c r="B165" s="3"/>
       <c r="C165" s="3"/>
     </row>
-    <row r="166" spans="1:3" ht="16" customHeight="1">
+    <row r="166" spans="1:3" ht="15.95" customHeight="1">
       <c r="A166" s="2"/>
       <c r="B166" s="3"/>
       <c r="C166" s="3"/>
     </row>
-    <row r="167" spans="1:3" ht="16" customHeight="1">
+    <row r="167" spans="1:3" ht="15.95" customHeight="1">
       <c r="A167" s="2"/>
       <c r="B167" s="3"/>
       <c r="C167" s="3"/>
     </row>
-    <row r="168" spans="1:3" ht="16" customHeight="1">
+    <row r="168" spans="1:3" ht="15.95" customHeight="1">
       <c r="A168" s="2"/>
       <c r="B168" s="3"/>
       <c r="C168" s="3"/>
     </row>
-    <row r="169" spans="1:3" ht="16" customHeight="1">
+    <row r="169" spans="1:3" ht="15.95" customHeight="1">
       <c r="A169" s="2"/>
       <c r="B169" s="3"/>
       <c r="C169" s="3"/>
     </row>
-    <row r="170" spans="1:3" ht="16" customHeight="1">
+    <row r="170" spans="1:3" ht="15.95" customHeight="1">
       <c r="A170" s="2"/>
       <c r="B170" s="3"/>
       <c r="C170" s="3"/>
     </row>
-    <row r="171" spans="1:3" ht="16" customHeight="1">
+    <row r="171" spans="1:3" ht="15.95" customHeight="1">
       <c r="A171" s="2"/>
       <c r="B171" s="3"/>
       <c r="C171" s="3"/>
     </row>
-    <row r="172" spans="1:3" ht="16" customHeight="1">
+    <row r="172" spans="1:3" ht="15.95" customHeight="1">
       <c r="A172" s="2"/>
       <c r="B172" s="3"/>
       <c r="C172" s="3"/>
     </row>
-    <row r="173" spans="1:3" ht="16" customHeight="1">
+    <row r="173" spans="1:3" ht="15.95" customHeight="1">
       <c r="A173" s="2"/>
       <c r="B173" s="3"/>
       <c r="C173" s="3"/>
     </row>
-    <row r="174" spans="1:3" ht="16" customHeight="1">
+    <row r="174" spans="1:3" ht="15.95" customHeight="1">
       <c r="A174" s="2"/>
       <c r="B174" s="3"/>
       <c r="C174" s="3"/>
     </row>
-    <row r="175" spans="1:3" ht="16" customHeight="1">
+    <row r="175" spans="1:3" ht="15.95" customHeight="1">
       <c r="A175" s="2"/>
       <c r="B175" s="3"/>
       <c r="C175" s="3"/>
     </row>
-    <row r="176" spans="1:3" ht="16" customHeight="1">
+    <row r="176" spans="1:3" ht="15.95" customHeight="1">
       <c r="A176" s="2"/>
       <c r="B176" s="3"/>
       <c r="C176" s="3"/>
     </row>
-    <row r="177" spans="1:3" ht="16" customHeight="1">
+    <row r="177" spans="1:3" ht="15.95" customHeight="1">
       <c r="A177" s="2"/>
       <c r="B177" s="3"/>
       <c r="C177" s="3"/>
     </row>
-    <row r="178" spans="1:3" ht="16" customHeight="1">
+    <row r="178" spans="1:3" ht="15.95" customHeight="1">
       <c r="A178" s="2"/>
       <c r="B178" s="3"/>
       <c r="C178" s="3"/>
     </row>
-    <row r="179" spans="1:3" ht="16" customHeight="1">
+    <row r="179" spans="1:3" ht="15.95" customHeight="1">
       <c r="A179" s="2"/>
       <c r="B179" s="3"/>
       <c r="C179" s="3"/>
     </row>
-    <row r="180" spans="1:3" ht="16" customHeight="1">
+    <row r="180" spans="1:3" ht="15.95" customHeight="1">
       <c r="A180" s="2"/>
       <c r="B180" s="3"/>
       <c r="C180" s="3"/>
     </row>
-    <row r="181" spans="1:3" ht="16" customHeight="1">
+    <row r="181" spans="1:3" ht="15.95" customHeight="1">
       <c r="A181" s="2"/>
       <c r="B181" s="3"/>
       <c r="C181" s="3"/>
     </row>
-    <row r="182" spans="1:3" ht="16" customHeight="1">
+    <row r="182" spans="1:3" ht="15.95" customHeight="1">
       <c r="A182" s="2"/>
       <c r="B182" s="3"/>
       <c r="C182" s="3"/>
     </row>
-    <row r="183" spans="1:3" ht="16" customHeight="1">
+    <row r="183" spans="1:3" ht="15.95" customHeight="1">
       <c r="A183" s="2"/>
       <c r="B183" s="3"/>
       <c r="C183" s="3"/>
     </row>
-    <row r="184" spans="1:3" ht="16" customHeight="1">
+    <row r="184" spans="1:3" ht="15.95" customHeight="1">
       <c r="A184" s="2"/>
       <c r="B184" s="3"/>
       <c r="C184" s="3"/>
     </row>
-    <row r="185" spans="1:3" ht="16" customHeight="1">
+    <row r="185" spans="1:3" ht="15.95" customHeight="1">
       <c r="A185" s="2"/>
       <c r="B185" s="3"/>
       <c r="C185" s="3"/>
     </row>
-    <row r="186" spans="1:3" ht="16" customHeight="1">
+    <row r="186" spans="1:3" ht="15.95" customHeight="1">
       <c r="A186" s="2"/>
       <c r="B186" s="3"/>
       <c r="C186" s="3"/>
     </row>
-    <row r="187" spans="1:3" ht="16" customHeight="1">
+    <row r="187" spans="1:3" ht="15.95" customHeight="1">
       <c r="A187" s="2"/>
       <c r="B187" s="3"/>
       <c r="C187" s="3"/>
     </row>
-    <row r="188" spans="1:3" ht="16" customHeight="1">
+    <row r="188" spans="1:3" ht="15.95" customHeight="1">
       <c r="A188" s="2"/>
       <c r="B188" s="3"/>
       <c r="C188" s="3"/>
     </row>
-    <row r="189" spans="1:3" ht="16" customHeight="1">
+    <row r="189" spans="1:3" ht="15.95" customHeight="1">
       <c r="A189" s="2"/>
       <c r="B189" s="3"/>
       <c r="C189" s="3"/>
     </row>
-    <row r="190" spans="1:3" ht="16" customHeight="1">
+    <row r="190" spans="1:3" ht="15.95" customHeight="1">
       <c r="A190" s="2"/>
       <c r="B190" s="3"/>
       <c r="C190" s="3"/>
     </row>
-    <row r="191" spans="1:3" ht="16" customHeight="1">
+    <row r="191" spans="1:3" ht="15.95" customHeight="1">
       <c r="A191" s="2"/>
       <c r="B191" s="3"/>
       <c r="C191" s="3"/>
     </row>
-    <row r="192" spans="1:3" ht="16" customHeight="1">
+    <row r="192" spans="1:3" ht="15.95" customHeight="1">
       <c r="A192" s="2"/>
       <c r="B192" s="3"/>
       <c r="C192" s="3"/>
     </row>
-    <row r="193" spans="1:3" ht="16" customHeight="1">
+    <row r="193" spans="1:3" ht="15.95" customHeight="1">
       <c r="A193" s="2"/>
       <c r="B193" s="3"/>
       <c r="C193" s="3"/>
     </row>
-    <row r="194" spans="1:3" ht="16" customHeight="1">
+    <row r="194" spans="1:3" ht="15.95" customHeight="1">
       <c r="A194" s="2"/>
       <c r="B194" s="3"/>
       <c r="C194" s="3"/>
     </row>
-    <row r="195" spans="1:3" ht="16" customHeight="1">
+    <row r="195" spans="1:3" ht="15.95" customHeight="1">
       <c r="A195" s="2"/>
       <c r="B195" s="3"/>
       <c r="C195" s="3"/>
     </row>
-    <row r="196" spans="1:3" ht="16" customHeight="1">
+    <row r="196" spans="1:3" ht="15.95" customHeight="1">
       <c r="A196" s="2"/>
       <c r="B196" s="3"/>
       <c r="C196" s="3"/>
     </row>
-    <row r="197" spans="1:3" ht="16" customHeight="1">
+    <row r="197" spans="1:3" ht="15.95" customHeight="1">
       <c r="A197" s="2"/>
       <c r="B197" s="3"/>
       <c r="C197" s="3"/>
     </row>
-    <row r="198" spans="1:3" ht="16" customHeight="1">
+    <row r="198" spans="1:3" ht="15.95" customHeight="1">
       <c r="A198" s="2"/>
       <c r="B198" s="3"/>
       <c r="C198" s="3"/>
     </row>
-    <row r="199" spans="1:3" ht="16" customHeight="1">
+    <row r="199" spans="1:3" ht="15.95" customHeight="1">
       <c r="A199" s="2"/>
       <c r="B199" s="3"/>
       <c r="C199" s="3"/>
     </row>
-    <row r="200" spans="1:3" ht="16" customHeight="1">
+    <row r="200" spans="1:3" ht="15.95" customHeight="1">
       <c r="A200" s="2"/>
       <c r="B200" s="3"/>
       <c r="C200" s="3"/>
     </row>
-    <row r="201" spans="1:3" ht="16" customHeight="1">
+    <row r="201" spans="1:3" ht="15.95" customHeight="1">
       <c r="A201" s="2"/>
       <c r="B201" s="3"/>
       <c r="C201" s="3"/>
     </row>
-    <row r="202" spans="1:3" ht="16" customHeight="1">
+    <row r="202" spans="1:3" ht="15.95" customHeight="1">
       <c r="A202" s="2"/>
       <c r="B202" s="3"/>
       <c r="C202" s="3"/>
     </row>
-    <row r="203" spans="1:3" ht="16" customHeight="1">
+    <row r="203" spans="1:3" ht="15.95" customHeight="1">
       <c r="A203" s="2"/>
       <c r="B203" s="3"/>
       <c r="C203" s="3"/>
     </row>
-    <row r="204" spans="1:3" ht="16" customHeight="1">
+    <row r="204" spans="1:3" ht="15.95" customHeight="1">
       <c r="A204" s="2"/>
       <c r="B204" s="3"/>
       <c r="C204" s="3"/>
     </row>
-    <row r="205" spans="1:3" ht="16" customHeight="1">
+    <row r="205" spans="1:3" ht="15.95" customHeight="1">
       <c r="A205" s="2"/>
       <c r="B205" s="3"/>
       <c r="C205" s="3"/>
     </row>
-    <row r="206" spans="1:3" ht="16" customHeight="1">
+    <row r="206" spans="1:3" ht="15.95" customHeight="1">
       <c r="A206" s="2"/>
       <c r="B206" s="3"/>
       <c r="C206" s="3"/>
     </row>
-    <row r="207" spans="1:3" ht="16" customHeight="1">
+    <row r="207" spans="1:3" ht="15.95" customHeight="1">
       <c r="A207" s="2"/>
       <c r="B207" s="3"/>
       <c r="C207" s="3"/>
     </row>
-    <row r="208" spans="1:3" ht="16" customHeight="1">
+    <row r="208" spans="1:3" ht="15.95" customHeight="1">
       <c r="A208" s="2"/>
       <c r="B208" s="3"/>
       <c r="C208" s="3"/>
     </row>
-    <row r="209" spans="1:3" ht="16" customHeight="1">
+    <row r="209" spans="1:3" ht="15.95" customHeight="1">
       <c r="A209" s="2"/>
       <c r="B209" s="3"/>
       <c r="C209" s="3"/>
     </row>
-    <row r="210" spans="1:3" ht="16" customHeight="1">
+    <row r="210" spans="1:3" ht="15.95" customHeight="1">
       <c r="A210" s="2"/>
       <c r="B210" s="3"/>
       <c r="C210" s="3"/>
     </row>
-    <row r="211" spans="1:3" ht="16" customHeight="1">
+    <row r="211" spans="1:3" ht="15.95" customHeight="1">
       <c r="A211" s="2"/>
       <c r="B211" s="3"/>
       <c r="C211" s="3"/>
     </row>
-    <row r="212" spans="1:3" ht="16" customHeight="1">
+    <row r="212" spans="1:3" ht="15.95" customHeight="1">
       <c r="A212" s="2"/>
       <c r="B212" s="3"/>
       <c r="C212" s="3"/>
     </row>
-    <row r="213" spans="1:3" ht="16" customHeight="1">
+    <row r="213" spans="1:3" ht="15.95" customHeight="1">
       <c r="A213" s="2"/>
       <c r="B213" s="3"/>
       <c r="C213" s="3"/>
     </row>
-    <row r="214" spans="1:3" ht="16" customHeight="1">
+    <row r="214" spans="1:3" ht="15.95" customHeight="1">
       <c r="A214" s="2"/>
       <c r="B214" s="3"/>
       <c r="C214" s="3"/>
     </row>
-    <row r="215" spans="1:3" ht="16" customHeight="1">
+    <row r="215" spans="1:3" ht="15.95" customHeight="1">
       <c r="A215" s="2"/>
       <c r="B215" s="3"/>
       <c r="C215" s="3"/>
     </row>
-    <row r="216" spans="1:3" ht="16" customHeight="1">
+    <row r="216" spans="1:3" ht="15.95" customHeight="1">
       <c r="A216" s="2"/>
       <c r="B216" s="3"/>
       <c r="C216" s="3"/>
     </row>
-    <row r="217" spans="1:3" ht="16" customHeight="1">
+    <row r="217" spans="1:3" ht="15.95" customHeight="1">
       <c r="A217" s="2"/>
       <c r="B217" s="3"/>
       <c r="C217" s="3"/>
     </row>
-    <row r="218" spans="1:3" ht="16" customHeight="1">
+    <row r="218" spans="1:3" ht="15.95" customHeight="1">
       <c r="A218" s="2"/>
       <c r="B218" s="3"/>
       <c r="C218" s="3"/>
     </row>
-    <row r="219" spans="1:3" ht="16" customHeight="1">
+    <row r="219" spans="1:3" ht="15.95" customHeight="1">
       <c r="A219" s="2"/>
       <c r="B219" s="3"/>
       <c r="C219" s="3"/>
     </row>
-    <row r="220" spans="1:3" ht="16" customHeight="1">
+    <row r="220" spans="1:3" ht="15.95" customHeight="1">
       <c r="A220" s="2"/>
       <c r="B220" s="3"/>
       <c r="C220" s="3"/>
     </row>
-    <row r="221" spans="1:3" ht="16" customHeight="1">
+    <row r="221" spans="1:3" ht="15.95" customHeight="1">
       <c r="A221" s="2"/>
       <c r="B221" s="3"/>
       <c r="C221" s="3"/>
     </row>
-    <row r="222" spans="1:3" ht="16" customHeight="1">
+    <row r="222" spans="1:3" ht="15.95" customHeight="1">
       <c r="A222" s="2"/>
       <c r="B222" s="3"/>
       <c r="C222" s="3"/>
     </row>
-    <row r="223" spans="1:3" ht="16" customHeight="1">
+    <row r="223" spans="1:3" ht="15.95" customHeight="1">
       <c r="A223" s="2"/>
       <c r="B223" s="3"/>
       <c r="C223" s="3"/>
     </row>
-    <row r="224" spans="1:3" ht="16" customHeight="1">
+    <row r="224" spans="1:3" ht="15.95" customHeight="1">
       <c r="A224" s="2"/>
       <c r="B224" s="3"/>
       <c r="C224" s="3"/>
     </row>
-    <row r="225" spans="1:3" ht="16" customHeight="1">
+    <row r="225" spans="1:3" ht="15.95" customHeight="1">
       <c r="A225" s="2"/>
       <c r="B225" s="3"/>
       <c r="C225" s="3"/>
     </row>
-    <row r="226" spans="1:3" ht="16" customHeight="1">
+    <row r="226" spans="1:3" ht="15.95" customHeight="1">
       <c r="A226" s="2"/>
       <c r="B226" s="3"/>
       <c r="C226" s="3"/>
     </row>
-    <row r="227" spans="1:3" ht="16" customHeight="1">
+    <row r="227" spans="1:3" ht="15.95" customHeight="1">
       <c r="A227" s="2"/>
       <c r="B227" s="3"/>
       <c r="C227" s="3"/>
     </row>
-    <row r="228" spans="1:3" ht="16" customHeight="1">
+    <row r="228" spans="1:3" ht="15.95" customHeight="1">
       <c r="A228" s="2"/>
       <c r="B228" s="3"/>
       <c r="C228" s="3"/>
     </row>
-    <row r="229" spans="1:3" ht="16" customHeight="1">
+    <row r="229" spans="1:3" ht="15.95" customHeight="1">
       <c r="A229" s="2"/>
       <c r="B229" s="3"/>
       <c r="C229" s="3"/>
     </row>
-    <row r="230" spans="1:3" ht="16" customHeight="1">
+    <row r="230" spans="1:3" ht="15.95" customHeight="1">
       <c r="A230" s="2"/>
       <c r="B230" s="3"/>
       <c r="C230" s="3"/>
     </row>
-    <row r="231" spans="1:3" ht="16" customHeight="1">
+    <row r="231" spans="1:3" ht="15.95" customHeight="1">
       <c r="A231" s="2"/>
       <c r="B231" s="3"/>
       <c r="C231" s="3"/>
     </row>
-    <row r="232" spans="1:3" ht="16" customHeight="1">
+    <row r="232" spans="1:3" ht="15.95" customHeight="1">
       <c r="A232" s="2"/>
       <c r="B232" s="3"/>
       <c r="C232" s="3"/>
     </row>
-    <row r="233" spans="1:3" ht="16" customHeight="1">
+    <row r="233" spans="1:3" ht="15.95" customHeight="1">
       <c r="A233" s="2"/>
       <c r="B233" s="3"/>
       <c r="C233" s="3"/>
     </row>
-    <row r="234" spans="1:3" ht="16" customHeight="1">
+    <row r="234" spans="1:3" ht="15.95" customHeight="1">
       <c r="A234" s="2"/>
       <c r="B234" s="3"/>
       <c r="C234" s="3"/>
     </row>
-    <row r="235" spans="1:3" ht="16" customHeight="1">
+    <row r="235" spans="1:3" ht="15.95" customHeight="1">
       <c r="A235" s="2"/>
       <c r="B235" s="3"/>
       <c r="C235" s="3"/>
     </row>
-    <row r="236" spans="1:3" ht="16" customHeight="1">
+    <row r="236" spans="1:3" ht="15.95" customHeight="1">
       <c r="A236" s="2"/>
       <c r="B236" s="3"/>
       <c r="C236" s="3"/>
     </row>
-    <row r="237" spans="1:3" ht="16" customHeight="1">
+    <row r="237" spans="1:3" ht="15.95" customHeight="1">
       <c r="A237" s="2"/>
       <c r="B237" s="3"/>
       <c r="C237" s="3"/>
     </row>
-    <row r="238" spans="1:3" ht="16" customHeight="1">
+    <row r="238" spans="1:3" ht="15.95" customHeight="1">
       <c r="A238" s="2"/>
       <c r="B238" s="3"/>
       <c r="C238" s="3"/>
     </row>
-    <row r="239" spans="1:3" ht="16" customHeight="1">
+    <row r="239" spans="1:3" ht="15.95" customHeight="1">
       <c r="A239" s="2"/>
       <c r="B239" s="3"/>
       <c r="C239" s="3"/>
     </row>
-    <row r="240" spans="1:3" ht="16" customHeight="1">
+    <row r="240" spans="1:3" ht="15.95" customHeight="1">
       <c r="A240" s="2"/>
       <c r="B240" s="3"/>
       <c r="C240" s="3"/>
     </row>
-    <row r="241" spans="1:3" ht="16" customHeight="1">
+    <row r="241" spans="1:3" ht="15.95" customHeight="1">
       <c r="A241" s="2"/>
       <c r="B241" s="3"/>
       <c r="C241" s="3"/>
     </row>
-    <row r="242" spans="1:3" ht="16" customHeight="1">
+    <row r="242" spans="1:3" ht="15.95" customHeight="1">
       <c r="A242" s="2"/>
       <c r="B242" s="3"/>
       <c r="C242" s="3"/>
     </row>
-    <row r="243" spans="1:3" ht="16" customHeight="1">
+    <row r="243" spans="1:3" ht="15.95" customHeight="1">
       <c r="A243" s="2"/>
       <c r="B243" s="3"/>
       <c r="C243" s="3"/>
     </row>
-    <row r="244" spans="1:3" ht="16" customHeight="1">
+    <row r="244" spans="1:3" ht="15.95" customHeight="1">
       <c r="A244" s="2"/>
       <c r="B244" s="3"/>
       <c r="C244" s="3"/>
     </row>
-    <row r="245" spans="1:3" ht="16" customHeight="1">
+    <row r="245" spans="1:3" ht="15.95" customHeight="1">
       <c r="A245" s="2"/>
       <c r="B245" s="3"/>
       <c r="C245" s="3"/>
     </row>
-    <row r="246" spans="1:3" ht="16" customHeight="1">
+    <row r="246" spans="1:3" ht="15.95" customHeight="1">
       <c r="A246" s="2"/>
       <c r="B246" s="3"/>
       <c r="C246" s="3"/>
     </row>
-    <row r="247" spans="1:3" ht="16" customHeight="1">
+    <row r="247" spans="1:3" ht="15.95" customHeight="1">
       <c r="A247" s="2"/>
       <c r="B247" s="3"/>
       <c r="C247" s="3"/>
     </row>
-    <row r="248" spans="1:3" ht="16" customHeight="1">
+    <row r="248" spans="1:3" ht="15.95" customHeight="1">
       <c r="A248" s="2"/>
       <c r="B248" s="3"/>
       <c r="C248" s="3"/>
     </row>
-    <row r="249" spans="1:3" ht="16" customHeight="1">
+    <row r="249" spans="1:3" ht="15.95" customHeight="1">
       <c r="A249" s="2"/>
       <c r="B249" s="3"/>
       <c r="C249" s="3"/>
     </row>
-    <row r="250" spans="1:3" ht="16" customHeight="1">
+    <row r="250" spans="1:3" ht="15.95" customHeight="1">
       <c r="A250" s="2"/>
       <c r="B250" s="3"/>
       <c r="C250" s="3"/>
     </row>
-    <row r="251" spans="1:3" ht="16" customHeight="1">
+    <row r="251" spans="1:3" ht="15.95" customHeight="1">
       <c r="A251" s="2"/>
       <c r="B251" s="3"/>
       <c r="C251" s="3"/>
     </row>
-    <row r="252" spans="1:3" ht="16" customHeight="1">
+    <row r="252" spans="1:3" ht="15.95" customHeight="1">
       <c r="A252" s="2"/>
       <c r="B252" s="3"/>
       <c r="C252" s="3"/>
     </row>
-    <row r="253" spans="1:3" ht="16" customHeight="1">
+    <row r="253" spans="1:3" ht="15.95" customHeight="1">
       <c r="A253" s="2"/>
       <c r="B253" s="3"/>
       <c r="C253" s="3"/>
     </row>
-    <row r="254" spans="1:3" ht="16" customHeight="1">
+    <row r="254" spans="1:3" ht="15.95" customHeight="1">
       <c r="A254" s="2"/>
       <c r="B254" s="3"/>
       <c r="C254" s="3"/>
     </row>
-    <row r="255" spans="1:3" ht="16" customHeight="1">
+    <row r="255" spans="1:3" ht="15.95" customHeight="1">
       <c r="A255" s="2"/>
       <c r="B255" s="3"/>
       <c r="C255" s="3"/>
     </row>
-    <row r="256" spans="1:3" ht="16" customHeight="1">
+    <row r="256" spans="1:3" ht="15.95" customHeight="1">
       <c r="A256" s="2"/>
       <c r="B256" s="3"/>
       <c r="C256" s="3"/>
     </row>
-    <row r="257" spans="1:3" ht="16" customHeight="1">
+    <row r="257" spans="1:3" ht="15.95" customHeight="1">
       <c r="A257" s="2"/>
       <c r="B257" s="3"/>
       <c r="C257" s="3"/>
     </row>
-    <row r="258" spans="1:3" ht="16" customHeight="1">
+    <row r="258" spans="1:3" ht="15.95" customHeight="1">
       <c r="A258" s="2"/>
       <c r="B258" s="3"/>
       <c r="C258" s="3"/>
     </row>
-    <row r="259" spans="1:3" ht="16" customHeight="1">
+    <row r="259" spans="1:3" ht="15.95" customHeight="1">
       <c r="A259" s="2"/>
       <c r="B259" s="3"/>
       <c r="C259" s="3"/>
     </row>
-    <row r="260" spans="1:3" ht="16" customHeight="1">
+    <row r="260" spans="1:3" ht="15.95" customHeight="1">
       <c r="A260" s="2"/>
       <c r="B260" s="3"/>
       <c r="C260" s="3"/>
     </row>
-    <row r="261" spans="1:3" ht="16" customHeight="1">
+    <row r="261" spans="1:3" ht="15.95" customHeight="1">
       <c r="A261" s="2"/>
       <c r="B261" s="3"/>
       <c r="C261" s="3"/>
     </row>
-    <row r="262" spans="1:3" ht="16" customHeight="1">
+    <row r="262" spans="1:3" ht="15.95" customHeight="1">
       <c r="A262" s="2"/>
       <c r="B262" s="3"/>
       <c r="C262" s="3"/>
     </row>
-    <row r="263" spans="1:3" ht="16" customHeight="1">
+    <row r="263" spans="1:3" ht="15.95" customHeight="1">
       <c r="A263" s="2"/>
       <c r="B263" s="3"/>
       <c r="C263" s="3"/>
     </row>
-    <row r="264" spans="1:3" ht="16" customHeight="1">
+    <row r="264" spans="1:3" ht="15.95" customHeight="1">
       <c r="A264" s="2"/>
       <c r="B264" s="3"/>
       <c r="C264" s="3"/>
     </row>
-    <row r="265" spans="1:3" ht="16" customHeight="1">
+    <row r="265" spans="1:3" ht="15.95" customHeight="1">
       <c r="A265" s="2"/>
       <c r="B265" s="3"/>
       <c r="C265" s="3"/>
     </row>
-    <row r="266" spans="1:3" ht="16" customHeight="1">
+    <row r="266" spans="1:3" ht="15.95" customHeight="1">
       <c r="A266" s="2"/>
       <c r="B266" s="3"/>
       <c r="C266" s="3"/>
     </row>
-    <row r="267" spans="1:3" ht="16" customHeight="1">
+    <row r="267" spans="1:3" ht="15.95" customHeight="1">
       <c r="A267" s="2"/>
       <c r="B267" s="3"/>
       <c r="C267" s="3"/>
     </row>
-    <row r="268" spans="1:3" ht="16" customHeight="1">
+    <row r="268" spans="1:3" ht="15.95" customHeight="1">
       <c r="A268" s="2"/>
       <c r="B268" s="3"/>
       <c r="C268" s="3"/>
     </row>
-    <row r="269" spans="1:3" ht="16" customHeight="1">
+    <row r="269" spans="1:3" ht="15.95" customHeight="1">
       <c r="A269" s="2"/>
       <c r="B269" s="3"/>
       <c r="C269" s="3"/>
     </row>
-    <row r="270" spans="1:3" ht="16" customHeight="1">
+    <row r="270" spans="1:3" ht="15.95" customHeight="1">
       <c r="A270" s="2"/>
       <c r="B270" s="3"/>
       <c r="C270" s="3"/>
     </row>
-    <row r="271" spans="1:3" ht="16" customHeight="1">
+    <row r="271" spans="1:3" ht="15.95" customHeight="1">
       <c r="A271" s="2"/>
       <c r="B271" s="3"/>
       <c r="C271" s="3"/>
     </row>
-    <row r="272" spans="1:3" ht="16" customHeight="1">
+    <row r="272" spans="1:3" ht="15.95" customHeight="1">
       <c r="A272" s="2"/>
       <c r="B272" s="3"/>
       <c r="C272" s="3"/>
     </row>
-    <row r="273" spans="1:3" ht="16" customHeight="1">
+    <row r="273" spans="1:3" ht="15.95" customHeight="1">
       <c r="A273" s="2"/>
       <c r="B273" s="3"/>
       <c r="C273" s="3"/>
     </row>
-    <row r="274" spans="1:3" ht="16" customHeight="1">
+    <row r="274" spans="1:3" ht="15.95" customHeight="1">
       <c r="A274" s="2"/>
       <c r="B274" s="3"/>
       <c r="C274" s="3"/>
     </row>
-    <row r="275" spans="1:3" ht="16" customHeight="1">
+    <row r="275" spans="1:3" ht="15.95" customHeight="1">
       <c r="A275" s="2"/>
       <c r="B275" s="3"/>
       <c r="C275" s="3"/>
     </row>
-    <row r="276" spans="1:3" ht="16" customHeight="1">
+    <row r="276" spans="1:3" ht="15.95" customHeight="1">
       <c r="A276" s="2"/>
       <c r="B276" s="3"/>
       <c r="C276" s="3"/>
     </row>
-    <row r="277" spans="1:3" ht="16" customHeight="1">
+    <row r="277" spans="1:3" ht="15.95" customHeight="1">
       <c r="A277" s="2"/>
       <c r="B277" s="3"/>
       <c r="C277" s="3"/>
     </row>
-    <row r="278" spans="1:3" ht="16" customHeight="1">
+    <row r="278" spans="1:3" ht="15.95" customHeight="1">
       <c r="A278" s="2"/>
       <c r="B278" s="3"/>
       <c r="C278" s="3"/>
     </row>
-    <row r="279" spans="1:3" ht="16" customHeight="1">
+    <row r="279" spans="1:3" ht="15.95" customHeight="1">
       <c r="A279" s="2"/>
       <c r="B279" s="3"/>
       <c r="C279" s="3"/>
     </row>
-    <row r="280" spans="1:3" ht="16" customHeight="1">
+    <row r="280" spans="1:3" ht="15.95" customHeight="1">
       <c r="A280" s="2"/>
       <c r="B280" s="3"/>
       <c r="C280" s="3"/>
     </row>
-    <row r="281" spans="1:3" ht="16" customHeight="1">
+    <row r="281" spans="1:3" ht="15.95" customHeight="1">
       <c r="A281" s="2"/>
       <c r="B281" s="3"/>
       <c r="C281" s="3"/>
     </row>
-    <row r="282" spans="1:3" ht="16" customHeight="1">
+    <row r="282" spans="1:3" ht="15.95" customHeight="1">
       <c r="A282" s="2"/>
       <c r="B282" s="3"/>
       <c r="C282" s="3"/>
     </row>
-    <row r="283" spans="1:3" ht="16" customHeight="1">
+    <row r="283" spans="1:3" ht="15.95" customHeight="1">
       <c r="A283" s="2"/>
       <c r="B283" s="3"/>
       <c r="C283" s="3"/>
     </row>
-    <row r="284" spans="1:3" ht="16" customHeight="1">
+    <row r="284" spans="1:3" ht="15.95" customHeight="1">
       <c r="A284" s="2"/>
       <c r="B284" s="3"/>
       <c r="C284" s="3"/>
     </row>
-    <row r="285" spans="1:3" ht="16" customHeight="1">
+    <row r="285" spans="1:3" ht="15.95" customHeight="1">
       <c r="A285" s="2"/>
       <c r="B285" s="3"/>
       <c r="C285" s="3"/>
     </row>
-    <row r="286" spans="1:3" ht="16" customHeight="1">
+    <row r="286" spans="1:3" ht="15.95" customHeight="1">
       <c r="A286" s="2"/>
       <c r="B286" s="3"/>
       <c r="C286" s="3"/>
     </row>
-    <row r="287" spans="1:3" ht="16" customHeight="1">
+    <row r="287" spans="1:3" ht="15.95" customHeight="1">
       <c r="A287" s="2"/>
       <c r="B287" s="3"/>
       <c r="C287" s="3"/>
     </row>
-    <row r="288" spans="1:3" ht="16" customHeight="1">
+    <row r="288" spans="1:3" ht="15.95" customHeight="1">
       <c r="A288" s="2"/>
       <c r="B288" s="3"/>
       <c r="C288" s="3"/>
     </row>
-    <row r="289" spans="1:3" ht="16" customHeight="1">
+    <row r="289" spans="1:3" ht="15.95" customHeight="1">
       <c r="A289" s="2"/>
       <c r="B289" s="3"/>
       <c r="C289" s="3"/>
     </row>
-    <row r="290" spans="1:3" ht="16" customHeight="1">
+    <row r="290" spans="1:3" ht="15.95" customHeight="1">
       <c r="A290" s="2"/>
       <c r="B290" s="3"/>
       <c r="C290" s="3"/>
     </row>
-    <row r="291" spans="1:3" ht="16" customHeight="1">
+    <row r="291" spans="1:3" ht="15.95" customHeight="1">
       <c r="A291" s="2"/>
       <c r="B291" s="3"/>
       <c r="C291" s="3"/>
     </row>
-    <row r="292" spans="1:3" ht="16" customHeight="1">
+    <row r="292" spans="1:3" ht="15.95" customHeight="1">
       <c r="A292" s="2"/>
       <c r="B292" s="3"/>
       <c r="C292" s="3"/>
     </row>
-    <row r="293" spans="1:3" ht="16" customHeight="1">
+    <row r="293" spans="1:3" ht="15.95" customHeight="1">
       <c r="A293" s="2"/>
       <c r="B293" s="3"/>
       <c r="C293" s="3"/>
     </row>
-    <row r="294" spans="1:3" ht="16" customHeight="1">
+    <row r="294" spans="1:3" ht="15.95" customHeight="1">
       <c r="A294" s="2"/>
       <c r="B294" s="3"/>
       <c r="C294" s="3"/>
     </row>
-    <row r="295" spans="1:3" ht="16" customHeight="1">
+    <row r="295" spans="1:3" ht="15.95" customHeight="1">
       <c r="A295" s="2"/>
       <c r="B295" s="3"/>
       <c r="C295" s="3"/>
     </row>
-    <row r="296" spans="1:3" ht="16" customHeight="1">
+    <row r="296" spans="1:3" ht="15.95" customHeight="1">
       <c r="A296" s="2"/>
       <c r="B296" s="3"/>
       <c r="C296" s="3"/>
     </row>
-    <row r="297" spans="1:3" ht="16" customHeight="1">
+    <row r="297" spans="1:3" ht="15.95" customHeight="1">
       <c r="A297" s="2"/>
       <c r="B297" s="3"/>
       <c r="C297" s="3"/>
     </row>
-    <row r="298" spans="1:3" ht="16" customHeight="1">
+    <row r="298" spans="1:3" ht="15.95" customHeight="1">
       <c r="A298" s="2"/>
       <c r="B298" s="3"/>
       <c r="C298" s="3"/>
     </row>
-    <row r="299" spans="1:3" ht="16" customHeight="1">
+    <row r="299" spans="1:3" ht="15.95" customHeight="1">
       <c r="A299" s="2"/>
       <c r="B299" s="3"/>
       <c r="C299" s="3"/>
     </row>
-    <row r="300" spans="1:3" ht="16" customHeight="1">
+    <row r="300" spans="1:3" ht="15.95" customHeight="1">
       <c r="A300" s="2"/>
       <c r="B300" s="3"/>
       <c r="C300" s="3"/>
     </row>
-    <row r="301" spans="1:3" ht="16" customHeight="1">
+    <row r="301" spans="1:3" ht="15.95" customHeight="1">
       <c r="A301" s="2"/>
       <c r="B301" s="3"/>
       <c r="C301" s="3"/>
     </row>
-    <row r="302" spans="1:3" ht="16" customHeight="1">
+    <row r="302" spans="1:3" ht="15.95" customHeight="1">
       <c r="A302" s="2"/>
       <c r="B302" s="3"/>
       <c r="C302" s="3"/>
     </row>
-    <row r="303" spans="1:3" ht="16" customHeight="1">
+    <row r="303" spans="1:3" ht="15.95" customHeight="1">
       <c r="A303" s="2"/>
       <c r="B303" s="3"/>
       <c r="C303" s="3"/>
     </row>
-    <row r="304" spans="1:3" ht="16" customHeight="1">
+    <row r="304" spans="1:3" ht="15.95" customHeight="1">
       <c r="A304" s="2"/>
       <c r="B304" s="3"/>
       <c r="C304" s="3"/>
     </row>
-    <row r="305" spans="1:3" ht="16" customHeight="1">
+    <row r="305" spans="1:3" ht="15.95" customHeight="1">
       <c r="A305" s="2"/>
       <c r="B305" s="3"/>
       <c r="C305" s="3"/>
     </row>
-    <row r="306" spans="1:3" ht="16" customHeight="1">
+    <row r="306" spans="1:3" ht="15.95" customHeight="1">
       <c r="A306" s="2"/>
       <c r="B306" s="3"/>
       <c r="C306" s="3"/>
     </row>
-    <row r="307" spans="1:3" ht="16" customHeight="1">
+    <row r="307" spans="1:3" ht="15.95" customHeight="1">
       <c r="A307" s="2"/>
       <c r="B307" s="3"/>
       <c r="C307" s="3"/>
     </row>
-    <row r="308" spans="1:3" ht="16" customHeight="1">
+    <row r="308" spans="1:3" ht="15.95" customHeight="1">
       <c r="A308" s="2"/>
       <c r="B308" s="3"/>
       <c r="C308" s="3"/>
     </row>
-    <row r="309" spans="1:3" ht="16" customHeight="1">
+    <row r="309" spans="1:3" ht="15.95" customHeight="1">
       <c r="A309" s="2"/>
       <c r="B309" s="3"/>
       <c r="C309" s="3"/>
     </row>
-    <row r="310" spans="1:3" ht="16" customHeight="1">
+    <row r="310" spans="1:3" ht="15.95" customHeight="1">
       <c r="A310" s="2"/>
       <c r="B310" s="3"/>
       <c r="C310" s="3"/>
     </row>
-    <row r="311" spans="1:3" ht="16" customHeight="1">
+    <row r="311" spans="1:3" ht="15.95" customHeight="1">
       <c r="A311" s="2"/>
       <c r="B311" s="3"/>
       <c r="C311" s="3"/>
     </row>
-    <row r="312" spans="1:3" ht="16" customHeight="1">
+    <row r="312" spans="1:3" ht="15.95" customHeight="1">
       <c r="A312" s="2"/>
       <c r="B312" s="3"/>
       <c r="C312" s="3"/>
     </row>
-    <row r="313" spans="1:3" ht="16" customHeight="1">
+    <row r="313" spans="1:3" ht="15.95" customHeight="1">
       <c r="A313" s="2"/>
       <c r="B313" s="3"/>
       <c r="C313" s="3"/>
     </row>
-    <row r="314" spans="1:3" ht="16" customHeight="1">
+    <row r="314" spans="1:3" ht="15.95" customHeight="1">
       <c r="A314" s="2"/>
       <c r="B314" s="3"/>
       <c r="C314" s="3"/>
     </row>
-    <row r="315" spans="1:3" ht="16" customHeight="1">
+    <row r="315" spans="1:3" ht="15.95" customHeight="1">
       <c r="A315" s="2"/>
       <c r="B315" s="3"/>
       <c r="C315" s="3"/>
     </row>
-    <row r="316" spans="1:3" ht="16" customHeight="1">
+    <row r="316" spans="1:3" ht="15.95" customHeight="1">
       <c r="A316" s="2"/>
       <c r="B316" s="3"/>
       <c r="C316" s="3"/>
     </row>
-    <row r="317" spans="1:3" ht="16" customHeight="1">
+    <row r="317" spans="1:3" ht="15.95" customHeight="1">
       <c r="A317" s="2"/>
       <c r="B317" s="3"/>
       <c r="C317" s="3"/>
     </row>
-    <row r="318" spans="1:3" ht="16" customHeight="1">
+    <row r="318" spans="1:3" ht="15.95" customHeight="1">
       <c r="A318" s="2"/>
       <c r="B318" s="3"/>
       <c r="C318" s="3"/>
     </row>
-    <row r="319" spans="1:3" ht="16" customHeight="1">
+    <row r="319" spans="1:3" ht="15.95" customHeight="1">
       <c r="A319" s="2"/>
       <c r="B319" s="3"/>
       <c r="C319" s="3"/>
     </row>
-    <row r="320" spans="1:3" ht="16" customHeight="1">
+    <row r="320" spans="1:3" ht="15.95" customHeight="1">
       <c r="A320" s="2"/>
       <c r="B320" s="3"/>
       <c r="C320" s="3"/>
     </row>
-    <row r="321" spans="1:3" ht="16" customHeight="1">
+    <row r="321" spans="1:3" ht="15.95" customHeight="1">
       <c r="A321" s="2"/>
       <c r="B321" s="3"/>
       <c r="C321" s="3"/>
     </row>
-    <row r="322" spans="1:3" ht="16" customHeight="1">
+    <row r="322" spans="1:3" ht="15.95" customHeight="1">
       <c r="A322" s="2"/>
       <c r="B322" s="3"/>
       <c r="C322" s="3"/>
     </row>
-    <row r="323" spans="1:3" ht="16" customHeight="1">
+    <row r="323" spans="1:3" ht="15.95" customHeight="1">
       <c r="A323" s="2"/>
       <c r="B323" s="3"/>
       <c r="C323" s="3"/>
     </row>
-    <row r="324" spans="1:3" ht="16" customHeight="1">
+    <row r="324" spans="1:3" ht="15.95" customHeight="1">
       <c r="A324" s="2"/>
       <c r="B324" s="3"/>
       <c r="C324" s="3"/>
     </row>
-    <row r="325" spans="1:3" ht="16" customHeight="1">
+    <row r="325" spans="1:3" ht="15.95" customHeight="1">
       <c r="A325" s="2"/>
       <c r="B325" s="3"/>
       <c r="C325" s="3"/>
     </row>
-    <row r="326" spans="1:3" ht="16" customHeight="1">
+    <row r="326" spans="1:3" ht="15.95" customHeight="1">
       <c r="A326" s="2"/>
       <c r="B326" s="3"/>
       <c r="C326" s="3"/>
     </row>
-    <row r="327" spans="1:3" ht="16" customHeight="1">
+    <row r="327" spans="1:3" ht="15.95" customHeight="1">
       <c r="A327" s="2"/>
       <c r="B327" s="3"/>
       <c r="C327" s="3"/>
     </row>
-    <row r="328" spans="1:3" ht="16" customHeight="1">
+    <row r="328" spans="1:3" ht="15.95" customHeight="1">
       <c r="A328" s="2"/>
       <c r="B328" s="3"/>
       <c r="C328" s="3"/>
     </row>
-    <row r="329" spans="1:3" ht="16" customHeight="1">
+    <row r="329" spans="1:3" ht="15.95" customHeight="1">
       <c r="A329" s="2"/>
       <c r="B329" s="3"/>
       <c r="C329" s="3"/>
     </row>
-    <row r="330" spans="1:3" ht="16" customHeight="1">
+    <row r="330" spans="1:3" ht="15.95" customHeight="1">
       <c r="A330" s="2"/>
       <c r="B330" s="3"/>
       <c r="C330" s="3"/>
     </row>
-    <row r="331" spans="1:3" ht="16" customHeight="1">
+    <row r="331" spans="1:3" ht="15.95" customHeight="1">
       <c r="A331" s="2"/>
       <c r="B331" s="3"/>
       <c r="C331" s="3"/>
     </row>
-    <row r="332" spans="1:3" ht="16" customHeight="1">
+    <row r="332" spans="1:3" ht="15.95" customHeight="1">
       <c r="A332" s="2"/>
       <c r="B332" s="3"/>
       <c r="C332" s="3"/>
     </row>
-    <row r="333" spans="1:3" ht="16" customHeight="1">
+    <row r="333" spans="1:3" ht="15.95" customHeight="1">
       <c r="A333" s="2"/>
       <c r="B333" s="3"/>
       <c r="C333" s="3"/>
     </row>
-    <row r="334" spans="1:3" ht="16" customHeight="1">
+    <row r="334" spans="1:3" ht="15.95" customHeight="1">
       <c r="A334" s="2"/>
       <c r="B334" s="3"/>
       <c r="C334" s="3"/>
     </row>
-    <row r="335" spans="1:3" ht="16" customHeight="1">
+    <row r="335" spans="1:3" ht="15.95" customHeight="1">
       <c r="A335" s="2"/>
       <c r="B335" s="3"/>
       <c r="C335" s="3"/>
     </row>
-    <row r="336" spans="1:3" ht="16" customHeight="1">
+    <row r="336" spans="1:3" ht="15.95" customHeight="1">
       <c r="A336" s="2"/>
       <c r="B336" s="3"/>
       <c r="C336" s="3"/>
     </row>
-    <row r="337" spans="1:3" ht="16" customHeight="1">
+    <row r="337" spans="1:3" ht="15.95" customHeight="1">
       <c r="A337" s="2"/>
       <c r="B337" s="3"/>
       <c r="C337" s="3"/>
     </row>
-    <row r="338" spans="1:3" ht="16" customHeight="1">
+    <row r="338" spans="1:3" ht="15.95" customHeight="1">
       <c r="A338" s="2"/>
       <c r="B338" s="3"/>
       <c r="C338" s="3"/>
     </row>
-    <row r="339" spans="1:3" ht="16" customHeight="1">
+    <row r="339" spans="1:3" ht="15.95" customHeight="1">
       <c r="A339" s="2"/>
       <c r="B339" s="3"/>
       <c r="C339" s="3"/>
     </row>
-    <row r="340" spans="1:3" ht="16" customHeight="1">
+    <row r="340" spans="1:3" ht="15.95" customHeight="1">
       <c r="A340" s="2"/>
       <c r="B340" s="3"/>
       <c r="C340" s="3"/>
     </row>
-    <row r="341" spans="1:3" ht="16" customHeight="1">
+    <row r="341" spans="1:3" ht="15.95" customHeight="1">
       <c r="A341" s="2"/>
       <c r="B341" s="3"/>
       <c r="C341" s="3"/>
     </row>
-    <row r="342" spans="1:3" ht="16" customHeight="1">
+    <row r="342" spans="1:3" ht="15.95" customHeight="1">
       <c r="A342" s="2"/>
       <c r="B342" s="3"/>
       <c r="C342" s="3"/>
     </row>
-    <row r="343" spans="1:3" ht="16" customHeight="1">
+    <row r="343" spans="1:3" ht="15.95" customHeight="1">
       <c r="A343" s="2"/>
       <c r="B343" s="3"/>
       <c r="C343" s="3"/>
     </row>
-    <row r="344" spans="1:3" ht="16" customHeight="1">
+    <row r="344" spans="1:3" ht="15.95" customHeight="1">
       <c r="A344" s="2"/>
       <c r="B344" s="3"/>
       <c r="C344" s="3"/>
     </row>
-    <row r="345" spans="1:3" ht="16" customHeight="1">
+    <row r="345" spans="1:3" ht="15.95" customHeight="1">
       <c r="A345" s="2"/>
       <c r="B345" s="3"/>
       <c r="C345" s="3"/>
     </row>
-    <row r="346" spans="1:3" ht="16" customHeight="1">
+    <row r="346" spans="1:3" ht="15.95" customHeight="1">
       <c r="A346" s="2"/>
       <c r="B346" s="3"/>
       <c r="C346" s="3"/>
     </row>
-    <row r="347" spans="1:3" ht="16" customHeight="1">
+    <row r="347" spans="1:3" ht="15.95" customHeight="1">
       <c r="A347" s="2"/>
       <c r="B347" s="3"/>
       <c r="C347" s="3"/>
     </row>
-    <row r="348" spans="1:3" ht="16" customHeight="1">
+    <row r="348" spans="1:3" ht="15.95" customHeight="1">
       <c r="A348" s="2"/>
       <c r="B348" s="3"/>
       <c r="C348" s="3"/>
     </row>
-    <row r="349" spans="1:3" ht="16" customHeight="1">
+    <row r="349" spans="1:3" ht="15.95" customHeight="1">
       <c r="A349" s="2"/>
       <c r="B349" s="3"/>
       <c r="C349" s="3"/>
     </row>
-    <row r="350" spans="1:3" ht="16" customHeight="1">
+    <row r="350" spans="1:3" ht="15.95" customHeight="1">
       <c r="A350" s="2"/>
       <c r="B350" s="3"/>
       <c r="C350" s="3"/>
     </row>
-    <row r="351" spans="1:3" ht="16" customHeight="1">
+    <row r="351" spans="1:3" ht="15.95" customHeight="1">
       <c r="A351" s="2"/>
       <c r="B351" s="3"/>
       <c r="C351" s="3"/>
     </row>
-    <row r="352" spans="1:3" ht="14" customHeight="1">
+    <row r="352" spans="1:3" ht="14.1" customHeight="1">
       <c r="A352" s="4"/>
     </row>
   </sheetData>
@@ -3147,35 +3156,35 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:S20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="18.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="12.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="31.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="38.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="18.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="31.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="38.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="30" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="27.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="28.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="18" width="11.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="22.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="16384" width="8.83203125" style="1"/>
+    <col min="15" max="15" width="27.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="28.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="18" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="22.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="14" customHeight="1">
+    <row r="1" spans="1:19" ht="14.1" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>53</v>
       </c>
@@ -3234,7 +3243,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:19" ht="16" customHeight="1">
+    <row r="2" spans="1:19" ht="15.95" customHeight="1">
       <c r="A2" s="2">
         <v>1000121</v>
       </c>
@@ -3293,7 +3302,7 @@
         <v>854.88</v>
       </c>
     </row>
-    <row r="3" spans="1:19" ht="16" customHeight="1">
+    <row r="3" spans="1:19" ht="15.95" customHeight="1">
       <c r="A3" s="2">
         <v>1000122</v>
       </c>
@@ -3352,7 +3361,7 @@
         <v>4346.07</v>
       </c>
     </row>
-    <row r="4" spans="1:19" ht="16" customHeight="1">
+    <row r="4" spans="1:19" ht="15.95" customHeight="1">
       <c r="A4" s="2">
         <v>1000123</v>
       </c>
@@ -3411,7 +3420,7 @@
         <v>15355.88</v>
       </c>
     </row>
-    <row r="5" spans="1:19" ht="16" customHeight="1">
+    <row r="5" spans="1:19" ht="15.95" customHeight="1">
       <c r="A5" s="2">
         <v>1000124</v>
       </c>
@@ -3470,7 +3479,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:19" ht="16" customHeight="1">
+    <row r="6" spans="1:19" ht="15.95" customHeight="1">
       <c r="A6" s="2">
         <v>1000125</v>
       </c>
@@ -3529,7 +3538,7 @@
         <v>182.58</v>
       </c>
     </row>
-    <row r="7" spans="1:19" ht="16" customHeight="1">
+    <row r="7" spans="1:19" ht="15.95" customHeight="1">
       <c r="A7" s="2">
         <v>1000126</v>
       </c>
@@ -3588,7 +3597,7 @@
         <v>405.46</v>
       </c>
     </row>
-    <row r="8" spans="1:19" ht="16" customHeight="1">
+    <row r="8" spans="1:19" ht="15.95" customHeight="1">
       <c r="A8" s="2">
         <v>1000127</v>
       </c>
@@ -3647,7 +3656,7 @@
         <v>935.81</v>
       </c>
     </row>
-    <row r="9" spans="1:19" ht="16" customHeight="1">
+    <row r="9" spans="1:19" ht="15.95" customHeight="1">
       <c r="A9" s="2">
         <v>1000128</v>
       </c>
@@ -3706,7 +3715,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:19" ht="16" customHeight="1">
+    <row r="10" spans="1:19" ht="15.95" customHeight="1">
       <c r="A10" s="2">
         <v>1000129</v>
       </c>
@@ -3765,7 +3774,7 @@
         <v>163.47999999999999</v>
       </c>
     </row>
-    <row r="11" spans="1:19" ht="16" customHeight="1">
+    <row r="11" spans="1:19" ht="15.95" customHeight="1">
       <c r="A11" s="2">
         <v>1000130</v>
       </c>
@@ -3824,7 +3833,7 @@
         <v>924.71</v>
       </c>
     </row>
-    <row r="12" spans="1:19" ht="16" customHeight="1">
+    <row r="12" spans="1:19" ht="15.95" customHeight="1">
       <c r="A12" s="2">
         <v>1000131</v>
       </c>
@@ -3883,7 +3892,7 @@
         <v>794.82</v>
       </c>
     </row>
-    <row r="13" spans="1:19" ht="16" customHeight="1">
+    <row r="13" spans="1:19" ht="15.95" customHeight="1">
       <c r="A13" s="2">
         <v>1000132</v>
       </c>
@@ -3942,7 +3951,7 @@
         <v>41.74</v>
       </c>
     </row>
-    <row r="14" spans="1:19" ht="16" customHeight="1">
+    <row r="14" spans="1:19" ht="15.95" customHeight="1">
       <c r="A14" s="2">
         <v>1000133</v>
       </c>
@@ -4001,7 +4010,7 @@
         <v>196.24</v>
       </c>
     </row>
-    <row r="15" spans="1:19" ht="16" customHeight="1">
+    <row r="15" spans="1:19" ht="15.95" customHeight="1">
       <c r="A15" s="2">
         <v>1000134</v>
       </c>
@@ -4060,7 +4069,7 @@
         <v>65.25</v>
       </c>
     </row>
-    <row r="16" spans="1:19" ht="16" customHeight="1">
+    <row r="16" spans="1:19" ht="15.95" customHeight="1">
       <c r="A16" s="2">
         <v>1000135</v>
       </c>
@@ -4119,7 +4128,7 @@
         <v>128.57</v>
       </c>
     </row>
-    <row r="17" spans="1:19" ht="16" customHeight="1">
+    <row r="17" spans="1:19" ht="15.95" customHeight="1">
       <c r="A17" s="2">
         <v>1000136</v>
       </c>
@@ -4178,7 +4187,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:19" ht="16" customHeight="1">
+    <row r="18" spans="1:19" ht="15.95" customHeight="1">
       <c r="A18" s="2">
         <v>1000137</v>
       </c>
@@ -4237,7 +4246,7 @@
         <v>121.37</v>
       </c>
     </row>
-    <row r="19" spans="1:19" ht="16" customHeight="1">
+    <row r="19" spans="1:19" ht="15.95" customHeight="1">
       <c r="A19" s="2">
         <v>1000138</v>
       </c>
@@ -4296,7 +4305,7 @@
         <v>47.19</v>
       </c>
     </row>
-    <row r="20" spans="1:19" ht="16" customHeight="1">
+    <row r="20" spans="1:19" ht="15.95" customHeight="1">
       <c r="A20" s="2">
         <v>1000139</v>
       </c>
@@ -4368,27 +4377,27 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.33203125" style="1" customWidth="1"/>
-    <col min="3" max="4" width="11.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.83203125" style="1"/>
+    <col min="1" max="1" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.28515625" style="1" customWidth="1"/>
+    <col min="3" max="4" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="14" customHeight="1">
+    <row r="1" spans="1:4" ht="14.1" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>53</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="C1" s="5" t="s">
         <v>54</v>
@@ -4397,7 +4406,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="16" customHeight="1">
+    <row r="2" spans="1:4" ht="15.95" customHeight="1">
       <c r="A2" s="2">
         <v>1000121</v>
       </c>
@@ -4411,7 +4420,7 @@
         <v>26.8</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="16" customHeight="1">
+    <row r="3" spans="1:4" ht="15.95" customHeight="1">
       <c r="A3" s="2">
         <v>1000122</v>
       </c>
@@ -4425,7 +4434,7 @@
         <v>32.4</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="16" customHeight="1">
+    <row r="4" spans="1:4" ht="15.95" customHeight="1">
       <c r="A4" s="2">
         <v>1000123</v>
       </c>
@@ -4439,7 +4448,7 @@
         <v>33.4</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="16" customHeight="1">
+    <row r="5" spans="1:4" ht="15.95" customHeight="1">
       <c r="A5" s="2">
         <v>1000124</v>
       </c>
@@ -4453,7 +4462,7 @@
         <v>29.7</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="16" customHeight="1">
+    <row r="6" spans="1:4" ht="15.95" customHeight="1">
       <c r="A6" s="2">
         <v>1000125</v>
       </c>
@@ -4467,7 +4476,7 @@
         <v>22.7</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="16" customHeight="1">
+    <row r="7" spans="1:4" ht="15.95" customHeight="1">
       <c r="A7" s="2">
         <v>1000126</v>
       </c>
@@ -4481,7 +4490,7 @@
         <v>26.4</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="16" customHeight="1">
+    <row r="8" spans="1:4" ht="15.95" customHeight="1">
       <c r="A8" s="2">
         <v>1000127</v>
       </c>
@@ -4495,7 +4504,7 @@
         <v>24.9</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="16" customHeight="1">
+    <row r="9" spans="1:4" ht="15.95" customHeight="1">
       <c r="A9" s="2">
         <v>1000128</v>
       </c>
@@ -4509,7 +4518,7 @@
         <v>22.4</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="16" customHeight="1">
+    <row r="10" spans="1:4" ht="15.95" customHeight="1">
       <c r="A10" s="2">
         <v>1000129</v>
       </c>
@@ -4523,7 +4532,7 @@
         <v>28.6</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="16" customHeight="1">
+    <row r="11" spans="1:4" ht="15.95" customHeight="1">
       <c r="A11" s="2">
         <v>1000130</v>
       </c>
@@ -4537,7 +4546,7 @@
         <v>21.4</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="16" customHeight="1">
+    <row r="12" spans="1:4" ht="15.95" customHeight="1">
       <c r="A12" s="2">
         <v>1000131</v>
       </c>
@@ -4551,7 +4560,7 @@
         <v>20.7</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="16" customHeight="1">
+    <row r="13" spans="1:4" ht="15.95" customHeight="1">
       <c r="A13" s="2">
         <v>1000132</v>
       </c>
@@ -4565,7 +4574,7 @@
         <v>29.4</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="16" customHeight="1">
+    <row r="14" spans="1:4" ht="15.95" customHeight="1">
       <c r="A14" s="2">
         <v>1000133</v>
       </c>
@@ -4579,7 +4588,7 @@
         <v>28.7</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="16" customHeight="1">
+    <row r="15" spans="1:4" ht="15.95" customHeight="1">
       <c r="A15" s="2">
         <v>1000134</v>
       </c>
@@ -4593,7 +4602,7 @@
         <v>26.8</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="16" customHeight="1">
+    <row r="16" spans="1:4" ht="15.95" customHeight="1">
       <c r="A16" s="2">
         <v>1000135</v>
       </c>
@@ -4607,7 +4616,7 @@
         <v>27.3</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="16" customHeight="1">
+    <row r="17" spans="1:4" ht="15.95" customHeight="1">
       <c r="A17" s="2">
         <v>1000136</v>
       </c>
@@ -4621,7 +4630,7 @@
         <v>22.4</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="16" customHeight="1">
+    <row r="18" spans="1:4" ht="15.95" customHeight="1">
       <c r="A18" s="2">
         <v>1000137</v>
       </c>
@@ -4635,7 +4644,7 @@
         <v>21.6</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="16" customHeight="1">
+    <row r="19" spans="1:4" ht="15.95" customHeight="1">
       <c r="A19" s="2">
         <v>1000138</v>
       </c>
@@ -4649,7 +4658,7 @@
         <v>23.4</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="16" customHeight="1">
+    <row r="20" spans="1:4" ht="15.95" customHeight="1">
       <c r="A20" s="2">
         <v>1000139</v>
       </c>
@@ -4676,19 +4685,19 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26.1640625" customWidth="1"/>
-    <col min="2" max="2" width="51.1640625" customWidth="1"/>
-    <col min="3" max="3" width="28.6640625" customWidth="1"/>
-    <col min="4" max="4" width="52.5" customWidth="1"/>
+    <col min="1" max="1" width="26.140625" customWidth="1"/>
+    <col min="2" max="2" width="51.140625" customWidth="1"/>
+    <col min="3" max="3" width="28.7109375" customWidth="1"/>
+    <col min="4" max="4" width="57.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -4705,68 +4714,74 @@
         <v>59</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" ht="16.5" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>60</v>
+        <v>76</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>62</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="2" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>65</v>
+        <v>81</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="2" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>67</v>
+        <v>84</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>68</v>
+        <v>82</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="2" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>69</v>
+        <v>83</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>82</v>
+        <v>63</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>79</v>
+        <v>86</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="B6" s="13" t="s">
         <v>85</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>85</v>
+        <v>79</v>
+      </c>
+      <c r="D6" s="12" t="s">
+        <v>87</v>
       </c>
     </row>
   </sheetData>
@@ -4780,64 +4795,64 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B15" sqref="A14:B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="4" width="42.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="36.33203125" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.83203125" style="1"/>
+    <col min="1" max="4" width="42.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="36.28515625" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="14" customHeight="1">
+    <row r="1" spans="1:5" ht="14.1" customHeight="1">
       <c r="A1" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="15.95" customHeight="1">
+      <c r="A2" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C2" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="D2" s="3"/>
+    </row>
+    <row r="3" spans="1:5" ht="15.95" customHeight="1">
+      <c r="A3" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="E1" s="8" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="16" customHeight="1">
-      <c r="A2" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="C2" s="3" t="s">
+      <c r="B3" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="D2" s="3"/>
-    </row>
-    <row r="3" spans="1:5" ht="16" customHeight="1">
-      <c r="A3" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="14" customHeight="1">
+    </row>
+    <row r="4" spans="1:5" ht="14.1" customHeight="1">
       <c r="A4" s="4"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modified FilterCOMETS function and generalized to allow more than 1 "where" rule
</commit_message>
<xml_diff>
--- a/inst/extdata/cometsInputAge.xlsx
+++ b/inst/extdata/cometsInputAge.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="27729"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1320" yWindow="645" windowWidth="24240" windowHeight="13740" activeTab="3"/>
+    <workbookView xWindow="1400" yWindow="640" windowWidth="24240" windowHeight="13740" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Metabolites" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="91">
   <si>
     <t>METABOLITE_NAME</t>
   </si>
@@ -287,13 +287,22 @@
   </si>
   <si>
     <t>site identifier.</t>
+  </si>
+  <si>
+    <t>WHERE</t>
+  </si>
+  <si>
+    <t>1.3 Unadjusted, age filtered</t>
+  </si>
+  <si>
+    <t xml:space="preserve">age &gt; 40,bmi&gt;22 </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="22">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="24" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -447,6 +456,22 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="37">
@@ -790,7 +815,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -833,6 +858,10 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -868,7 +897,7 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="46">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -897,11 +926,15 @@
     <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
     <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
     <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="43" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="45" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
     <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Hyperlink" xfId="42" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="44" builtinId="8" hidden="1"/>
     <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
@@ -1180,29 +1213,29 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E352"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="36.42578125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="38.42578125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="8.85546875" style="1"/>
+    <col min="1" max="1" width="36.5" style="1" customWidth="1"/>
+    <col min="2" max="2" width="38.5" style="1" customWidth="1"/>
+    <col min="3" max="3" width="12.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="14.1" customHeight="1">
+    <row r="1" spans="1:5" ht="14" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>73</v>
       </c>
@@ -1219,7 +1252,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15.95" customHeight="1">
+    <row r="2" spans="1:5" ht="16" customHeight="1">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -1236,7 +1269,7 @@
         <v>146.11689999999999</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="15.95" customHeight="1">
+    <row r="3" spans="1:5" ht="16" customHeight="1">
       <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
@@ -1250,7 +1283,7 @@
         <v>117.04259999999999</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15.95" customHeight="1">
+    <row r="4" spans="1:5" ht="16" customHeight="1">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
@@ -1264,7 +1297,7 @@
         <v>188.03210000000001</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="15.95" customHeight="1">
+    <row r="5" spans="1:5" ht="16" customHeight="1">
       <c r="A5" s="2" t="s">
         <v>11</v>
       </c>
@@ -1278,7 +1311,7 @@
         <v>135.05449999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="15.95" customHeight="1">
+    <row r="6" spans="1:5" ht="16" customHeight="1">
       <c r="A6" s="2" t="s">
         <v>14</v>
       </c>
@@ -1292,7 +1325,7 @@
         <v>267.09675499999997</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="15.95" customHeight="1">
+    <row r="7" spans="1:5" ht="16" customHeight="1">
       <c r="A7" s="2" t="s">
         <v>17</v>
       </c>
@@ -1306,7 +1339,7 @@
         <v>145.1</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="15.95" customHeight="1">
+    <row r="8" spans="1:5" ht="16" customHeight="1">
       <c r="A8" s="2" t="s">
         <v>20</v>
       </c>
@@ -1323,7 +1356,7 @@
         <v>203.15</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="15.95" customHeight="1">
+    <row r="9" spans="1:5" ht="16" customHeight="1">
       <c r="A9" s="2" t="s">
         <v>22</v>
       </c>
@@ -1337,7 +1370,7 @@
         <v>462.2</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="15.95" customHeight="1">
+    <row r="10" spans="1:5" ht="16" customHeight="1">
       <c r="A10" s="2" t="s">
         <v>24</v>
       </c>
@@ -1354,7 +1387,7 @@
         <v>90.06</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="15.95" customHeight="1">
+    <row r="11" spans="1:5" ht="16" customHeight="1">
       <c r="A11" s="2" t="s">
         <v>27</v>
       </c>
@@ -1368,7 +1401,7 @@
         <v>157.1</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="15.95" customHeight="1">
+    <row r="12" spans="1:5" ht="16" customHeight="1">
       <c r="A12" s="2" t="s">
         <v>30</v>
       </c>
@@ -1379,7 +1412,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="15.95" customHeight="1">
+    <row r="13" spans="1:5" ht="16" customHeight="1">
       <c r="A13" s="2" t="s">
         <v>33</v>
       </c>
@@ -1396,7 +1429,7 @@
         <v>258.1105</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="15.95" customHeight="1">
+    <row r="14" spans="1:5" ht="16" customHeight="1">
       <c r="A14" s="2" t="s">
         <v>36</v>
       </c>
@@ -1407,7 +1440,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="15.95" customHeight="1">
+    <row r="15" spans="1:5" ht="16" customHeight="1">
       <c r="A15" s="2" t="s">
         <v>39</v>
       </c>
@@ -1418,7 +1451,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="15.95" customHeight="1">
+    <row r="16" spans="1:5" ht="16" customHeight="1">
       <c r="A16" s="2" t="s">
         <v>42</v>
       </c>
@@ -1435,7 +1468,7 @@
         <v>104.07</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="15.95" customHeight="1">
+    <row r="17" spans="1:5" ht="16" customHeight="1">
       <c r="A17" s="2" t="s">
         <v>45</v>
       </c>
@@ -1449,7 +1482,7 @@
         <v>346.2</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="15.95" customHeight="1">
+    <row r="18" spans="1:5" ht="16" customHeight="1">
       <c r="A18" s="2" t="s">
         <v>47</v>
       </c>
@@ -1466,7 +1499,7 @@
         <v>241.13</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="15.95" customHeight="1">
+    <row r="19" spans="1:5" ht="16" customHeight="1">
       <c r="A19" s="2" t="s">
         <v>50</v>
       </c>
@@ -1480,1667 +1513,1667 @@
         <v>136.1</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="15.95" customHeight="1">
+    <row r="20" spans="1:5" ht="16" customHeight="1">
       <c r="A20" s="2"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
     </row>
-    <row r="21" spans="1:5" ht="15.95" customHeight="1">
+    <row r="21" spans="1:5" ht="16" customHeight="1">
       <c r="A21" s="2"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
     </row>
-    <row r="22" spans="1:5" ht="15.95" customHeight="1">
+    <row r="22" spans="1:5" ht="16" customHeight="1">
       <c r="A22" s="2"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
     </row>
-    <row r="23" spans="1:5" ht="15.95" customHeight="1">
+    <row r="23" spans="1:5" ht="16" customHeight="1">
       <c r="A23" s="2"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
     </row>
-    <row r="24" spans="1:5" ht="15.95" customHeight="1">
+    <row r="24" spans="1:5" ht="16" customHeight="1">
       <c r="A24" s="2"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
     </row>
-    <row r="25" spans="1:5" ht="15.95" customHeight="1">
+    <row r="25" spans="1:5" ht="16" customHeight="1">
       <c r="A25" s="2"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
     </row>
-    <row r="26" spans="1:5" ht="15.95" customHeight="1">
+    <row r="26" spans="1:5" ht="16" customHeight="1">
       <c r="A26" s="2"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
     </row>
-    <row r="27" spans="1:5" ht="15.95" customHeight="1">
+    <row r="27" spans="1:5" ht="16" customHeight="1">
       <c r="A27" s="2"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
     </row>
-    <row r="28" spans="1:5" ht="15.95" customHeight="1">
+    <row r="28" spans="1:5" ht="16" customHeight="1">
       <c r="A28" s="2"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
     </row>
-    <row r="29" spans="1:5" ht="15.95" customHeight="1">
+    <row r="29" spans="1:5" ht="16" customHeight="1">
       <c r="A29" s="2"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
     </row>
-    <row r="30" spans="1:5" ht="15.95" customHeight="1">
+    <row r="30" spans="1:5" ht="16" customHeight="1">
       <c r="A30" s="2"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
     </row>
-    <row r="31" spans="1:5" ht="15.95" customHeight="1">
+    <row r="31" spans="1:5" ht="16" customHeight="1">
       <c r="A31" s="2"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
     </row>
-    <row r="32" spans="1:5" ht="15.95" customHeight="1">
+    <row r="32" spans="1:5" ht="16" customHeight="1">
       <c r="A32" s="2"/>
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
     </row>
-    <row r="33" spans="1:3" ht="15.95" customHeight="1">
+    <row r="33" spans="1:3" ht="16" customHeight="1">
       <c r="A33" s="2"/>
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
     </row>
-    <row r="34" spans="1:3" ht="15.95" customHeight="1">
+    <row r="34" spans="1:3" ht="16" customHeight="1">
       <c r="A34" s="2"/>
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
     </row>
-    <row r="35" spans="1:3" ht="15.95" customHeight="1">
+    <row r="35" spans="1:3" ht="16" customHeight="1">
       <c r="A35" s="2"/>
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
     </row>
-    <row r="36" spans="1:3" ht="15.95" customHeight="1">
+    <row r="36" spans="1:3" ht="16" customHeight="1">
       <c r="A36" s="2"/>
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
     </row>
-    <row r="37" spans="1:3" ht="15.95" customHeight="1">
+    <row r="37" spans="1:3" ht="16" customHeight="1">
       <c r="A37" s="2"/>
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
     </row>
-    <row r="38" spans="1:3" ht="15.95" customHeight="1">
+    <row r="38" spans="1:3" ht="16" customHeight="1">
       <c r="A38" s="2"/>
       <c r="B38" s="3"/>
       <c r="C38" s="3"/>
     </row>
-    <row r="39" spans="1:3" ht="15.95" customHeight="1">
+    <row r="39" spans="1:3" ht="16" customHeight="1">
       <c r="A39" s="2"/>
       <c r="B39" s="3"/>
       <c r="C39" s="3"/>
     </row>
-    <row r="40" spans="1:3" ht="15.95" customHeight="1">
+    <row r="40" spans="1:3" ht="16" customHeight="1">
       <c r="A40" s="2"/>
       <c r="B40" s="3"/>
       <c r="C40" s="3"/>
     </row>
-    <row r="41" spans="1:3" ht="15.95" customHeight="1">
+    <row r="41" spans="1:3" ht="16" customHeight="1">
       <c r="A41" s="2"/>
       <c r="B41" s="3"/>
       <c r="C41" s="3"/>
     </row>
-    <row r="42" spans="1:3" ht="15.95" customHeight="1">
+    <row r="42" spans="1:3" ht="16" customHeight="1">
       <c r="A42" s="2"/>
       <c r="B42" s="3"/>
       <c r="C42" s="3"/>
     </row>
-    <row r="43" spans="1:3" ht="15.95" customHeight="1">
+    <row r="43" spans="1:3" ht="16" customHeight="1">
       <c r="A43" s="2"/>
       <c r="B43" s="3"/>
       <c r="C43" s="3"/>
     </row>
-    <row r="44" spans="1:3" ht="15.95" customHeight="1">
+    <row r="44" spans="1:3" ht="16" customHeight="1">
       <c r="A44" s="2"/>
       <c r="B44" s="3"/>
       <c r="C44" s="3"/>
     </row>
-    <row r="45" spans="1:3" ht="15.95" customHeight="1">
+    <row r="45" spans="1:3" ht="16" customHeight="1">
       <c r="A45" s="2"/>
       <c r="B45" s="3"/>
       <c r="C45" s="3"/>
     </row>
-    <row r="46" spans="1:3" ht="15.95" customHeight="1">
+    <row r="46" spans="1:3" ht="16" customHeight="1">
       <c r="A46" s="2"/>
       <c r="B46" s="3"/>
       <c r="C46" s="3"/>
     </row>
-    <row r="47" spans="1:3" ht="15.95" customHeight="1">
+    <row r="47" spans="1:3" ht="16" customHeight="1">
       <c r="A47" s="2"/>
       <c r="B47" s="3"/>
       <c r="C47" s="3"/>
     </row>
-    <row r="48" spans="1:3" ht="15.95" customHeight="1">
+    <row r="48" spans="1:3" ht="16" customHeight="1">
       <c r="A48" s="2"/>
       <c r="B48" s="3"/>
       <c r="C48" s="3"/>
     </row>
-    <row r="49" spans="1:3" ht="15.95" customHeight="1">
+    <row r="49" spans="1:3" ht="16" customHeight="1">
       <c r="A49" s="2"/>
       <c r="B49" s="3"/>
       <c r="C49" s="3"/>
     </row>
-    <row r="50" spans="1:3" ht="15.95" customHeight="1">
+    <row r="50" spans="1:3" ht="16" customHeight="1">
       <c r="A50" s="2"/>
       <c r="B50" s="3"/>
       <c r="C50" s="3"/>
     </row>
-    <row r="51" spans="1:3" ht="15.95" customHeight="1">
+    <row r="51" spans="1:3" ht="16" customHeight="1">
       <c r="A51" s="2"/>
       <c r="B51" s="3"/>
       <c r="C51" s="3"/>
     </row>
-    <row r="52" spans="1:3" ht="15.95" customHeight="1">
+    <row r="52" spans="1:3" ht="16" customHeight="1">
       <c r="A52" s="2"/>
       <c r="B52" s="3"/>
       <c r="C52" s="3"/>
     </row>
-    <row r="53" spans="1:3" ht="15.95" customHeight="1">
+    <row r="53" spans="1:3" ht="16" customHeight="1">
       <c r="A53" s="2"/>
       <c r="B53" s="3"/>
       <c r="C53" s="3"/>
     </row>
-    <row r="54" spans="1:3" ht="15.95" customHeight="1">
+    <row r="54" spans="1:3" ht="16" customHeight="1">
       <c r="A54" s="2"/>
       <c r="B54" s="3"/>
       <c r="C54" s="3"/>
     </row>
-    <row r="55" spans="1:3" ht="15.95" customHeight="1">
+    <row r="55" spans="1:3" ht="16" customHeight="1">
       <c r="A55" s="2"/>
       <c r="B55" s="3"/>
       <c r="C55" s="3"/>
     </row>
-    <row r="56" spans="1:3" ht="15.95" customHeight="1">
+    <row r="56" spans="1:3" ht="16" customHeight="1">
       <c r="A56" s="2"/>
       <c r="B56" s="3"/>
       <c r="C56" s="3"/>
     </row>
-    <row r="57" spans="1:3" ht="15.95" customHeight="1">
+    <row r="57" spans="1:3" ht="16" customHeight="1">
       <c r="A57" s="2"/>
       <c r="B57" s="3"/>
       <c r="C57" s="3"/>
     </row>
-    <row r="58" spans="1:3" ht="15.95" customHeight="1">
+    <row r="58" spans="1:3" ht="16" customHeight="1">
       <c r="A58" s="2"/>
       <c r="B58" s="3"/>
       <c r="C58" s="3"/>
     </row>
-    <row r="59" spans="1:3" ht="15.95" customHeight="1">
+    <row r="59" spans="1:3" ht="16" customHeight="1">
       <c r="A59" s="2"/>
       <c r="B59" s="3"/>
       <c r="C59" s="3"/>
     </row>
-    <row r="60" spans="1:3" ht="15.95" customHeight="1">
+    <row r="60" spans="1:3" ht="16" customHeight="1">
       <c r="A60" s="2"/>
       <c r="B60" s="3"/>
       <c r="C60" s="3"/>
     </row>
-    <row r="61" spans="1:3" ht="15.95" customHeight="1">
+    <row r="61" spans="1:3" ht="16" customHeight="1">
       <c r="A61" s="2"/>
       <c r="B61" s="3"/>
       <c r="C61" s="3"/>
     </row>
-    <row r="62" spans="1:3" ht="15.95" customHeight="1">
+    <row r="62" spans="1:3" ht="16" customHeight="1">
       <c r="A62" s="2"/>
       <c r="B62" s="3"/>
       <c r="C62" s="3"/>
     </row>
-    <row r="63" spans="1:3" ht="15.95" customHeight="1">
+    <row r="63" spans="1:3" ht="16" customHeight="1">
       <c r="A63" s="2"/>
       <c r="B63" s="3"/>
       <c r="C63" s="3"/>
     </row>
-    <row r="64" spans="1:3" ht="15.95" customHeight="1">
+    <row r="64" spans="1:3" ht="16" customHeight="1">
       <c r="A64" s="2"/>
       <c r="B64" s="3"/>
       <c r="C64" s="3"/>
     </row>
-    <row r="65" spans="1:3" ht="15.95" customHeight="1">
+    <row r="65" spans="1:3" ht="16" customHeight="1">
       <c r="A65" s="2"/>
       <c r="B65" s="3"/>
       <c r="C65" s="3"/>
     </row>
-    <row r="66" spans="1:3" ht="15.95" customHeight="1">
+    <row r="66" spans="1:3" ht="16" customHeight="1">
       <c r="A66" s="2"/>
       <c r="B66" s="3"/>
       <c r="C66" s="3"/>
     </row>
-    <row r="67" spans="1:3" ht="15.95" customHeight="1">
+    <row r="67" spans="1:3" ht="16" customHeight="1">
       <c r="A67" s="2"/>
       <c r="B67" s="3"/>
       <c r="C67" s="3"/>
     </row>
-    <row r="68" spans="1:3" ht="15.95" customHeight="1">
+    <row r="68" spans="1:3" ht="16" customHeight="1">
       <c r="A68" s="2"/>
       <c r="B68" s="3"/>
       <c r="C68" s="3"/>
     </row>
-    <row r="69" spans="1:3" ht="15.95" customHeight="1">
+    <row r="69" spans="1:3" ht="16" customHeight="1">
       <c r="A69" s="2"/>
       <c r="B69" s="3"/>
       <c r="C69" s="3"/>
     </row>
-    <row r="70" spans="1:3" ht="15.95" customHeight="1">
+    <row r="70" spans="1:3" ht="16" customHeight="1">
       <c r="A70" s="2"/>
       <c r="B70" s="3"/>
       <c r="C70" s="3"/>
     </row>
-    <row r="71" spans="1:3" ht="15.95" customHeight="1">
+    <row r="71" spans="1:3" ht="16" customHeight="1">
       <c r="A71" s="2"/>
       <c r="B71" s="3"/>
       <c r="C71" s="3"/>
     </row>
-    <row r="72" spans="1:3" ht="15.95" customHeight="1">
+    <row r="72" spans="1:3" ht="16" customHeight="1">
       <c r="A72" s="2"/>
       <c r="B72" s="3"/>
       <c r="C72" s="3"/>
     </row>
-    <row r="73" spans="1:3" ht="15.95" customHeight="1">
+    <row r="73" spans="1:3" ht="16" customHeight="1">
       <c r="A73" s="2"/>
       <c r="B73" s="3"/>
       <c r="C73" s="3"/>
     </row>
-    <row r="74" spans="1:3" ht="15.95" customHeight="1">
+    <row r="74" spans="1:3" ht="16" customHeight="1">
       <c r="A74" s="2"/>
       <c r="B74" s="3"/>
       <c r="C74" s="3"/>
     </row>
-    <row r="75" spans="1:3" ht="15.95" customHeight="1">
+    <row r="75" spans="1:3" ht="16" customHeight="1">
       <c r="A75" s="2"/>
       <c r="B75" s="3"/>
       <c r="C75" s="3"/>
     </row>
-    <row r="76" spans="1:3" ht="15.95" customHeight="1">
+    <row r="76" spans="1:3" ht="16" customHeight="1">
       <c r="A76" s="2"/>
       <c r="B76" s="3"/>
       <c r="C76" s="3"/>
     </row>
-    <row r="77" spans="1:3" ht="15.95" customHeight="1">
+    <row r="77" spans="1:3" ht="16" customHeight="1">
       <c r="A77" s="2"/>
       <c r="B77" s="3"/>
       <c r="C77" s="3"/>
     </row>
-    <row r="78" spans="1:3" ht="15.95" customHeight="1">
+    <row r="78" spans="1:3" ht="16" customHeight="1">
       <c r="A78" s="2"/>
       <c r="B78" s="3"/>
       <c r="C78" s="3"/>
     </row>
-    <row r="79" spans="1:3" ht="15.95" customHeight="1">
+    <row r="79" spans="1:3" ht="16" customHeight="1">
       <c r="A79" s="2"/>
       <c r="B79" s="3"/>
       <c r="C79" s="3"/>
     </row>
-    <row r="80" spans="1:3" ht="15.95" customHeight="1">
+    <row r="80" spans="1:3" ht="16" customHeight="1">
       <c r="A80" s="2"/>
       <c r="B80" s="3"/>
       <c r="C80" s="3"/>
     </row>
-    <row r="81" spans="1:3" ht="15.95" customHeight="1">
+    <row r="81" spans="1:3" ht="16" customHeight="1">
       <c r="A81" s="2"/>
       <c r="B81" s="3"/>
       <c r="C81" s="3"/>
     </row>
-    <row r="82" spans="1:3" ht="15.95" customHeight="1">
+    <row r="82" spans="1:3" ht="16" customHeight="1">
       <c r="A82" s="2"/>
       <c r="B82" s="3"/>
       <c r="C82" s="3"/>
     </row>
-    <row r="83" spans="1:3" ht="15.95" customHeight="1">
+    <row r="83" spans="1:3" ht="16" customHeight="1">
       <c r="A83" s="2"/>
       <c r="B83" s="3"/>
       <c r="C83" s="3"/>
     </row>
-    <row r="84" spans="1:3" ht="15.95" customHeight="1">
+    <row r="84" spans="1:3" ht="16" customHeight="1">
       <c r="A84" s="2"/>
       <c r="B84" s="3"/>
       <c r="C84" s="3"/>
     </row>
-    <row r="85" spans="1:3" ht="15.95" customHeight="1">
+    <row r="85" spans="1:3" ht="16" customHeight="1">
       <c r="A85" s="2"/>
       <c r="B85" s="3"/>
       <c r="C85" s="3"/>
     </row>
-    <row r="86" spans="1:3" ht="15.95" customHeight="1">
+    <row r="86" spans="1:3" ht="16" customHeight="1">
       <c r="A86" s="2"/>
       <c r="B86" s="3"/>
       <c r="C86" s="3"/>
     </row>
-    <row r="87" spans="1:3" ht="15.95" customHeight="1">
+    <row r="87" spans="1:3" ht="16" customHeight="1">
       <c r="A87" s="2"/>
       <c r="B87" s="3"/>
       <c r="C87" s="3"/>
     </row>
-    <row r="88" spans="1:3" ht="15.95" customHeight="1">
+    <row r="88" spans="1:3" ht="16" customHeight="1">
       <c r="A88" s="2"/>
       <c r="B88" s="3"/>
       <c r="C88" s="3"/>
     </row>
-    <row r="89" spans="1:3" ht="15.95" customHeight="1">
+    <row r="89" spans="1:3" ht="16" customHeight="1">
       <c r="A89" s="2"/>
       <c r="B89" s="3"/>
       <c r="C89" s="3"/>
     </row>
-    <row r="90" spans="1:3" ht="15.95" customHeight="1">
+    <row r="90" spans="1:3" ht="16" customHeight="1">
       <c r="A90" s="2"/>
       <c r="B90" s="3"/>
       <c r="C90" s="3"/>
     </row>
-    <row r="91" spans="1:3" ht="15.95" customHeight="1">
+    <row r="91" spans="1:3" ht="16" customHeight="1">
       <c r="A91" s="2"/>
       <c r="B91" s="3"/>
       <c r="C91" s="3"/>
     </row>
-    <row r="92" spans="1:3" ht="15.95" customHeight="1">
+    <row r="92" spans="1:3" ht="16" customHeight="1">
       <c r="A92" s="2"/>
       <c r="B92" s="3"/>
       <c r="C92" s="3"/>
     </row>
-    <row r="93" spans="1:3" ht="15.95" customHeight="1">
+    <row r="93" spans="1:3" ht="16" customHeight="1">
       <c r="A93" s="2"/>
       <c r="B93" s="3"/>
       <c r="C93" s="3"/>
     </row>
-    <row r="94" spans="1:3" ht="15.95" customHeight="1">
+    <row r="94" spans="1:3" ht="16" customHeight="1">
       <c r="A94" s="2"/>
       <c r="B94" s="3"/>
       <c r="C94" s="3"/>
     </row>
-    <row r="95" spans="1:3" ht="15.95" customHeight="1">
+    <row r="95" spans="1:3" ht="16" customHeight="1">
       <c r="A95" s="2"/>
       <c r="B95" s="3"/>
       <c r="C95" s="3"/>
     </row>
-    <row r="96" spans="1:3" ht="15.95" customHeight="1">
+    <row r="96" spans="1:3" ht="16" customHeight="1">
       <c r="A96" s="2"/>
       <c r="B96" s="3"/>
       <c r="C96" s="3"/>
     </row>
-    <row r="97" spans="1:3" ht="15.95" customHeight="1">
+    <row r="97" spans="1:3" ht="16" customHeight="1">
       <c r="A97" s="2"/>
       <c r="B97" s="3"/>
       <c r="C97" s="3"/>
     </row>
-    <row r="98" spans="1:3" ht="15.95" customHeight="1">
+    <row r="98" spans="1:3" ht="16" customHeight="1">
       <c r="A98" s="2"/>
       <c r="B98" s="3"/>
       <c r="C98" s="3"/>
     </row>
-    <row r="99" spans="1:3" ht="15.95" customHeight="1">
+    <row r="99" spans="1:3" ht="16" customHeight="1">
       <c r="A99" s="2"/>
       <c r="B99" s="3"/>
       <c r="C99" s="3"/>
     </row>
-    <row r="100" spans="1:3" ht="15.95" customHeight="1">
+    <row r="100" spans="1:3" ht="16" customHeight="1">
       <c r="A100" s="2"/>
       <c r="B100" s="3"/>
       <c r="C100" s="3"/>
     </row>
-    <row r="101" spans="1:3" ht="15.95" customHeight="1">
+    <row r="101" spans="1:3" ht="16" customHeight="1">
       <c r="A101" s="2"/>
       <c r="B101" s="3"/>
       <c r="C101" s="3"/>
     </row>
-    <row r="102" spans="1:3" ht="15.95" customHeight="1">
+    <row r="102" spans="1:3" ht="16" customHeight="1">
       <c r="A102" s="2"/>
       <c r="B102" s="3"/>
       <c r="C102" s="3"/>
     </row>
-    <row r="103" spans="1:3" ht="15.95" customHeight="1">
+    <row r="103" spans="1:3" ht="16" customHeight="1">
       <c r="A103" s="2"/>
       <c r="B103" s="3"/>
       <c r="C103" s="3"/>
     </row>
-    <row r="104" spans="1:3" ht="15.95" customHeight="1">
+    <row r="104" spans="1:3" ht="16" customHeight="1">
       <c r="A104" s="2"/>
       <c r="B104" s="3"/>
       <c r="C104" s="3"/>
     </row>
-    <row r="105" spans="1:3" ht="15.95" customHeight="1">
+    <row r="105" spans="1:3" ht="16" customHeight="1">
       <c r="A105" s="2"/>
       <c r="B105" s="3"/>
       <c r="C105" s="3"/>
     </row>
-    <row r="106" spans="1:3" ht="15.95" customHeight="1">
+    <row r="106" spans="1:3" ht="16" customHeight="1">
       <c r="A106" s="2"/>
       <c r="B106" s="3"/>
       <c r="C106" s="3"/>
     </row>
-    <row r="107" spans="1:3" ht="15.95" customHeight="1">
+    <row r="107" spans="1:3" ht="16" customHeight="1">
       <c r="A107" s="2"/>
       <c r="B107" s="3"/>
       <c r="C107" s="3"/>
     </row>
-    <row r="108" spans="1:3" ht="15.95" customHeight="1">
+    <row r="108" spans="1:3" ht="16" customHeight="1">
       <c r="A108" s="2"/>
       <c r="B108" s="3"/>
       <c r="C108" s="3"/>
     </row>
-    <row r="109" spans="1:3" ht="15.95" customHeight="1">
+    <row r="109" spans="1:3" ht="16" customHeight="1">
       <c r="A109" s="2"/>
       <c r="B109" s="3"/>
       <c r="C109" s="3"/>
     </row>
-    <row r="110" spans="1:3" ht="15.95" customHeight="1">
+    <row r="110" spans="1:3" ht="16" customHeight="1">
       <c r="A110" s="2"/>
       <c r="B110" s="3"/>
       <c r="C110" s="3"/>
     </row>
-    <row r="111" spans="1:3" ht="15.95" customHeight="1">
+    <row r="111" spans="1:3" ht="16" customHeight="1">
       <c r="A111" s="2"/>
       <c r="B111" s="3"/>
       <c r="C111" s="3"/>
     </row>
-    <row r="112" spans="1:3" ht="15.95" customHeight="1">
+    <row r="112" spans="1:3" ht="16" customHeight="1">
       <c r="A112" s="2"/>
       <c r="B112" s="3"/>
       <c r="C112" s="3"/>
     </row>
-    <row r="113" spans="1:3" ht="15.95" customHeight="1">
+    <row r="113" spans="1:3" ht="16" customHeight="1">
       <c r="A113" s="2"/>
       <c r="B113" s="3"/>
       <c r="C113" s="3"/>
     </row>
-    <row r="114" spans="1:3" ht="15.95" customHeight="1">
+    <row r="114" spans="1:3" ht="16" customHeight="1">
       <c r="A114" s="2"/>
       <c r="B114" s="3"/>
       <c r="C114" s="3"/>
     </row>
-    <row r="115" spans="1:3" ht="15.95" customHeight="1">
+    <row r="115" spans="1:3" ht="16" customHeight="1">
       <c r="A115" s="2"/>
       <c r="B115" s="3"/>
       <c r="C115" s="3"/>
     </row>
-    <row r="116" spans="1:3" ht="15.95" customHeight="1">
+    <row r="116" spans="1:3" ht="16" customHeight="1">
       <c r="A116" s="2"/>
       <c r="B116" s="3"/>
       <c r="C116" s="3"/>
     </row>
-    <row r="117" spans="1:3" ht="15.95" customHeight="1">
+    <row r="117" spans="1:3" ht="16" customHeight="1">
       <c r="A117" s="2"/>
       <c r="B117" s="3"/>
       <c r="C117" s="3"/>
     </row>
-    <row r="118" spans="1:3" ht="15.95" customHeight="1">
+    <row r="118" spans="1:3" ht="16" customHeight="1">
       <c r="A118" s="2"/>
       <c r="B118" s="3"/>
       <c r="C118" s="3"/>
     </row>
-    <row r="119" spans="1:3" ht="15.95" customHeight="1">
+    <row r="119" spans="1:3" ht="16" customHeight="1">
       <c r="A119" s="2"/>
       <c r="B119" s="3"/>
       <c r="C119" s="3"/>
     </row>
-    <row r="120" spans="1:3" ht="15.95" customHeight="1">
+    <row r="120" spans="1:3" ht="16" customHeight="1">
       <c r="A120" s="2"/>
       <c r="B120" s="3"/>
       <c r="C120" s="3"/>
     </row>
-    <row r="121" spans="1:3" ht="15.95" customHeight="1">
+    <row r="121" spans="1:3" ht="16" customHeight="1">
       <c r="A121" s="2"/>
       <c r="B121" s="3"/>
       <c r="C121" s="3"/>
     </row>
-    <row r="122" spans="1:3" ht="15.95" customHeight="1">
+    <row r="122" spans="1:3" ht="16" customHeight="1">
       <c r="A122" s="2"/>
       <c r="B122" s="3"/>
       <c r="C122" s="3"/>
     </row>
-    <row r="123" spans="1:3" ht="15.95" customHeight="1">
+    <row r="123" spans="1:3" ht="16" customHeight="1">
       <c r="A123" s="2"/>
       <c r="B123" s="3"/>
       <c r="C123" s="3"/>
     </row>
-    <row r="124" spans="1:3" ht="15.95" customHeight="1">
+    <row r="124" spans="1:3" ht="16" customHeight="1">
       <c r="A124" s="2"/>
       <c r="B124" s="3"/>
       <c r="C124" s="3"/>
     </row>
-    <row r="125" spans="1:3" ht="15.95" customHeight="1">
+    <row r="125" spans="1:3" ht="16" customHeight="1">
       <c r="A125" s="2"/>
       <c r="B125" s="3"/>
       <c r="C125" s="3"/>
     </row>
-    <row r="126" spans="1:3" ht="15.95" customHeight="1">
+    <row r="126" spans="1:3" ht="16" customHeight="1">
       <c r="A126" s="2"/>
       <c r="B126" s="3"/>
       <c r="C126" s="3"/>
     </row>
-    <row r="127" spans="1:3" ht="15.95" customHeight="1">
+    <row r="127" spans="1:3" ht="16" customHeight="1">
       <c r="A127" s="2"/>
       <c r="B127" s="3"/>
       <c r="C127" s="3"/>
     </row>
-    <row r="128" spans="1:3" ht="15.95" customHeight="1">
+    <row r="128" spans="1:3" ht="16" customHeight="1">
       <c r="A128" s="2"/>
       <c r="B128" s="3"/>
       <c r="C128" s="3"/>
     </row>
-    <row r="129" spans="1:3" ht="15.95" customHeight="1">
+    <row r="129" spans="1:3" ht="16" customHeight="1">
       <c r="A129" s="2"/>
       <c r="B129" s="3"/>
       <c r="C129" s="3"/>
     </row>
-    <row r="130" spans="1:3" ht="15.95" customHeight="1">
+    <row r="130" spans="1:3" ht="16" customHeight="1">
       <c r="A130" s="2"/>
       <c r="B130" s="3"/>
       <c r="C130" s="3"/>
     </row>
-    <row r="131" spans="1:3" ht="15.95" customHeight="1">
+    <row r="131" spans="1:3" ht="16" customHeight="1">
       <c r="A131" s="2"/>
       <c r="B131" s="3"/>
       <c r="C131" s="3"/>
     </row>
-    <row r="132" spans="1:3" ht="15.95" customHeight="1">
+    <row r="132" spans="1:3" ht="16" customHeight="1">
       <c r="A132" s="2"/>
       <c r="B132" s="3"/>
       <c r="C132" s="3"/>
     </row>
-    <row r="133" spans="1:3" ht="15.95" customHeight="1">
+    <row r="133" spans="1:3" ht="16" customHeight="1">
       <c r="A133" s="2"/>
       <c r="B133" s="3"/>
       <c r="C133" s="3"/>
     </row>
-    <row r="134" spans="1:3" ht="15.95" customHeight="1">
+    <row r="134" spans="1:3" ht="16" customHeight="1">
       <c r="A134" s="2"/>
       <c r="B134" s="3"/>
       <c r="C134" s="3"/>
     </row>
-    <row r="135" spans="1:3" ht="15.95" customHeight="1">
+    <row r="135" spans="1:3" ht="16" customHeight="1">
       <c r="A135" s="2"/>
       <c r="B135" s="3"/>
       <c r="C135" s="3"/>
     </row>
-    <row r="136" spans="1:3" ht="15.95" customHeight="1">
+    <row r="136" spans="1:3" ht="16" customHeight="1">
       <c r="A136" s="2"/>
       <c r="B136" s="3"/>
       <c r="C136" s="3"/>
     </row>
-    <row r="137" spans="1:3" ht="15.95" customHeight="1">
+    <row r="137" spans="1:3" ht="16" customHeight="1">
       <c r="A137" s="2"/>
       <c r="B137" s="3"/>
       <c r="C137" s="3"/>
     </row>
-    <row r="138" spans="1:3" ht="15.95" customHeight="1">
+    <row r="138" spans="1:3" ht="16" customHeight="1">
       <c r="A138" s="2"/>
       <c r="B138" s="3"/>
       <c r="C138" s="3"/>
     </row>
-    <row r="139" spans="1:3" ht="15.95" customHeight="1">
+    <row r="139" spans="1:3" ht="16" customHeight="1">
       <c r="A139" s="2"/>
       <c r="B139" s="3"/>
       <c r="C139" s="3"/>
     </row>
-    <row r="140" spans="1:3" ht="15.95" customHeight="1">
+    <row r="140" spans="1:3" ht="16" customHeight="1">
       <c r="A140" s="2"/>
       <c r="B140" s="3"/>
       <c r="C140" s="3"/>
     </row>
-    <row r="141" spans="1:3" ht="15.95" customHeight="1">
+    <row r="141" spans="1:3" ht="16" customHeight="1">
       <c r="A141" s="2"/>
       <c r="B141" s="3"/>
       <c r="C141" s="3"/>
     </row>
-    <row r="142" spans="1:3" ht="15.95" customHeight="1">
+    <row r="142" spans="1:3" ht="16" customHeight="1">
       <c r="A142" s="2"/>
       <c r="B142" s="3"/>
       <c r="C142" s="3"/>
     </row>
-    <row r="143" spans="1:3" ht="15.95" customHeight="1">
+    <row r="143" spans="1:3" ht="16" customHeight="1">
       <c r="A143" s="2"/>
       <c r="B143" s="3"/>
       <c r="C143" s="3"/>
     </row>
-    <row r="144" spans="1:3" ht="15.95" customHeight="1">
+    <row r="144" spans="1:3" ht="16" customHeight="1">
       <c r="A144" s="2"/>
       <c r="B144" s="3"/>
       <c r="C144" s="3"/>
     </row>
-    <row r="145" spans="1:3" ht="15.95" customHeight="1">
+    <row r="145" spans="1:3" ht="16" customHeight="1">
       <c r="A145" s="2"/>
       <c r="B145" s="3"/>
       <c r="C145" s="3"/>
     </row>
-    <row r="146" spans="1:3" ht="15.95" customHeight="1">
+    <row r="146" spans="1:3" ht="16" customHeight="1">
       <c r="A146" s="2"/>
       <c r="B146" s="3"/>
       <c r="C146" s="3"/>
     </row>
-    <row r="147" spans="1:3" ht="15.95" customHeight="1">
+    <row r="147" spans="1:3" ht="16" customHeight="1">
       <c r="A147" s="2"/>
       <c r="B147" s="3"/>
       <c r="C147" s="3"/>
     </row>
-    <row r="148" spans="1:3" ht="15.95" customHeight="1">
+    <row r="148" spans="1:3" ht="16" customHeight="1">
       <c r="A148" s="2"/>
       <c r="B148" s="3"/>
       <c r="C148" s="3"/>
     </row>
-    <row r="149" spans="1:3" ht="15.95" customHeight="1">
+    <row r="149" spans="1:3" ht="16" customHeight="1">
       <c r="A149" s="2"/>
       <c r="B149" s="3"/>
       <c r="C149" s="3"/>
     </row>
-    <row r="150" spans="1:3" ht="15.95" customHeight="1">
+    <row r="150" spans="1:3" ht="16" customHeight="1">
       <c r="A150" s="2"/>
       <c r="B150" s="3"/>
       <c r="C150" s="3"/>
     </row>
-    <row r="151" spans="1:3" ht="15.95" customHeight="1">
+    <row r="151" spans="1:3" ht="16" customHeight="1">
       <c r="A151" s="2"/>
       <c r="B151" s="3"/>
       <c r="C151" s="3"/>
     </row>
-    <row r="152" spans="1:3" ht="15.95" customHeight="1">
+    <row r="152" spans="1:3" ht="16" customHeight="1">
       <c r="A152" s="2"/>
       <c r="B152" s="3"/>
       <c r="C152" s="3"/>
     </row>
-    <row r="153" spans="1:3" ht="15.95" customHeight="1">
+    <row r="153" spans="1:3" ht="16" customHeight="1">
       <c r="A153" s="2"/>
       <c r="B153" s="3"/>
       <c r="C153" s="3"/>
     </row>
-    <row r="154" spans="1:3" ht="15.95" customHeight="1">
+    <row r="154" spans="1:3" ht="16" customHeight="1">
       <c r="A154" s="2"/>
       <c r="B154" s="3"/>
       <c r="C154" s="3"/>
     </row>
-    <row r="155" spans="1:3" ht="15.95" customHeight="1">
+    <row r="155" spans="1:3" ht="16" customHeight="1">
       <c r="A155" s="2"/>
       <c r="B155" s="3"/>
       <c r="C155" s="3"/>
     </row>
-    <row r="156" spans="1:3" ht="15.95" customHeight="1">
+    <row r="156" spans="1:3" ht="16" customHeight="1">
       <c r="A156" s="2"/>
       <c r="B156" s="3"/>
       <c r="C156" s="3"/>
     </row>
-    <row r="157" spans="1:3" ht="15.95" customHeight="1">
+    <row r="157" spans="1:3" ht="16" customHeight="1">
       <c r="A157" s="2"/>
       <c r="B157" s="3"/>
       <c r="C157" s="3"/>
     </row>
-    <row r="158" spans="1:3" ht="15.95" customHeight="1">
+    <row r="158" spans="1:3" ht="16" customHeight="1">
       <c r="A158" s="2"/>
       <c r="B158" s="3"/>
       <c r="C158" s="3"/>
     </row>
-    <row r="159" spans="1:3" ht="15.95" customHeight="1">
+    <row r="159" spans="1:3" ht="16" customHeight="1">
       <c r="A159" s="2"/>
       <c r="B159" s="3"/>
       <c r="C159" s="3"/>
     </row>
-    <row r="160" spans="1:3" ht="15.95" customHeight="1">
+    <row r="160" spans="1:3" ht="16" customHeight="1">
       <c r="A160" s="2"/>
       <c r="B160" s="3"/>
       <c r="C160" s="3"/>
     </row>
-    <row r="161" spans="1:3" ht="15.95" customHeight="1">
+    <row r="161" spans="1:3" ht="16" customHeight="1">
       <c r="A161" s="2"/>
       <c r="B161" s="3"/>
       <c r="C161" s="3"/>
     </row>
-    <row r="162" spans="1:3" ht="15.95" customHeight="1">
+    <row r="162" spans="1:3" ht="16" customHeight="1">
       <c r="A162" s="2"/>
       <c r="B162" s="3"/>
       <c r="C162" s="3"/>
     </row>
-    <row r="163" spans="1:3" ht="15.95" customHeight="1">
+    <row r="163" spans="1:3" ht="16" customHeight="1">
       <c r="A163" s="2"/>
       <c r="B163" s="3"/>
       <c r="C163" s="3"/>
     </row>
-    <row r="164" spans="1:3" ht="15.95" customHeight="1">
+    <row r="164" spans="1:3" ht="16" customHeight="1">
       <c r="A164" s="2"/>
       <c r="B164" s="3"/>
       <c r="C164" s="3"/>
     </row>
-    <row r="165" spans="1:3" ht="15.95" customHeight="1">
+    <row r="165" spans="1:3" ht="16" customHeight="1">
       <c r="A165" s="2"/>
       <c r="B165" s="3"/>
       <c r="C165" s="3"/>
     </row>
-    <row r="166" spans="1:3" ht="15.95" customHeight="1">
+    <row r="166" spans="1:3" ht="16" customHeight="1">
       <c r="A166" s="2"/>
       <c r="B166" s="3"/>
       <c r="C166" s="3"/>
     </row>
-    <row r="167" spans="1:3" ht="15.95" customHeight="1">
+    <row r="167" spans="1:3" ht="16" customHeight="1">
       <c r="A167" s="2"/>
       <c r="B167" s="3"/>
       <c r="C167" s="3"/>
     </row>
-    <row r="168" spans="1:3" ht="15.95" customHeight="1">
+    <row r="168" spans="1:3" ht="16" customHeight="1">
       <c r="A168" s="2"/>
       <c r="B168" s="3"/>
       <c r="C168" s="3"/>
     </row>
-    <row r="169" spans="1:3" ht="15.95" customHeight="1">
+    <row r="169" spans="1:3" ht="16" customHeight="1">
       <c r="A169" s="2"/>
       <c r="B169" s="3"/>
       <c r="C169" s="3"/>
     </row>
-    <row r="170" spans="1:3" ht="15.95" customHeight="1">
+    <row r="170" spans="1:3" ht="16" customHeight="1">
       <c r="A170" s="2"/>
       <c r="B170" s="3"/>
       <c r="C170" s="3"/>
     </row>
-    <row r="171" spans="1:3" ht="15.95" customHeight="1">
+    <row r="171" spans="1:3" ht="16" customHeight="1">
       <c r="A171" s="2"/>
       <c r="B171" s="3"/>
       <c r="C171" s="3"/>
     </row>
-    <row r="172" spans="1:3" ht="15.95" customHeight="1">
+    <row r="172" spans="1:3" ht="16" customHeight="1">
       <c r="A172" s="2"/>
       <c r="B172" s="3"/>
       <c r="C172" s="3"/>
     </row>
-    <row r="173" spans="1:3" ht="15.95" customHeight="1">
+    <row r="173" spans="1:3" ht="16" customHeight="1">
       <c r="A173" s="2"/>
       <c r="B173" s="3"/>
       <c r="C173" s="3"/>
     </row>
-    <row r="174" spans="1:3" ht="15.95" customHeight="1">
+    <row r="174" spans="1:3" ht="16" customHeight="1">
       <c r="A174" s="2"/>
       <c r="B174" s="3"/>
       <c r="C174" s="3"/>
     </row>
-    <row r="175" spans="1:3" ht="15.95" customHeight="1">
+    <row r="175" spans="1:3" ht="16" customHeight="1">
       <c r="A175" s="2"/>
       <c r="B175" s="3"/>
       <c r="C175" s="3"/>
     </row>
-    <row r="176" spans="1:3" ht="15.95" customHeight="1">
+    <row r="176" spans="1:3" ht="16" customHeight="1">
       <c r="A176" s="2"/>
       <c r="B176" s="3"/>
       <c r="C176" s="3"/>
     </row>
-    <row r="177" spans="1:3" ht="15.95" customHeight="1">
+    <row r="177" spans="1:3" ht="16" customHeight="1">
       <c r="A177" s="2"/>
       <c r="B177" s="3"/>
       <c r="C177" s="3"/>
     </row>
-    <row r="178" spans="1:3" ht="15.95" customHeight="1">
+    <row r="178" spans="1:3" ht="16" customHeight="1">
       <c r="A178" s="2"/>
       <c r="B178" s="3"/>
       <c r="C178" s="3"/>
     </row>
-    <row r="179" spans="1:3" ht="15.95" customHeight="1">
+    <row r="179" spans="1:3" ht="16" customHeight="1">
       <c r="A179" s="2"/>
       <c r="B179" s="3"/>
       <c r="C179" s="3"/>
     </row>
-    <row r="180" spans="1:3" ht="15.95" customHeight="1">
+    <row r="180" spans="1:3" ht="16" customHeight="1">
       <c r="A180" s="2"/>
       <c r="B180" s="3"/>
       <c r="C180" s="3"/>
     </row>
-    <row r="181" spans="1:3" ht="15.95" customHeight="1">
+    <row r="181" spans="1:3" ht="16" customHeight="1">
       <c r="A181" s="2"/>
       <c r="B181" s="3"/>
       <c r="C181" s="3"/>
     </row>
-    <row r="182" spans="1:3" ht="15.95" customHeight="1">
+    <row r="182" spans="1:3" ht="16" customHeight="1">
       <c r="A182" s="2"/>
       <c r="B182" s="3"/>
       <c r="C182" s="3"/>
     </row>
-    <row r="183" spans="1:3" ht="15.95" customHeight="1">
+    <row r="183" spans="1:3" ht="16" customHeight="1">
       <c r="A183" s="2"/>
       <c r="B183" s="3"/>
       <c r="C183" s="3"/>
     </row>
-    <row r="184" spans="1:3" ht="15.95" customHeight="1">
+    <row r="184" spans="1:3" ht="16" customHeight="1">
       <c r="A184" s="2"/>
       <c r="B184" s="3"/>
       <c r="C184" s="3"/>
     </row>
-    <row r="185" spans="1:3" ht="15.95" customHeight="1">
+    <row r="185" spans="1:3" ht="16" customHeight="1">
       <c r="A185" s="2"/>
       <c r="B185" s="3"/>
       <c r="C185" s="3"/>
     </row>
-    <row r="186" spans="1:3" ht="15.95" customHeight="1">
+    <row r="186" spans="1:3" ht="16" customHeight="1">
       <c r="A186" s="2"/>
       <c r="B186" s="3"/>
       <c r="C186" s="3"/>
     </row>
-    <row r="187" spans="1:3" ht="15.95" customHeight="1">
+    <row r="187" spans="1:3" ht="16" customHeight="1">
       <c r="A187" s="2"/>
       <c r="B187" s="3"/>
       <c r="C187" s="3"/>
     </row>
-    <row r="188" spans="1:3" ht="15.95" customHeight="1">
+    <row r="188" spans="1:3" ht="16" customHeight="1">
       <c r="A188" s="2"/>
       <c r="B188" s="3"/>
       <c r="C188" s="3"/>
     </row>
-    <row r="189" spans="1:3" ht="15.95" customHeight="1">
+    <row r="189" spans="1:3" ht="16" customHeight="1">
       <c r="A189" s="2"/>
       <c r="B189" s="3"/>
       <c r="C189" s="3"/>
     </row>
-    <row r="190" spans="1:3" ht="15.95" customHeight="1">
+    <row r="190" spans="1:3" ht="16" customHeight="1">
       <c r="A190" s="2"/>
       <c r="B190" s="3"/>
       <c r="C190" s="3"/>
     </row>
-    <row r="191" spans="1:3" ht="15.95" customHeight="1">
+    <row r="191" spans="1:3" ht="16" customHeight="1">
       <c r="A191" s="2"/>
       <c r="B191" s="3"/>
       <c r="C191" s="3"/>
     </row>
-    <row r="192" spans="1:3" ht="15.95" customHeight="1">
+    <row r="192" spans="1:3" ht="16" customHeight="1">
       <c r="A192" s="2"/>
       <c r="B192" s="3"/>
       <c r="C192" s="3"/>
     </row>
-    <row r="193" spans="1:3" ht="15.95" customHeight="1">
+    <row r="193" spans="1:3" ht="16" customHeight="1">
       <c r="A193" s="2"/>
       <c r="B193" s="3"/>
       <c r="C193" s="3"/>
     </row>
-    <row r="194" spans="1:3" ht="15.95" customHeight="1">
+    <row r="194" spans="1:3" ht="16" customHeight="1">
       <c r="A194" s="2"/>
       <c r="B194" s="3"/>
       <c r="C194" s="3"/>
     </row>
-    <row r="195" spans="1:3" ht="15.95" customHeight="1">
+    <row r="195" spans="1:3" ht="16" customHeight="1">
       <c r="A195" s="2"/>
       <c r="B195" s="3"/>
       <c r="C195" s="3"/>
     </row>
-    <row r="196" spans="1:3" ht="15.95" customHeight="1">
+    <row r="196" spans="1:3" ht="16" customHeight="1">
       <c r="A196" s="2"/>
       <c r="B196" s="3"/>
       <c r="C196" s="3"/>
     </row>
-    <row r="197" spans="1:3" ht="15.95" customHeight="1">
+    <row r="197" spans="1:3" ht="16" customHeight="1">
       <c r="A197" s="2"/>
       <c r="B197" s="3"/>
       <c r="C197" s="3"/>
     </row>
-    <row r="198" spans="1:3" ht="15.95" customHeight="1">
+    <row r="198" spans="1:3" ht="16" customHeight="1">
       <c r="A198" s="2"/>
       <c r="B198" s="3"/>
       <c r="C198" s="3"/>
     </row>
-    <row r="199" spans="1:3" ht="15.95" customHeight="1">
+    <row r="199" spans="1:3" ht="16" customHeight="1">
       <c r="A199" s="2"/>
       <c r="B199" s="3"/>
       <c r="C199" s="3"/>
     </row>
-    <row r="200" spans="1:3" ht="15.95" customHeight="1">
+    <row r="200" spans="1:3" ht="16" customHeight="1">
       <c r="A200" s="2"/>
       <c r="B200" s="3"/>
       <c r="C200" s="3"/>
     </row>
-    <row r="201" spans="1:3" ht="15.95" customHeight="1">
+    <row r="201" spans="1:3" ht="16" customHeight="1">
       <c r="A201" s="2"/>
       <c r="B201" s="3"/>
       <c r="C201" s="3"/>
     </row>
-    <row r="202" spans="1:3" ht="15.95" customHeight="1">
+    <row r="202" spans="1:3" ht="16" customHeight="1">
       <c r="A202" s="2"/>
       <c r="B202" s="3"/>
       <c r="C202" s="3"/>
     </row>
-    <row r="203" spans="1:3" ht="15.95" customHeight="1">
+    <row r="203" spans="1:3" ht="16" customHeight="1">
       <c r="A203" s="2"/>
       <c r="B203" s="3"/>
       <c r="C203" s="3"/>
     </row>
-    <row r="204" spans="1:3" ht="15.95" customHeight="1">
+    <row r="204" spans="1:3" ht="16" customHeight="1">
       <c r="A204" s="2"/>
       <c r="B204" s="3"/>
       <c r="C204" s="3"/>
     </row>
-    <row r="205" spans="1:3" ht="15.95" customHeight="1">
+    <row r="205" spans="1:3" ht="16" customHeight="1">
       <c r="A205" s="2"/>
       <c r="B205" s="3"/>
       <c r="C205" s="3"/>
     </row>
-    <row r="206" spans="1:3" ht="15.95" customHeight="1">
+    <row r="206" spans="1:3" ht="16" customHeight="1">
       <c r="A206" s="2"/>
       <c r="B206" s="3"/>
       <c r="C206" s="3"/>
     </row>
-    <row r="207" spans="1:3" ht="15.95" customHeight="1">
+    <row r="207" spans="1:3" ht="16" customHeight="1">
       <c r="A207" s="2"/>
       <c r="B207" s="3"/>
       <c r="C207" s="3"/>
     </row>
-    <row r="208" spans="1:3" ht="15.95" customHeight="1">
+    <row r="208" spans="1:3" ht="16" customHeight="1">
       <c r="A208" s="2"/>
       <c r="B208" s="3"/>
       <c r="C208" s="3"/>
     </row>
-    <row r="209" spans="1:3" ht="15.95" customHeight="1">
+    <row r="209" spans="1:3" ht="16" customHeight="1">
       <c r="A209" s="2"/>
       <c r="B209" s="3"/>
       <c r="C209" s="3"/>
     </row>
-    <row r="210" spans="1:3" ht="15.95" customHeight="1">
+    <row r="210" spans="1:3" ht="16" customHeight="1">
       <c r="A210" s="2"/>
       <c r="B210" s="3"/>
       <c r="C210" s="3"/>
     </row>
-    <row r="211" spans="1:3" ht="15.95" customHeight="1">
+    <row r="211" spans="1:3" ht="16" customHeight="1">
       <c r="A211" s="2"/>
       <c r="B211" s="3"/>
       <c r="C211" s="3"/>
     </row>
-    <row r="212" spans="1:3" ht="15.95" customHeight="1">
+    <row r="212" spans="1:3" ht="16" customHeight="1">
       <c r="A212" s="2"/>
       <c r="B212" s="3"/>
       <c r="C212" s="3"/>
     </row>
-    <row r="213" spans="1:3" ht="15.95" customHeight="1">
+    <row r="213" spans="1:3" ht="16" customHeight="1">
       <c r="A213" s="2"/>
       <c r="B213" s="3"/>
       <c r="C213" s="3"/>
     </row>
-    <row r="214" spans="1:3" ht="15.95" customHeight="1">
+    <row r="214" spans="1:3" ht="16" customHeight="1">
       <c r="A214" s="2"/>
       <c r="B214" s="3"/>
       <c r="C214" s="3"/>
     </row>
-    <row r="215" spans="1:3" ht="15.95" customHeight="1">
+    <row r="215" spans="1:3" ht="16" customHeight="1">
       <c r="A215" s="2"/>
       <c r="B215" s="3"/>
       <c r="C215" s="3"/>
     </row>
-    <row r="216" spans="1:3" ht="15.95" customHeight="1">
+    <row r="216" spans="1:3" ht="16" customHeight="1">
       <c r="A216" s="2"/>
       <c r="B216" s="3"/>
       <c r="C216" s="3"/>
     </row>
-    <row r="217" spans="1:3" ht="15.95" customHeight="1">
+    <row r="217" spans="1:3" ht="16" customHeight="1">
       <c r="A217" s="2"/>
       <c r="B217" s="3"/>
       <c r="C217" s="3"/>
     </row>
-    <row r="218" spans="1:3" ht="15.95" customHeight="1">
+    <row r="218" spans="1:3" ht="16" customHeight="1">
       <c r="A218" s="2"/>
       <c r="B218" s="3"/>
       <c r="C218" s="3"/>
     </row>
-    <row r="219" spans="1:3" ht="15.95" customHeight="1">
+    <row r="219" spans="1:3" ht="16" customHeight="1">
       <c r="A219" s="2"/>
       <c r="B219" s="3"/>
       <c r="C219" s="3"/>
     </row>
-    <row r="220" spans="1:3" ht="15.95" customHeight="1">
+    <row r="220" spans="1:3" ht="16" customHeight="1">
       <c r="A220" s="2"/>
       <c r="B220" s="3"/>
       <c r="C220" s="3"/>
     </row>
-    <row r="221" spans="1:3" ht="15.95" customHeight="1">
+    <row r="221" spans="1:3" ht="16" customHeight="1">
       <c r="A221" s="2"/>
       <c r="B221" s="3"/>
       <c r="C221" s="3"/>
     </row>
-    <row r="222" spans="1:3" ht="15.95" customHeight="1">
+    <row r="222" spans="1:3" ht="16" customHeight="1">
       <c r="A222" s="2"/>
       <c r="B222" s="3"/>
       <c r="C222" s="3"/>
     </row>
-    <row r="223" spans="1:3" ht="15.95" customHeight="1">
+    <row r="223" spans="1:3" ht="16" customHeight="1">
       <c r="A223" s="2"/>
       <c r="B223" s="3"/>
       <c r="C223" s="3"/>
     </row>
-    <row r="224" spans="1:3" ht="15.95" customHeight="1">
+    <row r="224" spans="1:3" ht="16" customHeight="1">
       <c r="A224" s="2"/>
       <c r="B224" s="3"/>
       <c r="C224" s="3"/>
     </row>
-    <row r="225" spans="1:3" ht="15.95" customHeight="1">
+    <row r="225" spans="1:3" ht="16" customHeight="1">
       <c r="A225" s="2"/>
       <c r="B225" s="3"/>
       <c r="C225" s="3"/>
     </row>
-    <row r="226" spans="1:3" ht="15.95" customHeight="1">
+    <row r="226" spans="1:3" ht="16" customHeight="1">
       <c r="A226" s="2"/>
       <c r="B226" s="3"/>
       <c r="C226" s="3"/>
     </row>
-    <row r="227" spans="1:3" ht="15.95" customHeight="1">
+    <row r="227" spans="1:3" ht="16" customHeight="1">
       <c r="A227" s="2"/>
       <c r="B227" s="3"/>
       <c r="C227" s="3"/>
     </row>
-    <row r="228" spans="1:3" ht="15.95" customHeight="1">
+    <row r="228" spans="1:3" ht="16" customHeight="1">
       <c r="A228" s="2"/>
       <c r="B228" s="3"/>
       <c r="C228" s="3"/>
     </row>
-    <row r="229" spans="1:3" ht="15.95" customHeight="1">
+    <row r="229" spans="1:3" ht="16" customHeight="1">
       <c r="A229" s="2"/>
       <c r="B229" s="3"/>
       <c r="C229" s="3"/>
     </row>
-    <row r="230" spans="1:3" ht="15.95" customHeight="1">
+    <row r="230" spans="1:3" ht="16" customHeight="1">
       <c r="A230" s="2"/>
       <c r="B230" s="3"/>
       <c r="C230" s="3"/>
     </row>
-    <row r="231" spans="1:3" ht="15.95" customHeight="1">
+    <row r="231" spans="1:3" ht="16" customHeight="1">
       <c r="A231" s="2"/>
       <c r="B231" s="3"/>
       <c r="C231" s="3"/>
     </row>
-    <row r="232" spans="1:3" ht="15.95" customHeight="1">
+    <row r="232" spans="1:3" ht="16" customHeight="1">
       <c r="A232" s="2"/>
       <c r="B232" s="3"/>
       <c r="C232" s="3"/>
     </row>
-    <row r="233" spans="1:3" ht="15.95" customHeight="1">
+    <row r="233" spans="1:3" ht="16" customHeight="1">
       <c r="A233" s="2"/>
       <c r="B233" s="3"/>
       <c r="C233" s="3"/>
     </row>
-    <row r="234" spans="1:3" ht="15.95" customHeight="1">
+    <row r="234" spans="1:3" ht="16" customHeight="1">
       <c r="A234" s="2"/>
       <c r="B234" s="3"/>
       <c r="C234" s="3"/>
     </row>
-    <row r="235" spans="1:3" ht="15.95" customHeight="1">
+    <row r="235" spans="1:3" ht="16" customHeight="1">
       <c r="A235" s="2"/>
       <c r="B235" s="3"/>
       <c r="C235" s="3"/>
     </row>
-    <row r="236" spans="1:3" ht="15.95" customHeight="1">
+    <row r="236" spans="1:3" ht="16" customHeight="1">
       <c r="A236" s="2"/>
       <c r="B236" s="3"/>
       <c r="C236" s="3"/>
     </row>
-    <row r="237" spans="1:3" ht="15.95" customHeight="1">
+    <row r="237" spans="1:3" ht="16" customHeight="1">
       <c r="A237" s="2"/>
       <c r="B237" s="3"/>
       <c r="C237" s="3"/>
     </row>
-    <row r="238" spans="1:3" ht="15.95" customHeight="1">
+    <row r="238" spans="1:3" ht="16" customHeight="1">
       <c r="A238" s="2"/>
       <c r="B238" s="3"/>
       <c r="C238" s="3"/>
     </row>
-    <row r="239" spans="1:3" ht="15.95" customHeight="1">
+    <row r="239" spans="1:3" ht="16" customHeight="1">
       <c r="A239" s="2"/>
       <c r="B239" s="3"/>
       <c r="C239" s="3"/>
     </row>
-    <row r="240" spans="1:3" ht="15.95" customHeight="1">
+    <row r="240" spans="1:3" ht="16" customHeight="1">
       <c r="A240" s="2"/>
       <c r="B240" s="3"/>
       <c r="C240" s="3"/>
     </row>
-    <row r="241" spans="1:3" ht="15.95" customHeight="1">
+    <row r="241" spans="1:3" ht="16" customHeight="1">
       <c r="A241" s="2"/>
       <c r="B241" s="3"/>
       <c r="C241" s="3"/>
     </row>
-    <row r="242" spans="1:3" ht="15.95" customHeight="1">
+    <row r="242" spans="1:3" ht="16" customHeight="1">
       <c r="A242" s="2"/>
       <c r="B242" s="3"/>
       <c r="C242" s="3"/>
     </row>
-    <row r="243" spans="1:3" ht="15.95" customHeight="1">
+    <row r="243" spans="1:3" ht="16" customHeight="1">
       <c r="A243" s="2"/>
       <c r="B243" s="3"/>
       <c r="C243" s="3"/>
     </row>
-    <row r="244" spans="1:3" ht="15.95" customHeight="1">
+    <row r="244" spans="1:3" ht="16" customHeight="1">
       <c r="A244" s="2"/>
       <c r="B244" s="3"/>
       <c r="C244" s="3"/>
     </row>
-    <row r="245" spans="1:3" ht="15.95" customHeight="1">
+    <row r="245" spans="1:3" ht="16" customHeight="1">
       <c r="A245" s="2"/>
       <c r="B245" s="3"/>
       <c r="C245" s="3"/>
     </row>
-    <row r="246" spans="1:3" ht="15.95" customHeight="1">
+    <row r="246" spans="1:3" ht="16" customHeight="1">
       <c r="A246" s="2"/>
       <c r="B246" s="3"/>
       <c r="C246" s="3"/>
     </row>
-    <row r="247" spans="1:3" ht="15.95" customHeight="1">
+    <row r="247" spans="1:3" ht="16" customHeight="1">
       <c r="A247" s="2"/>
       <c r="B247" s="3"/>
       <c r="C247" s="3"/>
     </row>
-    <row r="248" spans="1:3" ht="15.95" customHeight="1">
+    <row r="248" spans="1:3" ht="16" customHeight="1">
       <c r="A248" s="2"/>
       <c r="B248" s="3"/>
       <c r="C248" s="3"/>
     </row>
-    <row r="249" spans="1:3" ht="15.95" customHeight="1">
+    <row r="249" spans="1:3" ht="16" customHeight="1">
       <c r="A249" s="2"/>
       <c r="B249" s="3"/>
       <c r="C249" s="3"/>
     </row>
-    <row r="250" spans="1:3" ht="15.95" customHeight="1">
+    <row r="250" spans="1:3" ht="16" customHeight="1">
       <c r="A250" s="2"/>
       <c r="B250" s="3"/>
       <c r="C250" s="3"/>
     </row>
-    <row r="251" spans="1:3" ht="15.95" customHeight="1">
+    <row r="251" spans="1:3" ht="16" customHeight="1">
       <c r="A251" s="2"/>
       <c r="B251" s="3"/>
       <c r="C251" s="3"/>
     </row>
-    <row r="252" spans="1:3" ht="15.95" customHeight="1">
+    <row r="252" spans="1:3" ht="16" customHeight="1">
       <c r="A252" s="2"/>
       <c r="B252" s="3"/>
       <c r="C252" s="3"/>
     </row>
-    <row r="253" spans="1:3" ht="15.95" customHeight="1">
+    <row r="253" spans="1:3" ht="16" customHeight="1">
       <c r="A253" s="2"/>
       <c r="B253" s="3"/>
       <c r="C253" s="3"/>
     </row>
-    <row r="254" spans="1:3" ht="15.95" customHeight="1">
+    <row r="254" spans="1:3" ht="16" customHeight="1">
       <c r="A254" s="2"/>
       <c r="B254" s="3"/>
       <c r="C254" s="3"/>
     </row>
-    <row r="255" spans="1:3" ht="15.95" customHeight="1">
+    <row r="255" spans="1:3" ht="16" customHeight="1">
       <c r="A255" s="2"/>
       <c r="B255" s="3"/>
       <c r="C255" s="3"/>
     </row>
-    <row r="256" spans="1:3" ht="15.95" customHeight="1">
+    <row r="256" spans="1:3" ht="16" customHeight="1">
       <c r="A256" s="2"/>
       <c r="B256" s="3"/>
       <c r="C256" s="3"/>
     </row>
-    <row r="257" spans="1:3" ht="15.95" customHeight="1">
+    <row r="257" spans="1:3" ht="16" customHeight="1">
       <c r="A257" s="2"/>
       <c r="B257" s="3"/>
       <c r="C257" s="3"/>
     </row>
-    <row r="258" spans="1:3" ht="15.95" customHeight="1">
+    <row r="258" spans="1:3" ht="16" customHeight="1">
       <c r="A258" s="2"/>
       <c r="B258" s="3"/>
       <c r="C258" s="3"/>
     </row>
-    <row r="259" spans="1:3" ht="15.95" customHeight="1">
+    <row r="259" spans="1:3" ht="16" customHeight="1">
       <c r="A259" s="2"/>
       <c r="B259" s="3"/>
       <c r="C259" s="3"/>
     </row>
-    <row r="260" spans="1:3" ht="15.95" customHeight="1">
+    <row r="260" spans="1:3" ht="16" customHeight="1">
       <c r="A260" s="2"/>
       <c r="B260" s="3"/>
       <c r="C260" s="3"/>
     </row>
-    <row r="261" spans="1:3" ht="15.95" customHeight="1">
+    <row r="261" spans="1:3" ht="16" customHeight="1">
       <c r="A261" s="2"/>
       <c r="B261" s="3"/>
       <c r="C261" s="3"/>
     </row>
-    <row r="262" spans="1:3" ht="15.95" customHeight="1">
+    <row r="262" spans="1:3" ht="16" customHeight="1">
       <c r="A262" s="2"/>
       <c r="B262" s="3"/>
       <c r="C262" s="3"/>
     </row>
-    <row r="263" spans="1:3" ht="15.95" customHeight="1">
+    <row r="263" spans="1:3" ht="16" customHeight="1">
       <c r="A263" s="2"/>
       <c r="B263" s="3"/>
       <c r="C263" s="3"/>
     </row>
-    <row r="264" spans="1:3" ht="15.95" customHeight="1">
+    <row r="264" spans="1:3" ht="16" customHeight="1">
       <c r="A264" s="2"/>
       <c r="B264" s="3"/>
       <c r="C264" s="3"/>
     </row>
-    <row r="265" spans="1:3" ht="15.95" customHeight="1">
+    <row r="265" spans="1:3" ht="16" customHeight="1">
       <c r="A265" s="2"/>
       <c r="B265" s="3"/>
       <c r="C265" s="3"/>
     </row>
-    <row r="266" spans="1:3" ht="15.95" customHeight="1">
+    <row r="266" spans="1:3" ht="16" customHeight="1">
       <c r="A266" s="2"/>
       <c r="B266" s="3"/>
       <c r="C266" s="3"/>
     </row>
-    <row r="267" spans="1:3" ht="15.95" customHeight="1">
+    <row r="267" spans="1:3" ht="16" customHeight="1">
       <c r="A267" s="2"/>
       <c r="B267" s="3"/>
       <c r="C267" s="3"/>
     </row>
-    <row r="268" spans="1:3" ht="15.95" customHeight="1">
+    <row r="268" spans="1:3" ht="16" customHeight="1">
       <c r="A268" s="2"/>
       <c r="B268" s="3"/>
       <c r="C268" s="3"/>
     </row>
-    <row r="269" spans="1:3" ht="15.95" customHeight="1">
+    <row r="269" spans="1:3" ht="16" customHeight="1">
       <c r="A269" s="2"/>
       <c r="B269" s="3"/>
       <c r="C269" s="3"/>
     </row>
-    <row r="270" spans="1:3" ht="15.95" customHeight="1">
+    <row r="270" spans="1:3" ht="16" customHeight="1">
       <c r="A270" s="2"/>
       <c r="B270" s="3"/>
       <c r="C270" s="3"/>
     </row>
-    <row r="271" spans="1:3" ht="15.95" customHeight="1">
+    <row r="271" spans="1:3" ht="16" customHeight="1">
       <c r="A271" s="2"/>
       <c r="B271" s="3"/>
       <c r="C271" s="3"/>
     </row>
-    <row r="272" spans="1:3" ht="15.95" customHeight="1">
+    <row r="272" spans="1:3" ht="16" customHeight="1">
       <c r="A272" s="2"/>
       <c r="B272" s="3"/>
       <c r="C272" s="3"/>
     </row>
-    <row r="273" spans="1:3" ht="15.95" customHeight="1">
+    <row r="273" spans="1:3" ht="16" customHeight="1">
       <c r="A273" s="2"/>
       <c r="B273" s="3"/>
       <c r="C273" s="3"/>
     </row>
-    <row r="274" spans="1:3" ht="15.95" customHeight="1">
+    <row r="274" spans="1:3" ht="16" customHeight="1">
       <c r="A274" s="2"/>
       <c r="B274" s="3"/>
       <c r="C274" s="3"/>
     </row>
-    <row r="275" spans="1:3" ht="15.95" customHeight="1">
+    <row r="275" spans="1:3" ht="16" customHeight="1">
       <c r="A275" s="2"/>
       <c r="B275" s="3"/>
       <c r="C275" s="3"/>
     </row>
-    <row r="276" spans="1:3" ht="15.95" customHeight="1">
+    <row r="276" spans="1:3" ht="16" customHeight="1">
       <c r="A276" s="2"/>
       <c r="B276" s="3"/>
       <c r="C276" s="3"/>
     </row>
-    <row r="277" spans="1:3" ht="15.95" customHeight="1">
+    <row r="277" spans="1:3" ht="16" customHeight="1">
       <c r="A277" s="2"/>
       <c r="B277" s="3"/>
       <c r="C277" s="3"/>
     </row>
-    <row r="278" spans="1:3" ht="15.95" customHeight="1">
+    <row r="278" spans="1:3" ht="16" customHeight="1">
       <c r="A278" s="2"/>
       <c r="B278" s="3"/>
       <c r="C278" s="3"/>
     </row>
-    <row r="279" spans="1:3" ht="15.95" customHeight="1">
+    <row r="279" spans="1:3" ht="16" customHeight="1">
       <c r="A279" s="2"/>
       <c r="B279" s="3"/>
       <c r="C279" s="3"/>
     </row>
-    <row r="280" spans="1:3" ht="15.95" customHeight="1">
+    <row r="280" spans="1:3" ht="16" customHeight="1">
       <c r="A280" s="2"/>
       <c r="B280" s="3"/>
       <c r="C280" s="3"/>
     </row>
-    <row r="281" spans="1:3" ht="15.95" customHeight="1">
+    <row r="281" spans="1:3" ht="16" customHeight="1">
       <c r="A281" s="2"/>
       <c r="B281" s="3"/>
       <c r="C281" s="3"/>
     </row>
-    <row r="282" spans="1:3" ht="15.95" customHeight="1">
+    <row r="282" spans="1:3" ht="16" customHeight="1">
       <c r="A282" s="2"/>
       <c r="B282" s="3"/>
       <c r="C282" s="3"/>
     </row>
-    <row r="283" spans="1:3" ht="15.95" customHeight="1">
+    <row r="283" spans="1:3" ht="16" customHeight="1">
       <c r="A283" s="2"/>
       <c r="B283" s="3"/>
       <c r="C283" s="3"/>
     </row>
-    <row r="284" spans="1:3" ht="15.95" customHeight="1">
+    <row r="284" spans="1:3" ht="16" customHeight="1">
       <c r="A284" s="2"/>
       <c r="B284" s="3"/>
       <c r="C284" s="3"/>
     </row>
-    <row r="285" spans="1:3" ht="15.95" customHeight="1">
+    <row r="285" spans="1:3" ht="16" customHeight="1">
       <c r="A285" s="2"/>
       <c r="B285" s="3"/>
       <c r="C285" s="3"/>
     </row>
-    <row r="286" spans="1:3" ht="15.95" customHeight="1">
+    <row r="286" spans="1:3" ht="16" customHeight="1">
       <c r="A286" s="2"/>
       <c r="B286" s="3"/>
       <c r="C286" s="3"/>
     </row>
-    <row r="287" spans="1:3" ht="15.95" customHeight="1">
+    <row r="287" spans="1:3" ht="16" customHeight="1">
       <c r="A287" s="2"/>
       <c r="B287" s="3"/>
       <c r="C287" s="3"/>
     </row>
-    <row r="288" spans="1:3" ht="15.95" customHeight="1">
+    <row r="288" spans="1:3" ht="16" customHeight="1">
       <c r="A288" s="2"/>
       <c r="B288" s="3"/>
       <c r="C288" s="3"/>
     </row>
-    <row r="289" spans="1:3" ht="15.95" customHeight="1">
+    <row r="289" spans="1:3" ht="16" customHeight="1">
       <c r="A289" s="2"/>
       <c r="B289" s="3"/>
       <c r="C289" s="3"/>
     </row>
-    <row r="290" spans="1:3" ht="15.95" customHeight="1">
+    <row r="290" spans="1:3" ht="16" customHeight="1">
       <c r="A290" s="2"/>
       <c r="B290" s="3"/>
       <c r="C290" s="3"/>
     </row>
-    <row r="291" spans="1:3" ht="15.95" customHeight="1">
+    <row r="291" spans="1:3" ht="16" customHeight="1">
       <c r="A291" s="2"/>
       <c r="B291" s="3"/>
       <c r="C291" s="3"/>
     </row>
-    <row r="292" spans="1:3" ht="15.95" customHeight="1">
+    <row r="292" spans="1:3" ht="16" customHeight="1">
       <c r="A292" s="2"/>
       <c r="B292" s="3"/>
       <c r="C292" s="3"/>
     </row>
-    <row r="293" spans="1:3" ht="15.95" customHeight="1">
+    <row r="293" spans="1:3" ht="16" customHeight="1">
       <c r="A293" s="2"/>
       <c r="B293" s="3"/>
       <c r="C293" s="3"/>
     </row>
-    <row r="294" spans="1:3" ht="15.95" customHeight="1">
+    <row r="294" spans="1:3" ht="16" customHeight="1">
       <c r="A294" s="2"/>
       <c r="B294" s="3"/>
       <c r="C294" s="3"/>
     </row>
-    <row r="295" spans="1:3" ht="15.95" customHeight="1">
+    <row r="295" spans="1:3" ht="16" customHeight="1">
       <c r="A295" s="2"/>
       <c r="B295" s="3"/>
       <c r="C295" s="3"/>
     </row>
-    <row r="296" spans="1:3" ht="15.95" customHeight="1">
+    <row r="296" spans="1:3" ht="16" customHeight="1">
       <c r="A296" s="2"/>
       <c r="B296" s="3"/>
       <c r="C296" s="3"/>
     </row>
-    <row r="297" spans="1:3" ht="15.95" customHeight="1">
+    <row r="297" spans="1:3" ht="16" customHeight="1">
       <c r="A297" s="2"/>
       <c r="B297" s="3"/>
       <c r="C297" s="3"/>
     </row>
-    <row r="298" spans="1:3" ht="15.95" customHeight="1">
+    <row r="298" spans="1:3" ht="16" customHeight="1">
       <c r="A298" s="2"/>
       <c r="B298" s="3"/>
       <c r="C298" s="3"/>
     </row>
-    <row r="299" spans="1:3" ht="15.95" customHeight="1">
+    <row r="299" spans="1:3" ht="16" customHeight="1">
       <c r="A299" s="2"/>
       <c r="B299" s="3"/>
       <c r="C299" s="3"/>
     </row>
-    <row r="300" spans="1:3" ht="15.95" customHeight="1">
+    <row r="300" spans="1:3" ht="16" customHeight="1">
       <c r="A300" s="2"/>
       <c r="B300" s="3"/>
       <c r="C300" s="3"/>
     </row>
-    <row r="301" spans="1:3" ht="15.95" customHeight="1">
+    <row r="301" spans="1:3" ht="16" customHeight="1">
       <c r="A301" s="2"/>
       <c r="B301" s="3"/>
       <c r="C301" s="3"/>
     </row>
-    <row r="302" spans="1:3" ht="15.95" customHeight="1">
+    <row r="302" spans="1:3" ht="16" customHeight="1">
       <c r="A302" s="2"/>
       <c r="B302" s="3"/>
       <c r="C302" s="3"/>
     </row>
-    <row r="303" spans="1:3" ht="15.95" customHeight="1">
+    <row r="303" spans="1:3" ht="16" customHeight="1">
       <c r="A303" s="2"/>
       <c r="B303" s="3"/>
       <c r="C303" s="3"/>
     </row>
-    <row r="304" spans="1:3" ht="15.95" customHeight="1">
+    <row r="304" spans="1:3" ht="16" customHeight="1">
       <c r="A304" s="2"/>
       <c r="B304" s="3"/>
       <c r="C304" s="3"/>
     </row>
-    <row r="305" spans="1:3" ht="15.95" customHeight="1">
+    <row r="305" spans="1:3" ht="16" customHeight="1">
       <c r="A305" s="2"/>
       <c r="B305" s="3"/>
       <c r="C305" s="3"/>
     </row>
-    <row r="306" spans="1:3" ht="15.95" customHeight="1">
+    <row r="306" spans="1:3" ht="16" customHeight="1">
       <c r="A306" s="2"/>
       <c r="B306" s="3"/>
       <c r="C306" s="3"/>
     </row>
-    <row r="307" spans="1:3" ht="15.95" customHeight="1">
+    <row r="307" spans="1:3" ht="16" customHeight="1">
       <c r="A307" s="2"/>
       <c r="B307" s="3"/>
       <c r="C307" s="3"/>
     </row>
-    <row r="308" spans="1:3" ht="15.95" customHeight="1">
+    <row r="308" spans="1:3" ht="16" customHeight="1">
       <c r="A308" s="2"/>
       <c r="B308" s="3"/>
       <c r="C308" s="3"/>
     </row>
-    <row r="309" spans="1:3" ht="15.95" customHeight="1">
+    <row r="309" spans="1:3" ht="16" customHeight="1">
       <c r="A309" s="2"/>
       <c r="B309" s="3"/>
       <c r="C309" s="3"/>
     </row>
-    <row r="310" spans="1:3" ht="15.95" customHeight="1">
+    <row r="310" spans="1:3" ht="16" customHeight="1">
       <c r="A310" s="2"/>
       <c r="B310" s="3"/>
       <c r="C310" s="3"/>
     </row>
-    <row r="311" spans="1:3" ht="15.95" customHeight="1">
+    <row r="311" spans="1:3" ht="16" customHeight="1">
       <c r="A311" s="2"/>
       <c r="B311" s="3"/>
       <c r="C311" s="3"/>
     </row>
-    <row r="312" spans="1:3" ht="15.95" customHeight="1">
+    <row r="312" spans="1:3" ht="16" customHeight="1">
       <c r="A312" s="2"/>
       <c r="B312" s="3"/>
       <c r="C312" s="3"/>
     </row>
-    <row r="313" spans="1:3" ht="15.95" customHeight="1">
+    <row r="313" spans="1:3" ht="16" customHeight="1">
       <c r="A313" s="2"/>
       <c r="B313" s="3"/>
       <c r="C313" s="3"/>
     </row>
-    <row r="314" spans="1:3" ht="15.95" customHeight="1">
+    <row r="314" spans="1:3" ht="16" customHeight="1">
       <c r="A314" s="2"/>
       <c r="B314" s="3"/>
       <c r="C314" s="3"/>
     </row>
-    <row r="315" spans="1:3" ht="15.95" customHeight="1">
+    <row r="315" spans="1:3" ht="16" customHeight="1">
       <c r="A315" s="2"/>
       <c r="B315" s="3"/>
       <c r="C315" s="3"/>
     </row>
-    <row r="316" spans="1:3" ht="15.95" customHeight="1">
+    <row r="316" spans="1:3" ht="16" customHeight="1">
       <c r="A316" s="2"/>
       <c r="B316" s="3"/>
       <c r="C316" s="3"/>
     </row>
-    <row r="317" spans="1:3" ht="15.95" customHeight="1">
+    <row r="317" spans="1:3" ht="16" customHeight="1">
       <c r="A317" s="2"/>
       <c r="B317" s="3"/>
       <c r="C317" s="3"/>
     </row>
-    <row r="318" spans="1:3" ht="15.95" customHeight="1">
+    <row r="318" spans="1:3" ht="16" customHeight="1">
       <c r="A318" s="2"/>
       <c r="B318" s="3"/>
       <c r="C318" s="3"/>
     </row>
-    <row r="319" spans="1:3" ht="15.95" customHeight="1">
+    <row r="319" spans="1:3" ht="16" customHeight="1">
       <c r="A319" s="2"/>
       <c r="B319" s="3"/>
       <c r="C319" s="3"/>
     </row>
-    <row r="320" spans="1:3" ht="15.95" customHeight="1">
+    <row r="320" spans="1:3" ht="16" customHeight="1">
       <c r="A320" s="2"/>
       <c r="B320" s="3"/>
       <c r="C320" s="3"/>
     </row>
-    <row r="321" spans="1:3" ht="15.95" customHeight="1">
+    <row r="321" spans="1:3" ht="16" customHeight="1">
       <c r="A321" s="2"/>
       <c r="B321" s="3"/>
       <c r="C321" s="3"/>
     </row>
-    <row r="322" spans="1:3" ht="15.95" customHeight="1">
+    <row r="322" spans="1:3" ht="16" customHeight="1">
       <c r="A322" s="2"/>
       <c r="B322" s="3"/>
       <c r="C322" s="3"/>
     </row>
-    <row r="323" spans="1:3" ht="15.95" customHeight="1">
+    <row r="323" spans="1:3" ht="16" customHeight="1">
       <c r="A323" s="2"/>
       <c r="B323" s="3"/>
       <c r="C323" s="3"/>
     </row>
-    <row r="324" spans="1:3" ht="15.95" customHeight="1">
+    <row r="324" spans="1:3" ht="16" customHeight="1">
       <c r="A324" s="2"/>
       <c r="B324" s="3"/>
       <c r="C324" s="3"/>
     </row>
-    <row r="325" spans="1:3" ht="15.95" customHeight="1">
+    <row r="325" spans="1:3" ht="16" customHeight="1">
       <c r="A325" s="2"/>
       <c r="B325" s="3"/>
       <c r="C325" s="3"/>
     </row>
-    <row r="326" spans="1:3" ht="15.95" customHeight="1">
+    <row r="326" spans="1:3" ht="16" customHeight="1">
       <c r="A326" s="2"/>
       <c r="B326" s="3"/>
       <c r="C326" s="3"/>
     </row>
-    <row r="327" spans="1:3" ht="15.95" customHeight="1">
+    <row r="327" spans="1:3" ht="16" customHeight="1">
       <c r="A327" s="2"/>
       <c r="B327" s="3"/>
       <c r="C327" s="3"/>
     </row>
-    <row r="328" spans="1:3" ht="15.95" customHeight="1">
+    <row r="328" spans="1:3" ht="16" customHeight="1">
       <c r="A328" s="2"/>
       <c r="B328" s="3"/>
       <c r="C328" s="3"/>
     </row>
-    <row r="329" spans="1:3" ht="15.95" customHeight="1">
+    <row r="329" spans="1:3" ht="16" customHeight="1">
       <c r="A329" s="2"/>
       <c r="B329" s="3"/>
       <c r="C329" s="3"/>
     </row>
-    <row r="330" spans="1:3" ht="15.95" customHeight="1">
+    <row r="330" spans="1:3" ht="16" customHeight="1">
       <c r="A330" s="2"/>
       <c r="B330" s="3"/>
       <c r="C330" s="3"/>
     </row>
-    <row r="331" spans="1:3" ht="15.95" customHeight="1">
+    <row r="331" spans="1:3" ht="16" customHeight="1">
       <c r="A331" s="2"/>
       <c r="B331" s="3"/>
       <c r="C331" s="3"/>
     </row>
-    <row r="332" spans="1:3" ht="15.95" customHeight="1">
+    <row r="332" spans="1:3" ht="16" customHeight="1">
       <c r="A332" s="2"/>
       <c r="B332" s="3"/>
       <c r="C332" s="3"/>
     </row>
-    <row r="333" spans="1:3" ht="15.95" customHeight="1">
+    <row r="333" spans="1:3" ht="16" customHeight="1">
       <c r="A333" s="2"/>
       <c r="B333" s="3"/>
       <c r="C333" s="3"/>
     </row>
-    <row r="334" spans="1:3" ht="15.95" customHeight="1">
+    <row r="334" spans="1:3" ht="16" customHeight="1">
       <c r="A334" s="2"/>
       <c r="B334" s="3"/>
       <c r="C334" s="3"/>
     </row>
-    <row r="335" spans="1:3" ht="15.95" customHeight="1">
+    <row r="335" spans="1:3" ht="16" customHeight="1">
       <c r="A335" s="2"/>
       <c r="B335" s="3"/>
       <c r="C335" s="3"/>
     </row>
-    <row r="336" spans="1:3" ht="15.95" customHeight="1">
+    <row r="336" spans="1:3" ht="16" customHeight="1">
       <c r="A336" s="2"/>
       <c r="B336" s="3"/>
       <c r="C336" s="3"/>
     </row>
-    <row r="337" spans="1:3" ht="15.95" customHeight="1">
+    <row r="337" spans="1:3" ht="16" customHeight="1">
       <c r="A337" s="2"/>
       <c r="B337" s="3"/>
       <c r="C337" s="3"/>
     </row>
-    <row r="338" spans="1:3" ht="15.95" customHeight="1">
+    <row r="338" spans="1:3" ht="16" customHeight="1">
       <c r="A338" s="2"/>
       <c r="B338" s="3"/>
       <c r="C338" s="3"/>
     </row>
-    <row r="339" spans="1:3" ht="15.95" customHeight="1">
+    <row r="339" spans="1:3" ht="16" customHeight="1">
       <c r="A339" s="2"/>
       <c r="B339" s="3"/>
       <c r="C339" s="3"/>
     </row>
-    <row r="340" spans="1:3" ht="15.95" customHeight="1">
+    <row r="340" spans="1:3" ht="16" customHeight="1">
       <c r="A340" s="2"/>
       <c r="B340" s="3"/>
       <c r="C340" s="3"/>
     </row>
-    <row r="341" spans="1:3" ht="15.95" customHeight="1">
+    <row r="341" spans="1:3" ht="16" customHeight="1">
       <c r="A341" s="2"/>
       <c r="B341" s="3"/>
       <c r="C341" s="3"/>
     </row>
-    <row r="342" spans="1:3" ht="15.95" customHeight="1">
+    <row r="342" spans="1:3" ht="16" customHeight="1">
       <c r="A342" s="2"/>
       <c r="B342" s="3"/>
       <c r="C342" s="3"/>
     </row>
-    <row r="343" spans="1:3" ht="15.95" customHeight="1">
+    <row r="343" spans="1:3" ht="16" customHeight="1">
       <c r="A343" s="2"/>
       <c r="B343" s="3"/>
       <c r="C343" s="3"/>
     </row>
-    <row r="344" spans="1:3" ht="15.95" customHeight="1">
+    <row r="344" spans="1:3" ht="16" customHeight="1">
       <c r="A344" s="2"/>
       <c r="B344" s="3"/>
       <c r="C344" s="3"/>
     </row>
-    <row r="345" spans="1:3" ht="15.95" customHeight="1">
+    <row r="345" spans="1:3" ht="16" customHeight="1">
       <c r="A345" s="2"/>
       <c r="B345" s="3"/>
       <c r="C345" s="3"/>
     </row>
-    <row r="346" spans="1:3" ht="15.95" customHeight="1">
+    <row r="346" spans="1:3" ht="16" customHeight="1">
       <c r="A346" s="2"/>
       <c r="B346" s="3"/>
       <c r="C346" s="3"/>
     </row>
-    <row r="347" spans="1:3" ht="15.95" customHeight="1">
+    <row r="347" spans="1:3" ht="16" customHeight="1">
       <c r="A347" s="2"/>
       <c r="B347" s="3"/>
       <c r="C347" s="3"/>
     </row>
-    <row r="348" spans="1:3" ht="15.95" customHeight="1">
+    <row r="348" spans="1:3" ht="16" customHeight="1">
       <c r="A348" s="2"/>
       <c r="B348" s="3"/>
       <c r="C348" s="3"/>
     </row>
-    <row r="349" spans="1:3" ht="15.95" customHeight="1">
+    <row r="349" spans="1:3" ht="16" customHeight="1">
       <c r="A349" s="2"/>
       <c r="B349" s="3"/>
       <c r="C349" s="3"/>
     </row>
-    <row r="350" spans="1:3" ht="15.95" customHeight="1">
+    <row r="350" spans="1:3" ht="16" customHeight="1">
       <c r="A350" s="2"/>
       <c r="B350" s="3"/>
       <c r="C350" s="3"/>
     </row>
-    <row r="351" spans="1:3" ht="15.95" customHeight="1">
+    <row r="351" spans="1:3" ht="16" customHeight="1">
       <c r="A351" s="2"/>
       <c r="B351" s="3"/>
       <c r="C351" s="3"/>
     </row>
-    <row r="352" spans="1:3" ht="14.1" customHeight="1">
+    <row r="352" spans="1:3" ht="14" customHeight="1">
       <c r="A352" s="4"/>
     </row>
   </sheetData>
@@ -3156,35 +3189,35 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="I1" workbookViewId="0">
       <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="18.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="31.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="38.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="18.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="12.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="31.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="38.5" style="1" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="30" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="27.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="28.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="18" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="22.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="16384" width="8.85546875" style="1"/>
+    <col min="15" max="15" width="27.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="28.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="18" width="11.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="22.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="14.1" customHeight="1">
+    <row r="1" spans="1:19" ht="14" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>53</v>
       </c>
@@ -3243,7 +3276,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:19" ht="15.95" customHeight="1">
+    <row r="2" spans="1:19" ht="16" customHeight="1">
       <c r="A2" s="2">
         <v>1000121</v>
       </c>
@@ -3302,7 +3335,7 @@
         <v>854.88</v>
       </c>
     </row>
-    <row r="3" spans="1:19" ht="15.95" customHeight="1">
+    <row r="3" spans="1:19" ht="16" customHeight="1">
       <c r="A3" s="2">
         <v>1000122</v>
       </c>
@@ -3361,7 +3394,7 @@
         <v>4346.07</v>
       </c>
     </row>
-    <row r="4" spans="1:19" ht="15.95" customHeight="1">
+    <row r="4" spans="1:19" ht="16" customHeight="1">
       <c r="A4" s="2">
         <v>1000123</v>
       </c>
@@ -3420,7 +3453,7 @@
         <v>15355.88</v>
       </c>
     </row>
-    <row r="5" spans="1:19" ht="15.95" customHeight="1">
+    <row r="5" spans="1:19" ht="16" customHeight="1">
       <c r="A5" s="2">
         <v>1000124</v>
       </c>
@@ -3479,7 +3512,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:19" ht="15.95" customHeight="1">
+    <row r="6" spans="1:19" ht="16" customHeight="1">
       <c r="A6" s="2">
         <v>1000125</v>
       </c>
@@ -3538,7 +3571,7 @@
         <v>182.58</v>
       </c>
     </row>
-    <row r="7" spans="1:19" ht="15.95" customHeight="1">
+    <row r="7" spans="1:19" ht="16" customHeight="1">
       <c r="A7" s="2">
         <v>1000126</v>
       </c>
@@ -3597,7 +3630,7 @@
         <v>405.46</v>
       </c>
     </row>
-    <row r="8" spans="1:19" ht="15.95" customHeight="1">
+    <row r="8" spans="1:19" ht="16" customHeight="1">
       <c r="A8" s="2">
         <v>1000127</v>
       </c>
@@ -3656,7 +3689,7 @@
         <v>935.81</v>
       </c>
     </row>
-    <row r="9" spans="1:19" ht="15.95" customHeight="1">
+    <row r="9" spans="1:19" ht="16" customHeight="1">
       <c r="A9" s="2">
         <v>1000128</v>
       </c>
@@ -3715,7 +3748,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:19" ht="15.95" customHeight="1">
+    <row r="10" spans="1:19" ht="16" customHeight="1">
       <c r="A10" s="2">
         <v>1000129</v>
       </c>
@@ -3774,7 +3807,7 @@
         <v>163.47999999999999</v>
       </c>
     </row>
-    <row r="11" spans="1:19" ht="15.95" customHeight="1">
+    <row r="11" spans="1:19" ht="16" customHeight="1">
       <c r="A11" s="2">
         <v>1000130</v>
       </c>
@@ -3833,7 +3866,7 @@
         <v>924.71</v>
       </c>
     </row>
-    <row r="12" spans="1:19" ht="15.95" customHeight="1">
+    <row r="12" spans="1:19" ht="16" customHeight="1">
       <c r="A12" s="2">
         <v>1000131</v>
       </c>
@@ -3892,7 +3925,7 @@
         <v>794.82</v>
       </c>
     </row>
-    <row r="13" spans="1:19" ht="15.95" customHeight="1">
+    <row r="13" spans="1:19" ht="16" customHeight="1">
       <c r="A13" s="2">
         <v>1000132</v>
       </c>
@@ -3951,7 +3984,7 @@
         <v>41.74</v>
       </c>
     </row>
-    <row r="14" spans="1:19" ht="15.95" customHeight="1">
+    <row r="14" spans="1:19" ht="16" customHeight="1">
       <c r="A14" s="2">
         <v>1000133</v>
       </c>
@@ -4010,7 +4043,7 @@
         <v>196.24</v>
       </c>
     </row>
-    <row r="15" spans="1:19" ht="15.95" customHeight="1">
+    <row r="15" spans="1:19" ht="16" customHeight="1">
       <c r="A15" s="2">
         <v>1000134</v>
       </c>
@@ -4069,7 +4102,7 @@
         <v>65.25</v>
       </c>
     </row>
-    <row r="16" spans="1:19" ht="15.95" customHeight="1">
+    <row r="16" spans="1:19" ht="16" customHeight="1">
       <c r="A16" s="2">
         <v>1000135</v>
       </c>
@@ -4128,7 +4161,7 @@
         <v>128.57</v>
       </c>
     </row>
-    <row r="17" spans="1:19" ht="15.95" customHeight="1">
+    <row r="17" spans="1:19" ht="16" customHeight="1">
       <c r="A17" s="2">
         <v>1000136</v>
       </c>
@@ -4187,7 +4220,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:19" ht="15.95" customHeight="1">
+    <row r="18" spans="1:19" ht="16" customHeight="1">
       <c r="A18" s="2">
         <v>1000137</v>
       </c>
@@ -4246,7 +4279,7 @@
         <v>121.37</v>
       </c>
     </row>
-    <row r="19" spans="1:19" ht="15.95" customHeight="1">
+    <row r="19" spans="1:19" ht="16" customHeight="1">
       <c r="A19" s="2">
         <v>1000138</v>
       </c>
@@ -4305,7 +4338,7 @@
         <v>47.19</v>
       </c>
     </row>
-    <row r="20" spans="1:19" ht="15.95" customHeight="1">
+    <row r="20" spans="1:19" ht="16" customHeight="1">
       <c r="A20" s="2">
         <v>1000139</v>
       </c>
@@ -4377,22 +4410,22 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.28515625" style="1" customWidth="1"/>
-    <col min="3" max="4" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.85546875" style="1"/>
+    <col min="1" max="1" width="14.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.33203125" style="1" customWidth="1"/>
+    <col min="3" max="4" width="11.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="14.1" customHeight="1">
+    <row r="1" spans="1:4" ht="14" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>53</v>
       </c>
@@ -4406,7 +4439,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15.95" customHeight="1">
+    <row r="2" spans="1:4" ht="16" customHeight="1">
       <c r="A2" s="2">
         <v>1000121</v>
       </c>
@@ -4420,7 +4453,7 @@
         <v>26.8</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15.95" customHeight="1">
+    <row r="3" spans="1:4" ht="16" customHeight="1">
       <c r="A3" s="2">
         <v>1000122</v>
       </c>
@@ -4434,7 +4467,7 @@
         <v>32.4</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15.95" customHeight="1">
+    <row r="4" spans="1:4" ht="16" customHeight="1">
       <c r="A4" s="2">
         <v>1000123</v>
       </c>
@@ -4448,7 +4481,7 @@
         <v>33.4</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="15.95" customHeight="1">
+    <row r="5" spans="1:4" ht="16" customHeight="1">
       <c r="A5" s="2">
         <v>1000124</v>
       </c>
@@ -4462,7 +4495,7 @@
         <v>29.7</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="15.95" customHeight="1">
+    <row r="6" spans="1:4" ht="16" customHeight="1">
       <c r="A6" s="2">
         <v>1000125</v>
       </c>
@@ -4476,7 +4509,7 @@
         <v>22.7</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="15.95" customHeight="1">
+    <row r="7" spans="1:4" ht="16" customHeight="1">
       <c r="A7" s="2">
         <v>1000126</v>
       </c>
@@ -4490,7 +4523,7 @@
         <v>26.4</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="15.95" customHeight="1">
+    <row r="8" spans="1:4" ht="16" customHeight="1">
       <c r="A8" s="2">
         <v>1000127</v>
       </c>
@@ -4504,7 +4537,7 @@
         <v>24.9</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="15.95" customHeight="1">
+    <row r="9" spans="1:4" ht="16" customHeight="1">
       <c r="A9" s="2">
         <v>1000128</v>
       </c>
@@ -4518,7 +4551,7 @@
         <v>22.4</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="15.95" customHeight="1">
+    <row r="10" spans="1:4" ht="16" customHeight="1">
       <c r="A10" s="2">
         <v>1000129</v>
       </c>
@@ -4532,7 +4565,7 @@
         <v>28.6</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="15.95" customHeight="1">
+    <row r="11" spans="1:4" ht="16" customHeight="1">
       <c r="A11" s="2">
         <v>1000130</v>
       </c>
@@ -4546,7 +4579,7 @@
         <v>21.4</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="15.95" customHeight="1">
+    <row r="12" spans="1:4" ht="16" customHeight="1">
       <c r="A12" s="2">
         <v>1000131</v>
       </c>
@@ -4560,7 +4593,7 @@
         <v>20.7</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="15.95" customHeight="1">
+    <row r="13" spans="1:4" ht="16" customHeight="1">
       <c r="A13" s="2">
         <v>1000132</v>
       </c>
@@ -4574,7 +4607,7 @@
         <v>29.4</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="15.95" customHeight="1">
+    <row r="14" spans="1:4" ht="16" customHeight="1">
       <c r="A14" s="2">
         <v>1000133</v>
       </c>
@@ -4588,7 +4621,7 @@
         <v>28.7</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="15.95" customHeight="1">
+    <row r="15" spans="1:4" ht="16" customHeight="1">
       <c r="A15" s="2">
         <v>1000134</v>
       </c>
@@ -4602,7 +4635,7 @@
         <v>26.8</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="15.95" customHeight="1">
+    <row r="16" spans="1:4" ht="16" customHeight="1">
       <c r="A16" s="2">
         <v>1000135</v>
       </c>
@@ -4616,7 +4649,7 @@
         <v>27.3</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="15.95" customHeight="1">
+    <row r="17" spans="1:4" ht="16" customHeight="1">
       <c r="A17" s="2">
         <v>1000136</v>
       </c>
@@ -4630,7 +4663,7 @@
         <v>22.4</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="15.95" customHeight="1">
+    <row r="18" spans="1:4" ht="16" customHeight="1">
       <c r="A18" s="2">
         <v>1000137</v>
       </c>
@@ -4644,7 +4677,7 @@
         <v>21.6</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="15.95" customHeight="1">
+    <row r="19" spans="1:4" ht="16" customHeight="1">
       <c r="A19" s="2">
         <v>1000138</v>
       </c>
@@ -4658,7 +4691,7 @@
         <v>23.4</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="15.95" customHeight="1">
+    <row r="20" spans="1:4" ht="16" customHeight="1">
       <c r="A20" s="2">
         <v>1000139</v>
       </c>
@@ -4685,19 +4718,19 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="26.140625" customWidth="1"/>
-    <col min="2" max="2" width="51.140625" customWidth="1"/>
-    <col min="3" max="3" width="28.7109375" customWidth="1"/>
-    <col min="4" max="4" width="57.7109375" customWidth="1"/>
+    <col min="1" max="1" width="26.1640625" customWidth="1"/>
+    <col min="2" max="2" width="51.1640625" customWidth="1"/>
+    <col min="3" max="3" width="28.6640625" customWidth="1"/>
+    <col min="4" max="4" width="57.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -4795,21 +4828,21 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="A14:B15"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="4" width="42.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="36.28515625" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.85546875" style="1"/>
+    <col min="1" max="4" width="42.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="36.33203125" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="14.1" customHeight="1">
+    <row r="1" spans="1:6" ht="14" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>66</v>
       </c>
@@ -4825,8 +4858,11 @@
       <c r="E1" s="8" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="15.95" customHeight="1">
+      <c r="F1" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="16" customHeight="1">
       <c r="A2" s="2" t="s">
         <v>70</v>
       </c>
@@ -4838,7 +4874,7 @@
       </c>
       <c r="D2" s="3"/>
     </row>
-    <row r="3" spans="1:5" ht="15.95" customHeight="1">
+    <row r="3" spans="1:6" ht="16" customHeight="1">
       <c r="A3" s="2" t="s">
         <v>72</v>
       </c>
@@ -4852,8 +4888,19 @@
         <v>63</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="14.1" customHeight="1">
-      <c r="A4" s="4"/>
+    <row r="4" spans="1:6" ht="14" customHeight="1">
+      <c r="A4" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>90</v>
+      </c>
     </row>
   </sheetData>
   <printOptions verticalCentered="1" gridLines="1"/>

</xml_diff>